<commit_message>
add MMF and MMHF
</commit_message>
<xml_diff>
--- a/BNR/bayer.xlsx
+++ b/BNR/bayer.xlsx
@@ -14,13 +14,46 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="7">
+  <si>
+    <t>五个中的中值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>五个中的中值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三个数的中值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三个的均值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三个的均值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多级中滤波</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多级中值混合滤波</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -41,7 +74,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -78,8 +111,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="62">
+  <borders count="65">
     <border>
       <left/>
       <right/>
@@ -896,11 +941,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -977,6 +1059,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -992,6 +1126,1411 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>124239</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>24847</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>124239</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>223630</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="直接箭头连接符 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11173239" y="3039717"/>
+          <a:ext cx="0" cy="662609"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>110986</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>110986</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>226943</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="直接箭头连接符 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13561943" y="3043030"/>
+          <a:ext cx="0" cy="662609"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>23191</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>115957</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>215347</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="直接箭头连接符 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12364278" y="2574234"/>
+          <a:ext cx="1657" cy="1119809"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>107674</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1656</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>109330</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>223630</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="直接箭头连接符 9"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="12357652" y="4176091"/>
+          <a:ext cx="1656" cy="221974"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>67</xdr:col>
+      <xdr:colOff>124239</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>24847</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>67</xdr:col>
+      <xdr:colOff>124239</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>223630</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="直接箭头连接符 12"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11173239" y="3039717"/>
+          <a:ext cx="0" cy="662609"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>77</xdr:col>
+      <xdr:colOff>110986</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>77</xdr:col>
+      <xdr:colOff>110986</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>226943</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="直接箭头连接符 13"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13561943" y="3043030"/>
+          <a:ext cx="0" cy="662609"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>72</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>23191</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>72</xdr:col>
+      <xdr:colOff>115957</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>215347</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="直接箭头连接符 14"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12364278" y="2574234"/>
+          <a:ext cx="1657" cy="1119809"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>72</xdr:col>
+      <xdr:colOff>107674</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1656</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>72</xdr:col>
+      <xdr:colOff>109330</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>223630</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="直接箭头连接符 15"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="12357652" y="4176091"/>
+          <a:ext cx="1656" cy="221974"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>124239</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>24847</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>124239</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>223630</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="直接箭头连接符 16"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11173239" y="3039717"/>
+          <a:ext cx="0" cy="662609"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>110986</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>28160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>110986</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>226943</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="直接箭头连接符 17"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13561943" y="3043030"/>
+          <a:ext cx="0" cy="662609"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>23191</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>115957</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>215347</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="直接箭头连接符 18"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12364278" y="2574234"/>
+          <a:ext cx="1657" cy="1119809"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>124239</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>1657</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>125895</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>198783</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="直接箭头连接符 19"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="12374217" y="7654787"/>
+          <a:ext cx="1656" cy="429039"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>67</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>36443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>67</xdr:col>
+      <xdr:colOff>157369</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>215348</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="直接箭头连接符 28"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16245508" y="6298095"/>
+          <a:ext cx="4970" cy="874644"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>72</xdr:col>
+      <xdr:colOff>130864</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>23191</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>72</xdr:col>
+      <xdr:colOff>132522</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="直接箭头连接符 29"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17424951" y="6052930"/>
+          <a:ext cx="1658" cy="1094961"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>77</xdr:col>
+      <xdr:colOff>149087</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>43069</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>77</xdr:col>
+      <xdr:colOff>150743</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>173935</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="直接箭头连接符 30"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="18644152" y="6304721"/>
+          <a:ext cx="1656" cy="826605"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>72</xdr:col>
+      <xdr:colOff>132522</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>4968</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>72</xdr:col>
+      <xdr:colOff>137490</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>207066</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="直接箭头连接符 35"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="17426609" y="7658098"/>
+          <a:ext cx="4968" cy="434011"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>62</xdr:col>
+      <xdr:colOff>125895</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>34787</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>62</xdr:col>
+      <xdr:colOff>132522</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>223631</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="直接箭头连接符 36"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15018025" y="6064526"/>
+          <a:ext cx="6627" cy="2044148"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>62</xdr:col>
+      <xdr:colOff>135835</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>220316</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>62</xdr:col>
+      <xdr:colOff>137491</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>210377</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="直接箭头连接符 41"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="15027965" y="8801099"/>
+          <a:ext cx="1656" cy="221974"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>124239</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>24847</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>124239</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>223630</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="直接箭头连接符 42"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11173239" y="6518412"/>
+          <a:ext cx="0" cy="662609"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>58</xdr:col>
+      <xdr:colOff>110986</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>28160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>58</xdr:col>
+      <xdr:colOff>110986</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>226943</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="直接箭头连接符 43"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13561943" y="6521725"/>
+          <a:ext cx="0" cy="662609"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>23191</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>115957</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>215347</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="45" name="直接箭头连接符 44"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12364278" y="6052930"/>
+          <a:ext cx="1657" cy="1119808"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>124239</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>1657</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>125895</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>198783</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="直接箭头连接符 45"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="12374217" y="7654787"/>
+          <a:ext cx="1656" cy="429039"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>68</xdr:col>
+      <xdr:colOff>124239</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>24847</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>68</xdr:col>
+      <xdr:colOff>124239</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>223630</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="55" name="直接箭头连接符 54"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11653630" y="10924760"/>
+          <a:ext cx="0" cy="662609"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>78</xdr:col>
+      <xdr:colOff>110986</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>28160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>78</xdr:col>
+      <xdr:colOff>110986</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>226943</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="直接箭头连接符 55"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14042334" y="10928073"/>
+          <a:ext cx="0" cy="662609"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>73</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>23191</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>73</xdr:col>
+      <xdr:colOff>115957</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>215347</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="57" name="直接箭头连接符 56"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12844670" y="10459278"/>
+          <a:ext cx="1657" cy="1119808"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>73</xdr:col>
+      <xdr:colOff>124239</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>1657</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>73</xdr:col>
+      <xdr:colOff>125895</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>198783</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="58" name="直接箭头连接符 57"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="12854609" y="12061135"/>
+          <a:ext cx="1656" cy="429039"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>63</xdr:col>
+      <xdr:colOff>112642</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>13252</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>63</xdr:col>
+      <xdr:colOff>119269</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>202096</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="59" name="直接箭头连接符 58"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15244968" y="10449339"/>
+          <a:ext cx="6627" cy="2044148"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>63</xdr:col>
+      <xdr:colOff>130867</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>16565</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>63</xdr:col>
+      <xdr:colOff>132523</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>6625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="61" name="直接箭头连接符 60"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="15263193" y="13235608"/>
+          <a:ext cx="1656" cy="221974"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1257,19 +2796,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="J2:BB44"/>
+  <dimension ref="J2:CF62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AP28" sqref="AP28"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="BM10" sqref="BM10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="11:54" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="11:54" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="11:82" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="11:82" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="T3" s="7"/>
     </row>
-    <row r="6" spans="11:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="11:82" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="11:82" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="P6" s="4"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="4"/>
@@ -1277,8 +2817,51 @@
       <c r="T6" s="4"/>
       <c r="U6" s="5"/>
       <c r="V6" s="4"/>
+      <c r="AP6" s="29"/>
+      <c r="AQ6" s="82"/>
+      <c r="AR6" s="82"/>
+      <c r="AS6" s="82"/>
+      <c r="AT6" s="82"/>
+      <c r="AU6" s="82"/>
+      <c r="AV6" s="82"/>
+      <c r="AW6" s="82"/>
+      <c r="AX6" s="82"/>
+      <c r="AY6" s="82"/>
+      <c r="AZ6" s="82"/>
+      <c r="BA6" s="82"/>
+      <c r="BB6" s="82"/>
+      <c r="BC6" s="82"/>
+      <c r="BD6" s="82"/>
+      <c r="BE6" s="82"/>
+      <c r="BF6" s="95" t="s">
+        <v>5</v>
+      </c>
+      <c r="BG6" s="96"/>
+      <c r="BH6" s="96"/>
+      <c r="BI6" s="96"/>
+      <c r="BJ6" s="96"/>
+      <c r="BK6" s="96"/>
+      <c r="BL6" s="97"/>
+      <c r="BM6" s="82"/>
+      <c r="BN6" s="82"/>
+      <c r="BO6" s="82"/>
+      <c r="BP6" s="82"/>
+      <c r="BQ6" s="82"/>
+      <c r="BR6" s="82"/>
+      <c r="BS6" s="82"/>
+      <c r="BT6" s="82"/>
+      <c r="BU6" s="82"/>
+      <c r="BV6" s="82"/>
+      <c r="BW6" s="82"/>
+      <c r="BX6" s="82"/>
+      <c r="BY6" s="82"/>
+      <c r="BZ6" s="82"/>
+      <c r="CA6" s="82"/>
+      <c r="CB6" s="82"/>
+      <c r="CC6" s="82"/>
+      <c r="CD6" s="83"/>
     </row>
-    <row r="7" spans="11:54" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="11:82" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="P7" s="5"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="5"/>
@@ -1286,8 +2869,49 @@
       <c r="T7" s="5"/>
       <c r="U7" s="6"/>
       <c r="V7" s="5"/>
+      <c r="AP7" s="30"/>
+      <c r="AQ7" s="28"/>
+      <c r="AR7" s="28"/>
+      <c r="AS7" s="28"/>
+      <c r="AT7" s="28"/>
+      <c r="AU7" s="28"/>
+      <c r="AV7" s="28"/>
+      <c r="AW7" s="28"/>
+      <c r="AX7" s="28"/>
+      <c r="AY7" s="28"/>
+      <c r="AZ7" s="28"/>
+      <c r="BA7" s="28"/>
+      <c r="BB7" s="28"/>
+      <c r="BC7" s="28"/>
+      <c r="BD7" s="28"/>
+      <c r="BE7" s="28"/>
+      <c r="BF7" s="28"/>
+      <c r="BG7" s="28"/>
+      <c r="BH7" s="28"/>
+      <c r="BI7" s="28"/>
+      <c r="BJ7" s="28"/>
+      <c r="BK7" s="28"/>
+      <c r="BL7" s="28"/>
+      <c r="BM7" s="28"/>
+      <c r="BN7" s="28"/>
+      <c r="BO7" s="28"/>
+      <c r="BP7" s="28"/>
+      <c r="BQ7" s="28"/>
+      <c r="BR7" s="28"/>
+      <c r="BS7" s="28"/>
+      <c r="BT7" s="28"/>
+      <c r="BU7" s="28"/>
+      <c r="BV7" s="28"/>
+      <c r="BW7" s="28"/>
+      <c r="BX7" s="28"/>
+      <c r="BY7" s="28"/>
+      <c r="BZ7" s="28"/>
+      <c r="CA7" s="28"/>
+      <c r="CB7" s="28"/>
+      <c r="CC7" s="28"/>
+      <c r="CD7" s="84"/>
     </row>
-    <row r="8" spans="11:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="11:82" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P8" s="4"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="8"/>
@@ -1297,8 +2921,49 @@
       <c r="V8" s="11"/>
       <c r="W8" s="5"/>
       <c r="X8" s="4"/>
+      <c r="AP8" s="30"/>
+      <c r="AQ8" s="28"/>
+      <c r="AR8" s="28"/>
+      <c r="AS8" s="28"/>
+      <c r="AT8" s="28"/>
+      <c r="AU8" s="28"/>
+      <c r="AV8" s="28"/>
+      <c r="AW8" s="28"/>
+      <c r="AX8" s="28"/>
+      <c r="AY8" s="28"/>
+      <c r="AZ8" s="28"/>
+      <c r="BA8" s="28"/>
+      <c r="BB8" s="28"/>
+      <c r="BC8" s="28"/>
+      <c r="BD8" s="28"/>
+      <c r="BE8" s="28"/>
+      <c r="BF8" s="28"/>
+      <c r="BG8" s="28"/>
+      <c r="BH8" s="28"/>
+      <c r="BI8" s="28"/>
+      <c r="BJ8" s="28"/>
+      <c r="BK8" s="28"/>
+      <c r="BL8" s="28"/>
+      <c r="BM8" s="28"/>
+      <c r="BN8" s="28"/>
+      <c r="BO8" s="28"/>
+      <c r="BP8" s="28"/>
+      <c r="BQ8" s="28"/>
+      <c r="BR8" s="28"/>
+      <c r="BS8" s="28"/>
+      <c r="BT8" s="28"/>
+      <c r="BU8" s="28"/>
+      <c r="BV8" s="28"/>
+      <c r="BW8" s="28"/>
+      <c r="BX8" s="28"/>
+      <c r="BY8" s="28"/>
+      <c r="BZ8" s="28"/>
+      <c r="CA8" s="28"/>
+      <c r="CB8" s="28"/>
+      <c r="CC8" s="28"/>
+      <c r="CD8" s="84"/>
     </row>
-    <row r="9" spans="11:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="11:82" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P9" s="5"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="12"/>
@@ -1308,8 +2973,49 @@
       <c r="V9" s="13"/>
       <c r="W9" s="6"/>
       <c r="X9" s="5"/>
+      <c r="AP9" s="30"/>
+      <c r="AQ9" s="28"/>
+      <c r="AR9" s="28"/>
+      <c r="AS9" s="76"/>
+      <c r="AT9" s="76"/>
+      <c r="AU9" s="2"/>
+      <c r="AV9" s="76"/>
+      <c r="AW9" s="76"/>
+      <c r="AX9" s="28"/>
+      <c r="AY9" s="28"/>
+      <c r="AZ9" s="28"/>
+      <c r="BA9" s="28"/>
+      <c r="BB9" s="28"/>
+      <c r="BC9" s="76"/>
+      <c r="BD9" s="76"/>
+      <c r="BE9" s="76"/>
+      <c r="BF9" s="76"/>
+      <c r="BG9" s="76"/>
+      <c r="BH9" s="28"/>
+      <c r="BI9" s="28"/>
+      <c r="BJ9" s="28"/>
+      <c r="BK9" s="28"/>
+      <c r="BL9" s="28"/>
+      <c r="BM9" s="28"/>
+      <c r="BN9" s="76"/>
+      <c r="BO9" s="76"/>
+      <c r="BP9" s="93"/>
+      <c r="BQ9" s="76"/>
+      <c r="BR9" s="76"/>
+      <c r="BS9" s="28"/>
+      <c r="BT9" s="28"/>
+      <c r="BU9" s="28"/>
+      <c r="BV9" s="28"/>
+      <c r="BW9" s="28"/>
+      <c r="BX9" s="93"/>
+      <c r="BY9" s="76"/>
+      <c r="BZ9" s="76"/>
+      <c r="CA9" s="76"/>
+      <c r="CB9" s="93"/>
+      <c r="CC9" s="28"/>
+      <c r="CD9" s="84"/>
     </row>
-    <row r="10" spans="11:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="11:82" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P10" s="4"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="14"/>
@@ -1319,8 +3025,49 @@
       <c r="V10" s="15"/>
       <c r="W10" s="5"/>
       <c r="X10" s="4"/>
+      <c r="AP10" s="30"/>
+      <c r="AQ10" s="28"/>
+      <c r="AR10" s="28"/>
+      <c r="AS10" s="76"/>
+      <c r="AT10" s="76"/>
+      <c r="AU10" s="76"/>
+      <c r="AV10" s="76"/>
+      <c r="AW10" s="76"/>
+      <c r="AX10" s="28"/>
+      <c r="AY10" s="28"/>
+      <c r="AZ10" s="28"/>
+      <c r="BA10" s="28"/>
+      <c r="BB10" s="28"/>
+      <c r="BC10" s="76"/>
+      <c r="BD10" s="2"/>
+      <c r="BE10" s="76"/>
+      <c r="BF10" s="2"/>
+      <c r="BG10" s="76"/>
+      <c r="BH10" s="28"/>
+      <c r="BI10" s="28"/>
+      <c r="BJ10" s="28"/>
+      <c r="BK10" s="28"/>
+      <c r="BL10" s="28"/>
+      <c r="BM10" s="28"/>
+      <c r="BN10" s="76"/>
+      <c r="BO10" s="76"/>
+      <c r="BP10" s="76"/>
+      <c r="BQ10" s="76"/>
+      <c r="BR10" s="76"/>
+      <c r="BS10" s="28"/>
+      <c r="BT10" s="28"/>
+      <c r="BU10" s="28"/>
+      <c r="BV10" s="28"/>
+      <c r="BW10" s="28"/>
+      <c r="BX10" s="76"/>
+      <c r="BY10" s="77"/>
+      <c r="BZ10" s="76"/>
+      <c r="CA10" s="77"/>
+      <c r="CB10" s="77"/>
+      <c r="CC10" s="28"/>
+      <c r="CD10" s="84"/>
     </row>
-    <row r="11" spans="11:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="11:82" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P11" s="5"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="12"/>
@@ -1330,8 +3077,49 @@
       <c r="V11" s="13"/>
       <c r="W11" s="6"/>
       <c r="X11" s="5"/>
+      <c r="AP11" s="30"/>
+      <c r="AQ11" s="28"/>
+      <c r="AR11" s="28"/>
+      <c r="AS11" s="2"/>
+      <c r="AT11" s="76"/>
+      <c r="AU11" s="2"/>
+      <c r="AV11" s="76"/>
+      <c r="AW11" s="2"/>
+      <c r="AX11" s="28"/>
+      <c r="AY11" s="28"/>
+      <c r="AZ11" s="5"/>
+      <c r="BA11" s="28"/>
+      <c r="BB11" s="28"/>
+      <c r="BC11" s="76"/>
+      <c r="BD11" s="76"/>
+      <c r="BE11" s="2"/>
+      <c r="BF11" s="76"/>
+      <c r="BG11" s="76"/>
+      <c r="BH11" s="28"/>
+      <c r="BI11" s="28"/>
+      <c r="BJ11" s="28"/>
+      <c r="BK11" s="28"/>
+      <c r="BL11" s="28"/>
+      <c r="BM11" s="28"/>
+      <c r="BN11" s="93"/>
+      <c r="BO11" s="76"/>
+      <c r="BP11" s="93"/>
+      <c r="BQ11" s="76"/>
+      <c r="BR11" s="93"/>
+      <c r="BS11" s="28"/>
+      <c r="BT11" s="28"/>
+      <c r="BU11" s="94"/>
+      <c r="BV11" s="28"/>
+      <c r="BW11" s="28"/>
+      <c r="BX11" s="76"/>
+      <c r="BY11" s="76"/>
+      <c r="BZ11" s="93"/>
+      <c r="CA11" s="76"/>
+      <c r="CB11" s="76"/>
+      <c r="CC11" s="28"/>
+      <c r="CD11" s="84"/>
     </row>
-    <row r="12" spans="11:54" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="11:82" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="P12" s="4"/>
       <c r="Q12" s="5"/>
       <c r="R12" s="16"/>
@@ -1341,22 +3129,188 @@
       <c r="V12" s="19"/>
       <c r="W12" s="5"/>
       <c r="X12" s="4"/>
+      <c r="AP12" s="30"/>
+      <c r="AQ12" s="28"/>
+      <c r="AR12" s="28"/>
+      <c r="AS12" s="76"/>
+      <c r="AT12" s="76"/>
+      <c r="AU12" s="76"/>
+      <c r="AV12" s="76"/>
+      <c r="AW12" s="76"/>
+      <c r="AX12" s="28"/>
+      <c r="AY12" s="28"/>
+      <c r="AZ12" s="28"/>
+      <c r="BA12" s="28"/>
+      <c r="BB12" s="28"/>
+      <c r="BC12" s="76"/>
+      <c r="BD12" s="2"/>
+      <c r="BE12" s="76"/>
+      <c r="BF12" s="2"/>
+      <c r="BG12" s="76"/>
+      <c r="BH12" s="28"/>
+      <c r="BI12" s="28"/>
+      <c r="BJ12" s="28"/>
+      <c r="BK12" s="28"/>
+      <c r="BL12" s="28"/>
+      <c r="BM12" s="28"/>
+      <c r="BN12" s="76"/>
+      <c r="BO12" s="76"/>
+      <c r="BP12" s="76"/>
+      <c r="BQ12" s="76"/>
+      <c r="BR12" s="76"/>
+      <c r="BS12" s="28"/>
+      <c r="BT12" s="28"/>
+      <c r="BU12" s="28"/>
+      <c r="BV12" s="28"/>
+      <c r="BW12" s="28"/>
+      <c r="BX12" s="76"/>
+      <c r="BY12" s="77"/>
+      <c r="BZ12" s="76"/>
+      <c r="CA12" s="77"/>
+      <c r="CB12" s="76"/>
+      <c r="CC12" s="28"/>
+      <c r="CD12" s="84"/>
     </row>
-    <row r="13" spans="11:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="11:82" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R13" s="5"/>
       <c r="S13" s="6"/>
       <c r="T13" s="5"/>
       <c r="U13" s="6"/>
       <c r="V13" s="5"/>
+      <c r="AP13" s="30"/>
+      <c r="AQ13" s="28"/>
+      <c r="AR13" s="28"/>
+      <c r="AS13" s="76"/>
+      <c r="AT13" s="76"/>
+      <c r="AU13" s="2"/>
+      <c r="AV13" s="76"/>
+      <c r="AW13" s="76"/>
+      <c r="AX13" s="28"/>
+      <c r="AY13" s="28"/>
+      <c r="AZ13" s="28"/>
+      <c r="BA13" s="28"/>
+      <c r="BB13" s="28"/>
+      <c r="BC13" s="76"/>
+      <c r="BD13" s="76"/>
+      <c r="BE13" s="76"/>
+      <c r="BF13" s="76"/>
+      <c r="BG13" s="76"/>
+      <c r="BH13" s="28"/>
+      <c r="BI13" s="28"/>
+      <c r="BJ13" s="28"/>
+      <c r="BK13" s="28"/>
+      <c r="BL13" s="28"/>
+      <c r="BM13" s="28"/>
+      <c r="BN13" s="76"/>
+      <c r="BO13" s="76"/>
+      <c r="BP13" s="93"/>
+      <c r="BQ13" s="76"/>
+      <c r="BR13" s="76"/>
+      <c r="BS13" s="28"/>
+      <c r="BT13" s="28"/>
+      <c r="BU13" s="28"/>
+      <c r="BV13" s="28"/>
+      <c r="BW13" s="28"/>
+      <c r="BX13" s="93"/>
+      <c r="BY13" s="76"/>
+      <c r="BZ13" s="76"/>
+      <c r="CA13" s="76"/>
+      <c r="CB13" s="93"/>
+      <c r="CC13" s="28"/>
+      <c r="CD13" s="84"/>
     </row>
-    <row r="14" spans="11:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="11:82" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R14" s="4"/>
       <c r="S14" s="5"/>
       <c r="T14" s="4"/>
       <c r="U14" s="5"/>
       <c r="V14" s="4"/>
+      <c r="AP14" s="30"/>
+      <c r="AQ14" s="28"/>
+      <c r="AR14" s="28"/>
+      <c r="AS14" s="28"/>
+      <c r="AT14" s="28"/>
+      <c r="AU14" s="28"/>
+      <c r="AV14" s="28"/>
+      <c r="AW14" s="28"/>
+      <c r="AX14" s="28"/>
+      <c r="AY14" s="28"/>
+      <c r="AZ14" s="28"/>
+      <c r="BA14" s="28"/>
+      <c r="BB14" s="28"/>
+      <c r="BC14" s="28"/>
+      <c r="BD14" s="28"/>
+      <c r="BE14" s="28"/>
+      <c r="BF14" s="28"/>
+      <c r="BG14" s="28"/>
+      <c r="BH14" s="28"/>
+      <c r="BI14" s="28"/>
+      <c r="BJ14" s="28"/>
+      <c r="BK14" s="28"/>
+      <c r="BL14" s="28"/>
+      <c r="BM14" s="28"/>
+      <c r="BN14" s="28"/>
+      <c r="BO14" s="28"/>
+      <c r="BP14" s="28"/>
+      <c r="BQ14" s="28"/>
+      <c r="BR14" s="28"/>
+      <c r="BS14" s="28"/>
+      <c r="BT14" s="28"/>
+      <c r="BU14" s="28"/>
+      <c r="BV14" s="28"/>
+      <c r="BW14" s="28"/>
+      <c r="BX14" s="28"/>
+      <c r="BY14" s="28"/>
+      <c r="BZ14" s="28"/>
+      <c r="CA14" s="28"/>
+      <c r="CB14" s="28"/>
+      <c r="CC14" s="28"/>
+      <c r="CD14" s="84"/>
     </row>
-    <row r="16" spans="11:54" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="11:82" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AP15" s="30"/>
+      <c r="AQ15" s="28"/>
+      <c r="AR15" s="28"/>
+      <c r="AS15" s="28"/>
+      <c r="AT15" s="28"/>
+      <c r="AU15" s="28"/>
+      <c r="AV15" s="28"/>
+      <c r="AW15" s="28"/>
+      <c r="AX15" s="28"/>
+      <c r="AY15" s="28"/>
+      <c r="AZ15" s="28"/>
+      <c r="BA15" s="28"/>
+      <c r="BB15" s="28"/>
+      <c r="BC15" s="28"/>
+      <c r="BD15" s="28"/>
+      <c r="BE15" s="28"/>
+      <c r="BF15" s="28"/>
+      <c r="BG15" s="28"/>
+      <c r="BH15" s="28"/>
+      <c r="BI15" s="28"/>
+      <c r="BJ15" s="28"/>
+      <c r="BK15" s="28"/>
+      <c r="BL15" s="28"/>
+      <c r="BM15" s="28"/>
+      <c r="BN15" s="28"/>
+      <c r="BO15" s="28"/>
+      <c r="BP15" s="28"/>
+      <c r="BQ15" s="28"/>
+      <c r="BR15" s="28"/>
+      <c r="BS15" s="28"/>
+      <c r="BT15" s="28"/>
+      <c r="BU15" s="28"/>
+      <c r="BV15" s="28"/>
+      <c r="BW15" s="28"/>
+      <c r="BX15" s="28"/>
+      <c r="BY15" s="28"/>
+      <c r="BZ15" s="28"/>
+      <c r="CA15" s="28"/>
+      <c r="CB15" s="28"/>
+      <c r="CC15" s="28"/>
+      <c r="CD15" s="84"/>
+    </row>
+    <row r="16" spans="11:82" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
@@ -1388,21 +3342,49 @@
       <c r="AM16" s="20"/>
       <c r="AN16" s="20"/>
       <c r="AO16" s="20"/>
-      <c r="AP16" s="20"/>
+      <c r="AP16" s="23"/>
       <c r="AQ16" s="20"/>
-      <c r="AR16" s="20"/>
-      <c r="AS16" s="20"/>
-      <c r="AT16" s="20"/>
-      <c r="AU16" s="20"/>
-      <c r="AV16" s="20"/>
-      <c r="AW16" s="20"/>
-      <c r="AX16" s="20"/>
-      <c r="AY16" s="20"/>
-      <c r="AZ16" s="20"/>
-      <c r="BA16" s="20"/>
-      <c r="BB16" s="20"/>
+      <c r="AR16" s="81"/>
+      <c r="AS16" s="21"/>
+      <c r="AT16" s="21"/>
+      <c r="AU16" s="21"/>
+      <c r="AV16" s="21"/>
+      <c r="AW16" s="21"/>
+      <c r="AX16" s="21"/>
+      <c r="AY16" s="21"/>
+      <c r="AZ16" s="21"/>
+      <c r="BA16" s="21"/>
+      <c r="BB16" s="21"/>
+      <c r="BC16" s="82"/>
+      <c r="BD16" s="82"/>
+      <c r="BE16" s="82"/>
+      <c r="BF16" s="82"/>
+      <c r="BG16" s="82"/>
+      <c r="BH16" s="83"/>
+      <c r="BI16" s="28"/>
+      <c r="BJ16" s="28"/>
+      <c r="BK16" s="28"/>
+      <c r="BL16" s="20"/>
+      <c r="BM16" s="81"/>
+      <c r="BN16" s="21"/>
+      <c r="BO16" s="21"/>
+      <c r="BP16" s="21"/>
+      <c r="BQ16" s="21"/>
+      <c r="BR16" s="21"/>
+      <c r="BS16" s="21"/>
+      <c r="BT16" s="21"/>
+      <c r="BU16" s="21"/>
+      <c r="BV16" s="21"/>
+      <c r="BW16" s="21"/>
+      <c r="BX16" s="82"/>
+      <c r="BY16" s="82"/>
+      <c r="BZ16" s="82"/>
+      <c r="CA16" s="82"/>
+      <c r="CB16" s="82"/>
+      <c r="CC16" s="83"/>
+      <c r="CD16" s="84"/>
     </row>
-    <row r="17" spans="10:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J17" s="29"/>
       <c r="K17" s="21"/>
       <c r="L17" s="21"/>
@@ -1435,21 +3417,57 @@
       <c r="AM17" s="20"/>
       <c r="AN17" s="20"/>
       <c r="AO17" s="20"/>
-      <c r="AP17" s="20"/>
+      <c r="AP17" s="23"/>
       <c r="AQ17" s="20"/>
-      <c r="AR17" s="20"/>
-      <c r="AS17" s="20"/>
-      <c r="AT17" s="20"/>
-      <c r="AU17" s="20"/>
-      <c r="AV17" s="20"/>
-      <c r="AW17" s="20"/>
+      <c r="AR17" s="23"/>
+      <c r="AS17" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT17" s="79"/>
+      <c r="AU17" s="79"/>
+      <c r="AV17" s="79"/>
+      <c r="AW17" s="80"/>
       <c r="AX17" s="20"/>
       <c r="AY17" s="20"/>
-      <c r="AZ17" s="20"/>
+      <c r="AZ17" s="5"/>
       <c r="BA17" s="20"/>
-      <c r="BB17" s="20"/>
+      <c r="BB17" s="28"/>
+      <c r="BC17" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="BD17" s="79"/>
+      <c r="BE17" s="79"/>
+      <c r="BF17" s="79"/>
+      <c r="BG17" s="80"/>
+      <c r="BH17" s="84"/>
+      <c r="BI17" s="28"/>
+      <c r="BJ17" s="28"/>
+      <c r="BK17" s="28"/>
+      <c r="BL17" s="20"/>
+      <c r="BM17" s="23"/>
+      <c r="BN17" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="BO17" s="79"/>
+      <c r="BP17" s="79"/>
+      <c r="BQ17" s="79"/>
+      <c r="BR17" s="80"/>
+      <c r="BS17" s="20"/>
+      <c r="BT17" s="20"/>
+      <c r="BU17" s="94"/>
+      <c r="BV17" s="20"/>
+      <c r="BW17" s="28"/>
+      <c r="BX17" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="BY17" s="79"/>
+      <c r="BZ17" s="79"/>
+      <c r="CA17" s="79"/>
+      <c r="CB17" s="80"/>
+      <c r="CC17" s="84"/>
+      <c r="CD17" s="84"/>
     </row>
-    <row r="18" spans="10:54" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J18" s="30"/>
       <c r="K18" s="20"/>
       <c r="L18" s="20"/>
@@ -1482,21 +3500,49 @@
       <c r="AM18" s="20"/>
       <c r="AN18" s="20"/>
       <c r="AO18" s="20"/>
-      <c r="AP18" s="20"/>
+      <c r="AP18" s="23"/>
       <c r="AQ18" s="20"/>
-      <c r="AR18" s="20"/>
-      <c r="AS18" s="20"/>
-      <c r="AT18" s="20"/>
-      <c r="AU18" s="20"/>
-      <c r="AV18" s="20"/>
-      <c r="AW18" s="20"/>
-      <c r="AX18" s="20"/>
-      <c r="AY18" s="20"/>
-      <c r="AZ18" s="20"/>
-      <c r="BA18" s="20"/>
-      <c r="BB18" s="20"/>
+      <c r="AR18" s="25"/>
+      <c r="AS18" s="26"/>
+      <c r="AT18" s="26"/>
+      <c r="AU18" s="26"/>
+      <c r="AV18" s="26"/>
+      <c r="AW18" s="26"/>
+      <c r="AX18" s="26"/>
+      <c r="AY18" s="26"/>
+      <c r="AZ18" s="26"/>
+      <c r="BA18" s="26"/>
+      <c r="BB18" s="26"/>
+      <c r="BC18" s="85"/>
+      <c r="BD18" s="85"/>
+      <c r="BE18" s="85"/>
+      <c r="BF18" s="85"/>
+      <c r="BG18" s="85"/>
+      <c r="BH18" s="86"/>
+      <c r="BI18" s="28"/>
+      <c r="BJ18" s="28"/>
+      <c r="BK18" s="28"/>
+      <c r="BL18" s="20"/>
+      <c r="BM18" s="25"/>
+      <c r="BN18" s="26"/>
+      <c r="BO18" s="26"/>
+      <c r="BP18" s="26"/>
+      <c r="BQ18" s="26"/>
+      <c r="BR18" s="26"/>
+      <c r="BS18" s="26"/>
+      <c r="BT18" s="26"/>
+      <c r="BU18" s="26"/>
+      <c r="BV18" s="26"/>
+      <c r="BW18" s="26"/>
+      <c r="BX18" s="85"/>
+      <c r="BY18" s="85"/>
+      <c r="BZ18" s="85"/>
+      <c r="CA18" s="85"/>
+      <c r="CB18" s="85"/>
+      <c r="CC18" s="86"/>
+      <c r="CD18" s="84"/>
     </row>
-    <row r="19" spans="10:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J19" s="30"/>
       <c r="K19" s="20"/>
       <c r="L19" s="41"/>
@@ -1529,7 +3575,7 @@
       <c r="AM19" s="20"/>
       <c r="AN19" s="20"/>
       <c r="AO19" s="20"/>
-      <c r="AP19" s="20"/>
+      <c r="AP19" s="23"/>
       <c r="AQ19" s="20"/>
       <c r="AR19" s="20"/>
       <c r="AS19" s="20"/>
@@ -1542,8 +3588,36 @@
       <c r="AZ19" s="20"/>
       <c r="BA19" s="20"/>
       <c r="BB19" s="20"/>
+      <c r="BC19" s="28"/>
+      <c r="BD19" s="28"/>
+      <c r="BE19" s="28"/>
+      <c r="BF19" s="28"/>
+      <c r="BG19" s="28"/>
+      <c r="BH19" s="28"/>
+      <c r="BI19" s="28"/>
+      <c r="BJ19" s="28"/>
+      <c r="BK19" s="28"/>
+      <c r="BL19" s="20"/>
+      <c r="BM19" s="20"/>
+      <c r="BN19" s="20"/>
+      <c r="BO19" s="20"/>
+      <c r="BP19" s="20"/>
+      <c r="BQ19" s="20"/>
+      <c r="BR19" s="20"/>
+      <c r="BS19" s="20"/>
+      <c r="BT19" s="20"/>
+      <c r="BU19" s="20"/>
+      <c r="BV19" s="20"/>
+      <c r="BW19" s="20"/>
+      <c r="BX19" s="28"/>
+      <c r="BY19" s="28"/>
+      <c r="BZ19" s="28"/>
+      <c r="CA19" s="28"/>
+      <c r="CB19" s="28"/>
+      <c r="CC19" s="28"/>
+      <c r="CD19" s="84"/>
     </row>
-    <row r="20" spans="10:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="10:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J20" s="30"/>
       <c r="K20" s="20"/>
       <c r="L20" s="44"/>
@@ -1576,7 +3650,7 @@
       <c r="AM20" s="20"/>
       <c r="AN20" s="20"/>
       <c r="AO20" s="20"/>
-      <c r="AP20" s="20"/>
+      <c r="AP20" s="23"/>
       <c r="AQ20" s="20"/>
       <c r="AR20" s="20"/>
       <c r="AS20" s="20"/>
@@ -1585,12 +3659,44 @@
       <c r="AV20" s="20"/>
       <c r="AW20" s="20"/>
       <c r="AX20" s="20"/>
-      <c r="AY20" s="20"/>
-      <c r="AZ20" s="20"/>
-      <c r="BA20" s="20"/>
+      <c r="AY20" s="87" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ20" s="88"/>
+      <c r="BA20" s="89"/>
       <c r="BB20" s="20"/>
+      <c r="BC20" s="28"/>
+      <c r="BD20" s="28"/>
+      <c r="BE20" s="28"/>
+      <c r="BF20" s="28"/>
+      <c r="BG20" s="28"/>
+      <c r="BH20" s="28"/>
+      <c r="BI20" s="28"/>
+      <c r="BJ20" s="28"/>
+      <c r="BK20" s="28"/>
+      <c r="BL20" s="20"/>
+      <c r="BM20" s="20"/>
+      <c r="BN20" s="20"/>
+      <c r="BO20" s="20"/>
+      <c r="BP20" s="20"/>
+      <c r="BQ20" s="20"/>
+      <c r="BR20" s="20"/>
+      <c r="BS20" s="20"/>
+      <c r="BT20" s="87" t="s">
+        <v>2</v>
+      </c>
+      <c r="BU20" s="88"/>
+      <c r="BV20" s="89"/>
+      <c r="BW20" s="20"/>
+      <c r="BX20" s="28"/>
+      <c r="BY20" s="28"/>
+      <c r="BZ20" s="28"/>
+      <c r="CA20" s="28"/>
+      <c r="CB20" s="28"/>
+      <c r="CC20" s="28"/>
+      <c r="CD20" s="84"/>
     </row>
-    <row r="21" spans="10:54" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J21" s="31"/>
       <c r="K21" s="26"/>
       <c r="L21" s="75"/>
@@ -1623,7 +3729,7 @@
       <c r="AM21" s="20"/>
       <c r="AN21" s="20"/>
       <c r="AO21" s="20"/>
-      <c r="AP21" s="20"/>
+      <c r="AP21" s="23"/>
       <c r="AQ21" s="20"/>
       <c r="AR21" s="20"/>
       <c r="AS21" s="20"/>
@@ -1632,12 +3738,40 @@
       <c r="AV21" s="20"/>
       <c r="AW21" s="20"/>
       <c r="AX21" s="20"/>
-      <c r="AY21" s="20"/>
-      <c r="AZ21" s="20"/>
-      <c r="BA21" s="20"/>
+      <c r="AY21" s="90"/>
+      <c r="AZ21" s="91"/>
+      <c r="BA21" s="92"/>
       <c r="BB21" s="20"/>
+      <c r="BC21" s="28"/>
+      <c r="BD21" s="28"/>
+      <c r="BE21" s="28"/>
+      <c r="BF21" s="28"/>
+      <c r="BG21" s="28"/>
+      <c r="BH21" s="28"/>
+      <c r="BI21" s="28"/>
+      <c r="BJ21" s="28"/>
+      <c r="BK21" s="28"/>
+      <c r="BL21" s="20"/>
+      <c r="BM21" s="20"/>
+      <c r="BN21" s="20"/>
+      <c r="BO21" s="20"/>
+      <c r="BP21" s="20"/>
+      <c r="BQ21" s="20"/>
+      <c r="BR21" s="20"/>
+      <c r="BS21" s="20"/>
+      <c r="BT21" s="90"/>
+      <c r="BU21" s="91"/>
+      <c r="BV21" s="92"/>
+      <c r="BW21" s="20"/>
+      <c r="BX21" s="28"/>
+      <c r="BY21" s="28"/>
+      <c r="BZ21" s="28"/>
+      <c r="CA21" s="28"/>
+      <c r="CB21" s="28"/>
+      <c r="CC21" s="28"/>
+      <c r="CD21" s="84"/>
     </row>
-    <row r="22" spans="10:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J22" s="34"/>
       <c r="K22" s="20"/>
       <c r="L22" s="73"/>
@@ -1670,7 +3804,7 @@
       <c r="AM22" s="20"/>
       <c r="AN22" s="20"/>
       <c r="AO22" s="20"/>
-      <c r="AP22" s="20"/>
+      <c r="AP22" s="23"/>
       <c r="AQ22" s="20"/>
       <c r="AR22" s="20"/>
       <c r="AS22" s="20"/>
@@ -1683,8 +3817,36 @@
       <c r="AZ22" s="20"/>
       <c r="BA22" s="20"/>
       <c r="BB22" s="20"/>
+      <c r="BC22" s="28"/>
+      <c r="BD22" s="28"/>
+      <c r="BE22" s="28"/>
+      <c r="BF22" s="28"/>
+      <c r="BG22" s="28"/>
+      <c r="BH22" s="28"/>
+      <c r="BI22" s="28"/>
+      <c r="BJ22" s="28"/>
+      <c r="BK22" s="28"/>
+      <c r="BL22" s="20"/>
+      <c r="BM22" s="20"/>
+      <c r="BN22" s="20"/>
+      <c r="BO22" s="20"/>
+      <c r="BP22" s="20"/>
+      <c r="BQ22" s="20"/>
+      <c r="BR22" s="20"/>
+      <c r="BS22" s="20"/>
+      <c r="BT22" s="20"/>
+      <c r="BU22" s="20"/>
+      <c r="BV22" s="20"/>
+      <c r="BW22" s="20"/>
+      <c r="BX22" s="28"/>
+      <c r="BY22" s="28"/>
+      <c r="BZ22" s="28"/>
+      <c r="CA22" s="28"/>
+      <c r="CB22" s="28"/>
+      <c r="CC22" s="28"/>
+      <c r="CD22" s="84"/>
     </row>
-    <row r="23" spans="10:54" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J23" s="34"/>
       <c r="K23" s="20"/>
       <c r="L23" s="44"/>
@@ -1717,21 +3879,53 @@
       <c r="AM23" s="20"/>
       <c r="AN23" s="20"/>
       <c r="AO23" s="20"/>
-      <c r="AP23" s="20"/>
-      <c r="AQ23" s="20"/>
-      <c r="AR23" s="20"/>
-      <c r="AS23" s="20"/>
-      <c r="AT23" s="20"/>
-      <c r="AU23" s="20"/>
-      <c r="AV23" s="20"/>
-      <c r="AW23" s="20"/>
-      <c r="AX23" s="20"/>
-      <c r="AY23" s="20"/>
-      <c r="AZ23" s="20"/>
-      <c r="BA23" s="20"/>
-      <c r="BB23" s="20"/>
+      <c r="AP23" s="81"/>
+      <c r="AQ23" s="21"/>
+      <c r="AR23" s="21"/>
+      <c r="AS23" s="21"/>
+      <c r="AT23" s="21"/>
+      <c r="AU23" s="21"/>
+      <c r="AV23" s="21"/>
+      <c r="AW23" s="21"/>
+      <c r="AX23" s="21"/>
+      <c r="AY23" s="21"/>
+      <c r="AZ23" s="21"/>
+      <c r="BA23" s="21"/>
+      <c r="BB23" s="21"/>
+      <c r="BC23" s="82"/>
+      <c r="BD23" s="82"/>
+      <c r="BE23" s="82"/>
+      <c r="BF23" s="82"/>
+      <c r="BG23" s="82"/>
+      <c r="BH23" s="82"/>
+      <c r="BI23" s="95" t="s">
+        <v>6</v>
+      </c>
+      <c r="BJ23" s="96"/>
+      <c r="BK23" s="96"/>
+      <c r="BL23" s="96"/>
+      <c r="BM23" s="96"/>
+      <c r="BN23" s="96"/>
+      <c r="BO23" s="97"/>
+      <c r="BP23" s="82"/>
+      <c r="BQ23" s="82"/>
+      <c r="BR23" s="82"/>
+      <c r="BS23" s="82"/>
+      <c r="BT23" s="82"/>
+      <c r="BU23" s="82"/>
+      <c r="BV23" s="82"/>
+      <c r="BW23" s="82"/>
+      <c r="BX23" s="82"/>
+      <c r="BY23" s="82"/>
+      <c r="BZ23" s="82"/>
+      <c r="CA23" s="82"/>
+      <c r="CB23" s="82"/>
+      <c r="CC23" s="82"/>
+      <c r="CD23" s="82"/>
+      <c r="CE23" s="82"/>
+      <c r="CF23" s="83"/>
     </row>
-    <row r="24" spans="10:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="10:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J24" s="34"/>
       <c r="K24" s="20"/>
       <c r="L24" s="44"/>
@@ -1764,21 +3958,51 @@
       <c r="AM24" s="20"/>
       <c r="AN24" s="20"/>
       <c r="AO24" s="20"/>
-      <c r="AP24" s="20"/>
+      <c r="AP24" s="23"/>
       <c r="AQ24" s="20"/>
-      <c r="AR24" s="20"/>
-      <c r="AS24" s="20"/>
-      <c r="AT24" s="20"/>
-      <c r="AU24" s="20"/>
-      <c r="AV24" s="20"/>
-      <c r="AW24" s="20"/>
-      <c r="AX24" s="20"/>
-      <c r="AY24" s="20"/>
-      <c r="AZ24" s="20"/>
-      <c r="BA24" s="20"/>
-      <c r="BB24" s="20"/>
+      <c r="AR24" s="28"/>
+      <c r="AS24" s="76"/>
+      <c r="AT24" s="76"/>
+      <c r="AU24" s="2"/>
+      <c r="AV24" s="76"/>
+      <c r="AW24" s="76"/>
+      <c r="AX24" s="28"/>
+      <c r="AY24" s="28"/>
+      <c r="AZ24" s="28"/>
+      <c r="BA24" s="28"/>
+      <c r="BB24" s="28"/>
+      <c r="BC24" s="76"/>
+      <c r="BD24" s="76"/>
+      <c r="BE24" s="76"/>
+      <c r="BF24" s="76"/>
+      <c r="BG24" s="76"/>
+      <c r="BH24" s="28"/>
+      <c r="BI24" s="28"/>
+      <c r="BJ24" s="28"/>
+      <c r="BK24" s="28"/>
+      <c r="BL24" s="28"/>
+      <c r="BM24" s="28"/>
+      <c r="BN24" s="28"/>
+      <c r="BO24" s="28"/>
+      <c r="BP24" s="28"/>
+      <c r="BQ24" s="28"/>
+      <c r="BR24" s="28"/>
+      <c r="BS24" s="28"/>
+      <c r="BT24" s="28"/>
+      <c r="BU24" s="28"/>
+      <c r="BV24" s="28"/>
+      <c r="BW24" s="28"/>
+      <c r="BX24" s="28"/>
+      <c r="BY24" s="28"/>
+      <c r="BZ24" s="28"/>
+      <c r="CA24" s="28"/>
+      <c r="CB24" s="28"/>
+      <c r="CC24" s="28"/>
+      <c r="CD24" s="28"/>
+      <c r="CE24" s="28"/>
+      <c r="CF24" s="84"/>
     </row>
-    <row r="25" spans="10:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="10:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J25" s="34"/>
       <c r="K25" s="20"/>
       <c r="L25" s="44"/>
@@ -1811,21 +4035,51 @@
       <c r="AM25" s="20"/>
       <c r="AN25" s="20"/>
       <c r="AO25" s="20"/>
-      <c r="AP25" s="20"/>
+      <c r="AP25" s="23"/>
       <c r="AQ25" s="20"/>
-      <c r="AR25" s="20"/>
-      <c r="AS25" s="20"/>
-      <c r="AT25" s="20"/>
-      <c r="AU25" s="20"/>
-      <c r="AV25" s="20"/>
-      <c r="AW25" s="20"/>
-      <c r="AX25" s="20"/>
-      <c r="AY25" s="20"/>
-      <c r="AZ25" s="20"/>
-      <c r="BA25" s="20"/>
-      <c r="BB25" s="20"/>
+      <c r="AR25" s="28"/>
+      <c r="AS25" s="76"/>
+      <c r="AT25" s="76"/>
+      <c r="AU25" s="76"/>
+      <c r="AV25" s="76"/>
+      <c r="AW25" s="76"/>
+      <c r="AX25" s="28"/>
+      <c r="AY25" s="28"/>
+      <c r="AZ25" s="28"/>
+      <c r="BA25" s="28"/>
+      <c r="BB25" s="28"/>
+      <c r="BC25" s="76"/>
+      <c r="BD25" s="77"/>
+      <c r="BE25" s="76"/>
+      <c r="BF25" s="77"/>
+      <c r="BG25" s="76"/>
+      <c r="BH25" s="28"/>
+      <c r="BI25" s="28"/>
+      <c r="BJ25" s="28"/>
+      <c r="BK25" s="28"/>
+      <c r="BL25" s="28"/>
+      <c r="BM25" s="28"/>
+      <c r="BN25" s="28"/>
+      <c r="BO25" s="76"/>
+      <c r="BP25" s="76"/>
+      <c r="BQ25" s="2"/>
+      <c r="BR25" s="28"/>
+      <c r="BS25" s="28"/>
+      <c r="BT25" s="28"/>
+      <c r="BU25" s="28"/>
+      <c r="BV25" s="28"/>
+      <c r="BW25" s="28"/>
+      <c r="BX25" s="28"/>
+      <c r="BY25" s="2"/>
+      <c r="BZ25" s="76"/>
+      <c r="CA25" s="77"/>
+      <c r="CB25" s="28"/>
+      <c r="CC25" s="28"/>
+      <c r="CD25" s="28"/>
+      <c r="CE25" s="28"/>
+      <c r="CF25" s="84"/>
     </row>
-    <row r="26" spans="10:54" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J26" s="34"/>
       <c r="K26" s="20"/>
       <c r="L26" s="44"/>
@@ -1858,21 +4112,51 @@
       <c r="AM26" s="20"/>
       <c r="AN26" s="20"/>
       <c r="AO26" s="20"/>
-      <c r="AP26" s="20"/>
+      <c r="AP26" s="23"/>
       <c r="AQ26" s="20"/>
-      <c r="AR26" s="20"/>
-      <c r="AS26" s="20"/>
-      <c r="AT26" s="20"/>
-      <c r="AU26" s="20"/>
-      <c r="AV26" s="20"/>
-      <c r="AW26" s="20"/>
-      <c r="AX26" s="20"/>
-      <c r="AY26" s="20"/>
-      <c r="AZ26" s="20"/>
-      <c r="BA26" s="20"/>
-      <c r="BB26" s="20"/>
+      <c r="AR26" s="28"/>
+      <c r="AS26" s="77"/>
+      <c r="AT26" s="76"/>
+      <c r="AU26" s="2"/>
+      <c r="AV26" s="76"/>
+      <c r="AW26" s="77"/>
+      <c r="AX26" s="28"/>
+      <c r="AY26" s="28"/>
+      <c r="AZ26" s="5"/>
+      <c r="BA26" s="28"/>
+      <c r="BB26" s="28"/>
+      <c r="BC26" s="2"/>
+      <c r="BD26" s="76"/>
+      <c r="BE26" s="2"/>
+      <c r="BF26" s="76"/>
+      <c r="BG26" s="2"/>
+      <c r="BH26" s="28"/>
+      <c r="BI26" s="28"/>
+      <c r="BJ26" s="28"/>
+      <c r="BK26" s="5"/>
+      <c r="BL26" s="28"/>
+      <c r="BM26" s="28"/>
+      <c r="BN26" s="28"/>
+      <c r="BO26" s="76"/>
+      <c r="BP26" s="2"/>
+      <c r="BQ26" s="76"/>
+      <c r="BR26" s="28"/>
+      <c r="BS26" s="28"/>
+      <c r="BT26" s="28"/>
+      <c r="BU26" s="5"/>
+      <c r="BV26" s="28"/>
+      <c r="BW26" s="28"/>
+      <c r="BX26" s="28"/>
+      <c r="BY26" s="76"/>
+      <c r="BZ26" s="2"/>
+      <c r="CA26" s="76"/>
+      <c r="CB26" s="28"/>
+      <c r="CC26" s="28"/>
+      <c r="CD26" s="28"/>
+      <c r="CE26" s="28"/>
+      <c r="CF26" s="84"/>
     </row>
-    <row r="27" spans="10:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="10:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J27" s="34"/>
       <c r="K27" s="20"/>
       <c r="L27" s="44"/>
@@ -1905,21 +4189,51 @@
       <c r="AM27" s="20"/>
       <c r="AN27" s="20"/>
       <c r="AO27" s="20"/>
-      <c r="AP27" s="20"/>
+      <c r="AP27" s="23"/>
       <c r="AQ27" s="20"/>
-      <c r="AR27" s="20"/>
-      <c r="AS27" s="20"/>
-      <c r="AT27" s="20"/>
-      <c r="AU27" s="20"/>
-      <c r="AV27" s="20"/>
-      <c r="AW27" s="20"/>
-      <c r="AX27" s="20"/>
-      <c r="AY27" s="20"/>
-      <c r="AZ27" s="20"/>
-      <c r="BA27" s="20"/>
-      <c r="BB27" s="20"/>
+      <c r="AR27" s="28"/>
+      <c r="AS27" s="76"/>
+      <c r="AT27" s="76"/>
+      <c r="AU27" s="76"/>
+      <c r="AV27" s="76"/>
+      <c r="AW27" s="76"/>
+      <c r="AX27" s="28"/>
+      <c r="AY27" s="28"/>
+      <c r="AZ27" s="28"/>
+      <c r="BA27" s="28"/>
+      <c r="BB27" s="28"/>
+      <c r="BC27" s="76"/>
+      <c r="BD27" s="77"/>
+      <c r="BE27" s="76"/>
+      <c r="BF27" s="77"/>
+      <c r="BG27" s="77"/>
+      <c r="BH27" s="28"/>
+      <c r="BI27" s="28"/>
+      <c r="BJ27" s="28"/>
+      <c r="BK27" s="28"/>
+      <c r="BL27" s="28"/>
+      <c r="BM27" s="28"/>
+      <c r="BN27" s="28"/>
+      <c r="BO27" s="2"/>
+      <c r="BP27" s="76"/>
+      <c r="BQ27" s="76"/>
+      <c r="BR27" s="28"/>
+      <c r="BS27" s="28"/>
+      <c r="BT27" s="28"/>
+      <c r="BU27" s="28"/>
+      <c r="BV27" s="28"/>
+      <c r="BW27" s="28"/>
+      <c r="BX27" s="28"/>
+      <c r="BY27" s="77"/>
+      <c r="BZ27" s="76"/>
+      <c r="CA27" s="2"/>
+      <c r="CB27" s="28"/>
+      <c r="CC27" s="28"/>
+      <c r="CD27" s="28"/>
+      <c r="CE27" s="28"/>
+      <c r="CF27" s="84"/>
     </row>
-    <row r="28" spans="10:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="10:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J28" s="34"/>
       <c r="K28" s="20"/>
       <c r="L28" s="44"/>
@@ -1952,21 +4266,51 @@
       <c r="AM28" s="20"/>
       <c r="AN28" s="20"/>
       <c r="AO28" s="20"/>
-      <c r="AP28" s="20"/>
+      <c r="AP28" s="23"/>
       <c r="AQ28" s="20"/>
-      <c r="AR28" s="20"/>
-      <c r="AS28" s="20"/>
-      <c r="AT28" s="20"/>
-      <c r="AU28" s="20"/>
-      <c r="AV28" s="20"/>
-      <c r="AW28" s="20"/>
-      <c r="AX28" s="20"/>
-      <c r="AY28" s="20"/>
-      <c r="AZ28" s="20"/>
-      <c r="BA28" s="20"/>
-      <c r="BB28" s="20"/>
+      <c r="AR28" s="28"/>
+      <c r="AS28" s="76"/>
+      <c r="AT28" s="76"/>
+      <c r="AU28" s="2"/>
+      <c r="AV28" s="76"/>
+      <c r="AW28" s="76"/>
+      <c r="AX28" s="28"/>
+      <c r="AY28" s="28"/>
+      <c r="AZ28" s="28"/>
+      <c r="BA28" s="28"/>
+      <c r="BB28" s="28"/>
+      <c r="BC28" s="76"/>
+      <c r="BD28" s="76"/>
+      <c r="BE28" s="76"/>
+      <c r="BF28" s="76"/>
+      <c r="BG28" s="76"/>
+      <c r="BH28" s="28"/>
+      <c r="BI28" s="28"/>
+      <c r="BJ28" s="28"/>
+      <c r="BK28" s="28"/>
+      <c r="BL28" s="28"/>
+      <c r="BM28" s="28"/>
+      <c r="BN28" s="28"/>
+      <c r="BO28" s="28"/>
+      <c r="BP28" s="28"/>
+      <c r="BQ28" s="28"/>
+      <c r="BR28" s="28"/>
+      <c r="BS28" s="28"/>
+      <c r="BT28" s="28"/>
+      <c r="BU28" s="28"/>
+      <c r="BV28" s="28"/>
+      <c r="BW28" s="28"/>
+      <c r="BX28" s="28"/>
+      <c r="BY28" s="28"/>
+      <c r="BZ28" s="28"/>
+      <c r="CA28" s="28"/>
+      <c r="CB28" s="28"/>
+      <c r="CC28" s="28"/>
+      <c r="CD28" s="28"/>
+      <c r="CE28" s="28"/>
+      <c r="CF28" s="84"/>
     </row>
-    <row r="29" spans="10:54" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J29" s="34"/>
       <c r="K29" s="20"/>
       <c r="L29" s="46"/>
@@ -1999,21 +4343,51 @@
       <c r="AM29" s="20"/>
       <c r="AN29" s="20"/>
       <c r="AO29" s="20"/>
-      <c r="AP29" s="20"/>
+      <c r="AP29" s="23"/>
       <c r="AQ29" s="20"/>
-      <c r="AR29" s="20"/>
-      <c r="AS29" s="20"/>
-      <c r="AT29" s="20"/>
-      <c r="AU29" s="20"/>
-      <c r="AV29" s="20"/>
-      <c r="AW29" s="20"/>
-      <c r="AX29" s="20"/>
-      <c r="AY29" s="20"/>
-      <c r="AZ29" s="20"/>
-      <c r="BA29" s="20"/>
-      <c r="BB29" s="20"/>
+      <c r="AR29" s="28"/>
+      <c r="AS29" s="28"/>
+      <c r="AT29" s="28"/>
+      <c r="AU29" s="28"/>
+      <c r="AV29" s="28"/>
+      <c r="AW29" s="28"/>
+      <c r="AX29" s="28"/>
+      <c r="AY29" s="28"/>
+      <c r="AZ29" s="28"/>
+      <c r="BA29" s="28"/>
+      <c r="BB29" s="28"/>
+      <c r="BC29" s="28"/>
+      <c r="BD29" s="28"/>
+      <c r="BE29" s="28"/>
+      <c r="BF29" s="28"/>
+      <c r="BG29" s="28"/>
+      <c r="BH29" s="28"/>
+      <c r="BI29" s="28"/>
+      <c r="BJ29" s="28"/>
+      <c r="BK29" s="28"/>
+      <c r="BL29" s="28"/>
+      <c r="BM29" s="28"/>
+      <c r="BN29" s="28"/>
+      <c r="BO29" s="28"/>
+      <c r="BP29" s="28"/>
+      <c r="BQ29" s="28"/>
+      <c r="BR29" s="28"/>
+      <c r="BS29" s="28"/>
+      <c r="BT29" s="28"/>
+      <c r="BU29" s="28"/>
+      <c r="BV29" s="28"/>
+      <c r="BW29" s="28"/>
+      <c r="BX29" s="28"/>
+      <c r="BY29" s="28"/>
+      <c r="BZ29" s="28"/>
+      <c r="CA29" s="28"/>
+      <c r="CB29" s="28"/>
+      <c r="CC29" s="28"/>
+      <c r="CD29" s="28"/>
+      <c r="CE29" s="28"/>
+      <c r="CF29" s="84"/>
     </row>
-    <row r="30" spans="10:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J30" s="34"/>
       <c r="K30" s="20"/>
       <c r="L30" s="20"/>
@@ -2046,21 +4420,51 @@
       <c r="AM30" s="20"/>
       <c r="AN30" s="20"/>
       <c r="AO30" s="20"/>
-      <c r="AP30" s="20"/>
+      <c r="AP30" s="23"/>
       <c r="AQ30" s="20"/>
-      <c r="AR30" s="20"/>
-      <c r="AS30" s="20"/>
-      <c r="AT30" s="20"/>
-      <c r="AU30" s="20"/>
-      <c r="AV30" s="20"/>
-      <c r="AW30" s="20"/>
-      <c r="AX30" s="20"/>
-      <c r="AY30" s="20"/>
-      <c r="AZ30" s="20"/>
-      <c r="BA30" s="20"/>
-      <c r="BB30" s="20"/>
+      <c r="AR30" s="28"/>
+      <c r="AS30" s="28"/>
+      <c r="AT30" s="28"/>
+      <c r="AU30" s="28"/>
+      <c r="AV30" s="28"/>
+      <c r="AW30" s="28"/>
+      <c r="AX30" s="28"/>
+      <c r="AY30" s="28"/>
+      <c r="AZ30" s="28"/>
+      <c r="BA30" s="28"/>
+      <c r="BB30" s="28"/>
+      <c r="BC30" s="28"/>
+      <c r="BD30" s="28"/>
+      <c r="BE30" s="28"/>
+      <c r="BF30" s="28"/>
+      <c r="BG30" s="28"/>
+      <c r="BH30" s="28"/>
+      <c r="BI30" s="28"/>
+      <c r="BJ30" s="28"/>
+      <c r="BK30" s="28"/>
+      <c r="BL30" s="28"/>
+      <c r="BM30" s="28"/>
+      <c r="BN30" s="28"/>
+      <c r="BO30" s="28"/>
+      <c r="BP30" s="28"/>
+      <c r="BQ30" s="28"/>
+      <c r="BR30" s="28"/>
+      <c r="BS30" s="28"/>
+      <c r="BT30" s="28"/>
+      <c r="BU30" s="28"/>
+      <c r="BV30" s="28"/>
+      <c r="BW30" s="28"/>
+      <c r="BX30" s="28"/>
+      <c r="BY30" s="28"/>
+      <c r="BZ30" s="28"/>
+      <c r="CA30" s="28"/>
+      <c r="CB30" s="28"/>
+      <c r="CC30" s="28"/>
+      <c r="CD30" s="28"/>
+      <c r="CE30" s="28"/>
+      <c r="CF30" s="84"/>
     </row>
-    <row r="31" spans="10:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J31" s="34"/>
       <c r="K31" s="20"/>
       <c r="L31" s="20"/>
@@ -2093,21 +4497,51 @@
       <c r="AM31" s="20"/>
       <c r="AN31" s="20"/>
       <c r="AO31" s="20"/>
-      <c r="AP31" s="20"/>
+      <c r="AP31" s="23"/>
       <c r="AQ31" s="20"/>
-      <c r="AR31" s="20"/>
-      <c r="AS31" s="20"/>
-      <c r="AT31" s="20"/>
-      <c r="AU31" s="20"/>
-      <c r="AV31" s="20"/>
-      <c r="AW31" s="20"/>
-      <c r="AX31" s="20"/>
-      <c r="AY31" s="20"/>
-      <c r="AZ31" s="20"/>
-      <c r="BA31" s="20"/>
-      <c r="BB31" s="20"/>
+      <c r="AR31" s="81"/>
+      <c r="AS31" s="21"/>
+      <c r="AT31" s="21"/>
+      <c r="AU31" s="21"/>
+      <c r="AV31" s="21"/>
+      <c r="AW31" s="21"/>
+      <c r="AX31" s="21"/>
+      <c r="AY31" s="21"/>
+      <c r="AZ31" s="21"/>
+      <c r="BA31" s="21"/>
+      <c r="BB31" s="21"/>
+      <c r="BC31" s="82"/>
+      <c r="BD31" s="82"/>
+      <c r="BE31" s="82"/>
+      <c r="BF31" s="82"/>
+      <c r="BG31" s="82"/>
+      <c r="BH31" s="83"/>
+      <c r="BI31" s="28"/>
+      <c r="BJ31" s="28"/>
+      <c r="BK31" s="28"/>
+      <c r="BL31" s="28"/>
+      <c r="BM31" s="29"/>
+      <c r="BN31" s="82"/>
+      <c r="BO31" s="82"/>
+      <c r="BP31" s="82"/>
+      <c r="BQ31" s="82"/>
+      <c r="BR31" s="82"/>
+      <c r="BS31" s="82"/>
+      <c r="BT31" s="82"/>
+      <c r="BU31" s="82"/>
+      <c r="BV31" s="82"/>
+      <c r="BW31" s="82"/>
+      <c r="BX31" s="82"/>
+      <c r="BY31" s="82"/>
+      <c r="BZ31" s="82"/>
+      <c r="CA31" s="82"/>
+      <c r="CB31" s="82"/>
+      <c r="CC31" s="83"/>
+      <c r="CD31" s="28"/>
+      <c r="CE31" s="28"/>
+      <c r="CF31" s="84"/>
     </row>
-    <row r="32" spans="10:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J32" s="34"/>
       <c r="K32" s="20"/>
       <c r="L32" s="20"/>
@@ -2140,21 +4574,59 @@
       <c r="AM32" s="20"/>
       <c r="AN32" s="20"/>
       <c r="AO32" s="20"/>
-      <c r="AP32" s="20"/>
+      <c r="AP32" s="23"/>
       <c r="AQ32" s="20"/>
-      <c r="AR32" s="20"/>
-      <c r="AS32" s="20"/>
-      <c r="AT32" s="20"/>
-      <c r="AU32" s="20"/>
-      <c r="AV32" s="20"/>
-      <c r="AW32" s="20"/>
+      <c r="AR32" s="23"/>
+      <c r="AS32" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT32" s="79"/>
+      <c r="AU32" s="79"/>
+      <c r="AV32" s="79"/>
+      <c r="AW32" s="80"/>
       <c r="AX32" s="20"/>
       <c r="AY32" s="20"/>
-      <c r="AZ32" s="20"/>
+      <c r="AZ32" s="5"/>
       <c r="BA32" s="20"/>
-      <c r="BB32" s="20"/>
+      <c r="BB32" s="28"/>
+      <c r="BC32" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD32" s="79"/>
+      <c r="BE32" s="79"/>
+      <c r="BF32" s="79"/>
+      <c r="BG32" s="80"/>
+      <c r="BH32" s="84"/>
+      <c r="BI32" s="28"/>
+      <c r="BJ32" s="28"/>
+      <c r="BK32" s="28"/>
+      <c r="BL32" s="28"/>
+      <c r="BM32" s="30"/>
+      <c r="BN32" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="BO32" s="79"/>
+      <c r="BP32" s="79"/>
+      <c r="BQ32" s="79"/>
+      <c r="BR32" s="80"/>
+      <c r="BS32" s="28"/>
+      <c r="BT32" s="28"/>
+      <c r="BU32" s="5"/>
+      <c r="BV32" s="28"/>
+      <c r="BW32" s="28"/>
+      <c r="BX32" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="BY32" s="79"/>
+      <c r="BZ32" s="79"/>
+      <c r="CA32" s="79"/>
+      <c r="CB32" s="80"/>
+      <c r="CC32" s="84"/>
+      <c r="CD32" s="28"/>
+      <c r="CE32" s="28"/>
+      <c r="CF32" s="84"/>
     </row>
-    <row r="33" spans="10:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J33" s="34"/>
       <c r="K33" s="20"/>
       <c r="L33" s="20"/>
@@ -2187,21 +4659,51 @@
       <c r="AM33" s="20"/>
       <c r="AN33" s="20"/>
       <c r="AO33" s="20"/>
-      <c r="AP33" s="20"/>
+      <c r="AP33" s="23"/>
       <c r="AQ33" s="20"/>
-      <c r="AR33" s="20"/>
-      <c r="AS33" s="20"/>
-      <c r="AT33" s="20"/>
-      <c r="AU33" s="20"/>
-      <c r="AV33" s="20"/>
-      <c r="AW33" s="20"/>
-      <c r="AX33" s="20"/>
-      <c r="AY33" s="20"/>
-      <c r="AZ33" s="20"/>
-      <c r="BA33" s="20"/>
-      <c r="BB33" s="20"/>
+      <c r="AR33" s="25"/>
+      <c r="AS33" s="26"/>
+      <c r="AT33" s="26"/>
+      <c r="AU33" s="26"/>
+      <c r="AV33" s="26"/>
+      <c r="AW33" s="26"/>
+      <c r="AX33" s="26"/>
+      <c r="AY33" s="26"/>
+      <c r="AZ33" s="26"/>
+      <c r="BA33" s="26"/>
+      <c r="BB33" s="26"/>
+      <c r="BC33" s="85"/>
+      <c r="BD33" s="85"/>
+      <c r="BE33" s="85"/>
+      <c r="BF33" s="85"/>
+      <c r="BG33" s="85"/>
+      <c r="BH33" s="86"/>
+      <c r="BI33" s="28"/>
+      <c r="BJ33" s="28"/>
+      <c r="BK33" s="28"/>
+      <c r="BL33" s="28"/>
+      <c r="BM33" s="31"/>
+      <c r="BN33" s="85"/>
+      <c r="BO33" s="85"/>
+      <c r="BP33" s="85"/>
+      <c r="BQ33" s="85"/>
+      <c r="BR33" s="85"/>
+      <c r="BS33" s="85"/>
+      <c r="BT33" s="85"/>
+      <c r="BU33" s="85"/>
+      <c r="BV33" s="85"/>
+      <c r="BW33" s="85"/>
+      <c r="BX33" s="85"/>
+      <c r="BY33" s="85"/>
+      <c r="BZ33" s="85"/>
+      <c r="CA33" s="85"/>
+      <c r="CB33" s="85"/>
+      <c r="CC33" s="86"/>
+      <c r="CD33" s="28"/>
+      <c r="CE33" s="28"/>
+      <c r="CF33" s="84"/>
     </row>
-    <row r="34" spans="10:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J34" s="34"/>
       <c r="K34" s="20"/>
       <c r="L34" s="20"/>
@@ -2234,7 +4736,7 @@
       <c r="AM34" s="20"/>
       <c r="AN34" s="20"/>
       <c r="AO34" s="20"/>
-      <c r="AP34" s="20"/>
+      <c r="AP34" s="23"/>
       <c r="AQ34" s="20"/>
       <c r="AR34" s="20"/>
       <c r="AS34" s="20"/>
@@ -2247,8 +4749,38 @@
       <c r="AZ34" s="20"/>
       <c r="BA34" s="20"/>
       <c r="BB34" s="20"/>
+      <c r="BC34" s="28"/>
+      <c r="BD34" s="28"/>
+      <c r="BE34" s="28"/>
+      <c r="BF34" s="28"/>
+      <c r="BG34" s="28"/>
+      <c r="BH34" s="28"/>
+      <c r="BI34" s="28"/>
+      <c r="BJ34" s="28"/>
+      <c r="BK34" s="28"/>
+      <c r="BL34" s="28"/>
+      <c r="BM34" s="28"/>
+      <c r="BN34" s="28"/>
+      <c r="BO34" s="28"/>
+      <c r="BP34" s="28"/>
+      <c r="BQ34" s="28"/>
+      <c r="BR34" s="28"/>
+      <c r="BS34" s="28"/>
+      <c r="BT34" s="28"/>
+      <c r="BU34" s="28"/>
+      <c r="BV34" s="28"/>
+      <c r="BW34" s="28"/>
+      <c r="BX34" s="28"/>
+      <c r="BY34" s="28"/>
+      <c r="BZ34" s="28"/>
+      <c r="CA34" s="28"/>
+      <c r="CB34" s="28"/>
+      <c r="CC34" s="28"/>
+      <c r="CD34" s="28"/>
+      <c r="CE34" s="28"/>
+      <c r="CF34" s="84"/>
     </row>
-    <row r="35" spans="10:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J35" s="34"/>
       <c r="K35" s="20"/>
       <c r="L35" s="20"/>
@@ -2281,7 +4813,7 @@
       <c r="AM35" s="20"/>
       <c r="AN35" s="20"/>
       <c r="AO35" s="20"/>
-      <c r="AP35" s="20"/>
+      <c r="AP35" s="23"/>
       <c r="AQ35" s="20"/>
       <c r="AR35" s="20"/>
       <c r="AS35" s="20"/>
@@ -2289,13 +4821,43 @@
       <c r="AU35" s="20"/>
       <c r="AV35" s="20"/>
       <c r="AW35" s="20"/>
-      <c r="AX35" s="20"/>
-      <c r="AY35" s="20"/>
-      <c r="AZ35" s="20"/>
-      <c r="BA35" s="20"/>
-      <c r="BB35" s="20"/>
+      <c r="AX35" s="81"/>
+      <c r="AY35" s="82"/>
+      <c r="AZ35" s="82"/>
+      <c r="BA35" s="82"/>
+      <c r="BB35" s="21"/>
+      <c r="BC35" s="82"/>
+      <c r="BD35" s="82"/>
+      <c r="BE35" s="82"/>
+      <c r="BF35" s="82"/>
+      <c r="BG35" s="82"/>
+      <c r="BH35" s="82"/>
+      <c r="BI35" s="82"/>
+      <c r="BJ35" s="82"/>
+      <c r="BK35" s="82"/>
+      <c r="BL35" s="82"/>
+      <c r="BM35" s="82"/>
+      <c r="BN35" s="82"/>
+      <c r="BO35" s="82"/>
+      <c r="BP35" s="82"/>
+      <c r="BQ35" s="82"/>
+      <c r="BR35" s="82"/>
+      <c r="BS35" s="82"/>
+      <c r="BT35" s="82"/>
+      <c r="BU35" s="82"/>
+      <c r="BV35" s="82"/>
+      <c r="BW35" s="83"/>
+      <c r="BX35" s="28"/>
+      <c r="BY35" s="28"/>
+      <c r="BZ35" s="28"/>
+      <c r="CA35" s="28"/>
+      <c r="CB35" s="28"/>
+      <c r="CC35" s="28"/>
+      <c r="CD35" s="28"/>
+      <c r="CE35" s="28"/>
+      <c r="CF35" s="84"/>
     </row>
-    <row r="36" spans="10:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="10:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J36" s="34"/>
       <c r="K36" s="20"/>
       <c r="L36" s="20"/>
@@ -2328,7 +4890,7 @@
       <c r="AM36" s="20"/>
       <c r="AN36" s="20"/>
       <c r="AO36" s="20"/>
-      <c r="AP36" s="20"/>
+      <c r="AP36" s="23"/>
       <c r="AQ36" s="20"/>
       <c r="AR36" s="20"/>
       <c r="AS36" s="20"/>
@@ -2336,13 +4898,47 @@
       <c r="AU36" s="20"/>
       <c r="AV36" s="20"/>
       <c r="AW36" s="20"/>
-      <c r="AX36" s="20"/>
-      <c r="AY36" s="20"/>
-      <c r="AZ36" s="20"/>
-      <c r="BA36" s="20"/>
+      <c r="AX36" s="23"/>
+      <c r="AY36" s="87" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ36" s="88"/>
+      <c r="BA36" s="89"/>
       <c r="BB36" s="20"/>
+      <c r="BC36" s="28"/>
+      <c r="BD36" s="28"/>
+      <c r="BE36" s="28"/>
+      <c r="BF36" s="28"/>
+      <c r="BG36" s="28"/>
+      <c r="BH36" s="28"/>
+      <c r="BI36" s="28"/>
+      <c r="BJ36" s="28"/>
+      <c r="BK36" s="5"/>
+      <c r="BL36" s="28"/>
+      <c r="BM36" s="28"/>
+      <c r="BN36" s="28"/>
+      <c r="BO36" s="28"/>
+      <c r="BP36" s="28"/>
+      <c r="BQ36" s="28"/>
+      <c r="BR36" s="28"/>
+      <c r="BS36" s="28"/>
+      <c r="BT36" s="87" t="s">
+        <v>2</v>
+      </c>
+      <c r="BU36" s="88"/>
+      <c r="BV36" s="89"/>
+      <c r="BW36" s="84"/>
+      <c r="BX36" s="28"/>
+      <c r="BY36" s="28"/>
+      <c r="BZ36" s="28"/>
+      <c r="CA36" s="28"/>
+      <c r="CB36" s="28"/>
+      <c r="CC36" s="28"/>
+      <c r="CD36" s="28"/>
+      <c r="CE36" s="28"/>
+      <c r="CF36" s="84"/>
     </row>
-    <row r="37" spans="10:54" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J37" s="34"/>
       <c r="K37" s="20"/>
       <c r="L37" s="20"/>
@@ -2375,7 +4971,7 @@
       <c r="AM37" s="20"/>
       <c r="AN37" s="20"/>
       <c r="AO37" s="20"/>
-      <c r="AP37" s="20"/>
+      <c r="AP37" s="23"/>
       <c r="AQ37" s="20"/>
       <c r="AR37" s="20"/>
       <c r="AS37" s="20"/>
@@ -2383,13 +4979,43 @@
       <c r="AU37" s="20"/>
       <c r="AV37" s="20"/>
       <c r="AW37" s="20"/>
-      <c r="AX37" s="20"/>
-      <c r="AY37" s="20"/>
-      <c r="AZ37" s="20"/>
-      <c r="BA37" s="20"/>
+      <c r="AX37" s="23"/>
+      <c r="AY37" s="90"/>
+      <c r="AZ37" s="91"/>
+      <c r="BA37" s="92"/>
       <c r="BB37" s="20"/>
+      <c r="BC37" s="28"/>
+      <c r="BD37" s="28"/>
+      <c r="BE37" s="28"/>
+      <c r="BF37" s="28"/>
+      <c r="BG37" s="28"/>
+      <c r="BH37" s="28"/>
+      <c r="BI37" s="28"/>
+      <c r="BJ37" s="28"/>
+      <c r="BK37" s="28"/>
+      <c r="BL37" s="28"/>
+      <c r="BM37" s="28"/>
+      <c r="BN37" s="28"/>
+      <c r="BO37" s="28"/>
+      <c r="BP37" s="28"/>
+      <c r="BQ37" s="28"/>
+      <c r="BR37" s="28"/>
+      <c r="BS37" s="28"/>
+      <c r="BT37" s="90"/>
+      <c r="BU37" s="91"/>
+      <c r="BV37" s="92"/>
+      <c r="BW37" s="84"/>
+      <c r="BX37" s="28"/>
+      <c r="BY37" s="28"/>
+      <c r="BZ37" s="28"/>
+      <c r="CA37" s="28"/>
+      <c r="CB37" s="28"/>
+      <c r="CC37" s="28"/>
+      <c r="CD37" s="28"/>
+      <c r="CE37" s="28"/>
+      <c r="CF37" s="84"/>
     </row>
-    <row r="38" spans="10:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J38" s="34"/>
       <c r="K38" s="20"/>
       <c r="L38" s="20"/>
@@ -2422,7 +5048,7 @@
       <c r="AM38" s="20"/>
       <c r="AN38" s="20"/>
       <c r="AO38" s="20"/>
-      <c r="AP38" s="20"/>
+      <c r="AP38" s="23"/>
       <c r="AQ38" s="20"/>
       <c r="AR38" s="20"/>
       <c r="AS38" s="20"/>
@@ -2430,13 +5056,43 @@
       <c r="AU38" s="20"/>
       <c r="AV38" s="20"/>
       <c r="AW38" s="20"/>
-      <c r="AX38" s="20"/>
-      <c r="AY38" s="20"/>
-      <c r="AZ38" s="20"/>
-      <c r="BA38" s="20"/>
-      <c r="BB38" s="20"/>
+      <c r="AX38" s="25"/>
+      <c r="AY38" s="85"/>
+      <c r="AZ38" s="85"/>
+      <c r="BA38" s="85"/>
+      <c r="BB38" s="26"/>
+      <c r="BC38" s="85"/>
+      <c r="BD38" s="98"/>
+      <c r="BE38" s="98"/>
+      <c r="BF38" s="98"/>
+      <c r="BG38" s="85"/>
+      <c r="BH38" s="85"/>
+      <c r="BI38" s="85"/>
+      <c r="BJ38" s="85"/>
+      <c r="BK38" s="85"/>
+      <c r="BL38" s="85"/>
+      <c r="BM38" s="85"/>
+      <c r="BN38" s="85"/>
+      <c r="BO38" s="85"/>
+      <c r="BP38" s="85"/>
+      <c r="BQ38" s="85"/>
+      <c r="BR38" s="85"/>
+      <c r="BS38" s="85"/>
+      <c r="BT38" s="85"/>
+      <c r="BU38" s="85"/>
+      <c r="BV38" s="85"/>
+      <c r="BW38" s="86"/>
+      <c r="BX38" s="28"/>
+      <c r="BY38" s="28"/>
+      <c r="BZ38" s="28"/>
+      <c r="CA38" s="28"/>
+      <c r="CB38" s="28"/>
+      <c r="CC38" s="28"/>
+      <c r="CD38" s="28"/>
+      <c r="CE38" s="28"/>
+      <c r="CF38" s="84"/>
     </row>
-    <row r="39" spans="10:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J39" s="34"/>
       <c r="K39" s="28"/>
       <c r="L39" s="28"/>
@@ -2466,8 +5122,51 @@
       <c r="AJ39" s="28"/>
       <c r="AK39" s="28"/>
       <c r="AL39" s="36"/>
+      <c r="AP39" s="30"/>
+      <c r="AQ39" s="28"/>
+      <c r="AR39" s="28"/>
+      <c r="AS39" s="28"/>
+      <c r="AT39" s="28"/>
+      <c r="AU39" s="28"/>
+      <c r="AV39" s="28"/>
+      <c r="AW39" s="28"/>
+      <c r="AX39" s="28"/>
+      <c r="AY39" s="28"/>
+      <c r="AZ39" s="28"/>
+      <c r="BA39" s="28"/>
+      <c r="BB39" s="28"/>
+      <c r="BC39" s="28"/>
+      <c r="BD39" s="99"/>
+      <c r="BE39" s="99"/>
+      <c r="BF39" s="99"/>
+      <c r="BG39" s="28"/>
+      <c r="BH39" s="28"/>
+      <c r="BI39" s="28"/>
+      <c r="BJ39" s="28"/>
+      <c r="BK39" s="28"/>
+      <c r="BL39" s="28"/>
+      <c r="BM39" s="28"/>
+      <c r="BN39" s="28"/>
+      <c r="BO39" s="28"/>
+      <c r="BP39" s="28"/>
+      <c r="BQ39" s="28"/>
+      <c r="BR39" s="28"/>
+      <c r="BS39" s="28"/>
+      <c r="BT39" s="28"/>
+      <c r="BU39" s="28"/>
+      <c r="BV39" s="28"/>
+      <c r="BW39" s="28"/>
+      <c r="BX39" s="28"/>
+      <c r="BY39" s="28"/>
+      <c r="BZ39" s="28"/>
+      <c r="CA39" s="28"/>
+      <c r="CB39" s="28"/>
+      <c r="CC39" s="28"/>
+      <c r="CD39" s="28"/>
+      <c r="CE39" s="28"/>
+      <c r="CF39" s="84"/>
     </row>
-    <row r="40" spans="10:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="10:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J40" s="34"/>
       <c r="K40" s="28"/>
       <c r="L40" s="28"/>
@@ -2497,8 +5196,53 @@
       <c r="AJ40" s="28"/>
       <c r="AK40" s="28"/>
       <c r="AL40" s="36"/>
+      <c r="AP40" s="30"/>
+      <c r="AQ40" s="28"/>
+      <c r="AR40" s="28"/>
+      <c r="AS40" s="28"/>
+      <c r="AT40" s="28"/>
+      <c r="AU40" s="28"/>
+      <c r="AV40" s="28"/>
+      <c r="AW40" s="28"/>
+      <c r="AX40" s="28"/>
+      <c r="AY40" s="28"/>
+      <c r="AZ40" s="28"/>
+      <c r="BA40" s="28"/>
+      <c r="BB40" s="28"/>
+      <c r="BC40" s="28"/>
+      <c r="BD40" s="28"/>
+      <c r="BE40" s="28"/>
+      <c r="BF40" s="28"/>
+      <c r="BG40" s="28"/>
+      <c r="BH40" s="28"/>
+      <c r="BI40" s="28"/>
+      <c r="BJ40" s="87" t="s">
+        <v>2</v>
+      </c>
+      <c r="BK40" s="88"/>
+      <c r="BL40" s="89"/>
+      <c r="BM40" s="28"/>
+      <c r="BN40" s="28"/>
+      <c r="BO40" s="28"/>
+      <c r="BP40" s="28"/>
+      <c r="BQ40" s="28"/>
+      <c r="BR40" s="28"/>
+      <c r="BS40" s="28"/>
+      <c r="BT40" s="28"/>
+      <c r="BU40" s="28"/>
+      <c r="BV40" s="28"/>
+      <c r="BW40" s="28"/>
+      <c r="BX40" s="28"/>
+      <c r="BY40" s="28"/>
+      <c r="BZ40" s="28"/>
+      <c r="CA40" s="28"/>
+      <c r="CB40" s="28"/>
+      <c r="CC40" s="28"/>
+      <c r="CD40" s="28"/>
+      <c r="CE40" s="28"/>
+      <c r="CF40" s="84"/>
     </row>
-    <row r="41" spans="10:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J41" s="34"/>
       <c r="K41" s="28"/>
       <c r="L41" s="28"/>
@@ -2528,8 +5272,51 @@
       <c r="AJ41" s="28"/>
       <c r="AK41" s="28"/>
       <c r="AL41" s="36"/>
+      <c r="AP41" s="30"/>
+      <c r="AQ41" s="28"/>
+      <c r="AR41" s="28"/>
+      <c r="AS41" s="28"/>
+      <c r="AT41" s="28"/>
+      <c r="AU41" s="28"/>
+      <c r="AV41" s="28"/>
+      <c r="AW41" s="28"/>
+      <c r="AX41" s="28"/>
+      <c r="AY41" s="28"/>
+      <c r="AZ41" s="28"/>
+      <c r="BA41" s="28"/>
+      <c r="BB41" s="28"/>
+      <c r="BC41" s="28"/>
+      <c r="BD41" s="28"/>
+      <c r="BE41" s="28"/>
+      <c r="BF41" s="28"/>
+      <c r="BG41" s="28"/>
+      <c r="BH41" s="28"/>
+      <c r="BI41" s="28"/>
+      <c r="BJ41" s="90"/>
+      <c r="BK41" s="91"/>
+      <c r="BL41" s="92"/>
+      <c r="BM41" s="28"/>
+      <c r="BN41" s="28"/>
+      <c r="BO41" s="28"/>
+      <c r="BP41" s="28"/>
+      <c r="BQ41" s="28"/>
+      <c r="BR41" s="28"/>
+      <c r="BS41" s="28"/>
+      <c r="BT41" s="28"/>
+      <c r="BU41" s="28"/>
+      <c r="BV41" s="28"/>
+      <c r="BW41" s="28"/>
+      <c r="BX41" s="28"/>
+      <c r="BY41" s="28"/>
+      <c r="BZ41" s="28"/>
+      <c r="CA41" s="28"/>
+      <c r="CB41" s="28"/>
+      <c r="CC41" s="28"/>
+      <c r="CD41" s="28"/>
+      <c r="CE41" s="28"/>
+      <c r="CF41" s="84"/>
     </row>
-    <row r="42" spans="10:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="10:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J42" s="34"/>
       <c r="K42" s="28"/>
       <c r="L42" s="28"/>
@@ -2559,8 +5346,51 @@
       <c r="AJ42" s="28"/>
       <c r="AK42" s="28"/>
       <c r="AL42" s="36"/>
+      <c r="AP42" s="30"/>
+      <c r="AQ42" s="28"/>
+      <c r="AR42" s="28"/>
+      <c r="AS42" s="28"/>
+      <c r="AT42" s="28"/>
+      <c r="AU42" s="28"/>
+      <c r="AV42" s="28"/>
+      <c r="AW42" s="28"/>
+      <c r="AX42" s="28"/>
+      <c r="AY42" s="28"/>
+      <c r="AZ42" s="28"/>
+      <c r="BA42" s="28"/>
+      <c r="BB42" s="28"/>
+      <c r="BC42" s="28"/>
+      <c r="BD42" s="28"/>
+      <c r="BE42" s="28"/>
+      <c r="BF42" s="28"/>
+      <c r="BG42" s="28"/>
+      <c r="BH42" s="28"/>
+      <c r="BI42" s="28"/>
+      <c r="BJ42" s="28"/>
+      <c r="BK42" s="28"/>
+      <c r="BL42" s="28"/>
+      <c r="BM42" s="28"/>
+      <c r="BN42" s="28"/>
+      <c r="BO42" s="28"/>
+      <c r="BP42" s="28"/>
+      <c r="BQ42" s="28"/>
+      <c r="BR42" s="28"/>
+      <c r="BS42" s="28"/>
+      <c r="BT42" s="28"/>
+      <c r="BU42" s="28"/>
+      <c r="BV42" s="28"/>
+      <c r="BW42" s="28"/>
+      <c r="BX42" s="28"/>
+      <c r="BY42" s="28"/>
+      <c r="BZ42" s="28"/>
+      <c r="CA42" s="28"/>
+      <c r="CB42" s="28"/>
+      <c r="CC42" s="28"/>
+      <c r="CD42" s="28"/>
+      <c r="CE42" s="28"/>
+      <c r="CF42" s="84"/>
     </row>
-    <row r="43" spans="10:54" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="10:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J43" s="34"/>
       <c r="K43" s="28"/>
       <c r="L43" s="28"/>
@@ -2590,8 +5420,51 @@
       <c r="AJ43" s="28"/>
       <c r="AK43" s="28"/>
       <c r="AL43" s="36"/>
+      <c r="AP43" s="30"/>
+      <c r="AQ43" s="28"/>
+      <c r="AR43" s="28"/>
+      <c r="AS43" s="20"/>
+      <c r="AT43" s="28"/>
+      <c r="AU43" s="76"/>
+      <c r="AV43" s="76"/>
+      <c r="AW43" s="93"/>
+      <c r="AX43" s="76"/>
+      <c r="AY43" s="76"/>
+      <c r="AZ43" s="28"/>
+      <c r="BA43" s="28"/>
+      <c r="BB43" s="28"/>
+      <c r="BC43" s="28"/>
+      <c r="BD43" s="28"/>
+      <c r="BE43" s="76"/>
+      <c r="BF43" s="76"/>
+      <c r="BG43" s="76"/>
+      <c r="BH43" s="76"/>
+      <c r="BI43" s="76"/>
+      <c r="BJ43" s="28"/>
+      <c r="BK43" s="28"/>
+      <c r="BL43" s="28"/>
+      <c r="BM43" s="20"/>
+      <c r="BN43" s="28"/>
+      <c r="BO43" s="76"/>
+      <c r="BP43" s="76"/>
+      <c r="BQ43" s="77"/>
+      <c r="BR43" s="76"/>
+      <c r="BS43" s="93"/>
+      <c r="BT43" s="28"/>
+      <c r="BU43" s="28"/>
+      <c r="BV43" s="28"/>
+      <c r="BW43" s="28"/>
+      <c r="BX43" s="28"/>
+      <c r="BY43" s="93"/>
+      <c r="BZ43" s="76"/>
+      <c r="CA43" s="76"/>
+      <c r="CB43" s="76"/>
+      <c r="CC43" s="76"/>
+      <c r="CD43" s="28"/>
+      <c r="CE43" s="28"/>
+      <c r="CF43" s="84"/>
     </row>
-    <row r="44" spans="10:54" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J44" s="37"/>
       <c r="K44" s="38"/>
       <c r="L44" s="38"/>
@@ -2621,10 +5494,902 @@
       <c r="AJ44" s="38"/>
       <c r="AK44" s="38"/>
       <c r="AL44" s="39"/>
+      <c r="AP44" s="30"/>
+      <c r="AQ44" s="28"/>
+      <c r="AR44" s="28"/>
+      <c r="AS44" s="20"/>
+      <c r="AT44" s="28"/>
+      <c r="AU44" s="76"/>
+      <c r="AV44" s="76"/>
+      <c r="AW44" s="76"/>
+      <c r="AX44" s="76"/>
+      <c r="AY44" s="76"/>
+      <c r="AZ44" s="28"/>
+      <c r="BA44" s="28"/>
+      <c r="BB44" s="28"/>
+      <c r="BC44" s="28"/>
+      <c r="BD44" s="28"/>
+      <c r="BE44" s="76"/>
+      <c r="BF44" s="77"/>
+      <c r="BG44" s="76"/>
+      <c r="BH44" s="77"/>
+      <c r="BI44" s="76"/>
+      <c r="BJ44" s="28"/>
+      <c r="BK44" s="28"/>
+      <c r="BL44" s="28"/>
+      <c r="BM44" s="20"/>
+      <c r="BN44" s="28"/>
+      <c r="BO44" s="76"/>
+      <c r="BP44" s="76"/>
+      <c r="BQ44" s="76"/>
+      <c r="BR44" s="76"/>
+      <c r="BS44" s="76"/>
+      <c r="BT44" s="28"/>
+      <c r="BU44" s="28"/>
+      <c r="BV44" s="28"/>
+      <c r="BW44" s="28"/>
+      <c r="BX44" s="28"/>
+      <c r="BY44" s="76"/>
+      <c r="BZ44" s="77"/>
+      <c r="CA44" s="76"/>
+      <c r="CB44" s="77"/>
+      <c r="CC44" s="76"/>
+      <c r="CD44" s="28"/>
+      <c r="CE44" s="28"/>
+      <c r="CF44" s="84"/>
+    </row>
+    <row r="45" spans="10:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AP45" s="30"/>
+      <c r="AQ45" s="28"/>
+      <c r="AR45" s="28"/>
+      <c r="AS45" s="20"/>
+      <c r="AT45" s="28"/>
+      <c r="AU45" s="77"/>
+      <c r="AV45" s="76"/>
+      <c r="AW45" s="93"/>
+      <c r="AX45" s="76"/>
+      <c r="AY45" s="77"/>
+      <c r="AZ45" s="28"/>
+      <c r="BA45" s="28"/>
+      <c r="BB45" s="94"/>
+      <c r="BC45" s="28"/>
+      <c r="BD45" s="28"/>
+      <c r="BE45" s="93"/>
+      <c r="BF45" s="76"/>
+      <c r="BG45" s="93"/>
+      <c r="BH45" s="76"/>
+      <c r="BI45" s="93"/>
+      <c r="BJ45" s="28"/>
+      <c r="BK45" s="28"/>
+      <c r="BL45" s="94"/>
+      <c r="BM45" s="20"/>
+      <c r="BN45" s="28"/>
+      <c r="BO45" s="77"/>
+      <c r="BP45" s="76"/>
+      <c r="BQ45" s="93"/>
+      <c r="BR45" s="76"/>
+      <c r="BS45" s="77"/>
+      <c r="BT45" s="28"/>
+      <c r="BU45" s="28"/>
+      <c r="BV45" s="94"/>
+      <c r="BW45" s="28"/>
+      <c r="BX45" s="28"/>
+      <c r="BY45" s="77"/>
+      <c r="BZ45" s="76"/>
+      <c r="CA45" s="93"/>
+      <c r="CB45" s="76"/>
+      <c r="CC45" s="77"/>
+      <c r="CD45" s="28"/>
+      <c r="CE45" s="28"/>
+      <c r="CF45" s="84"/>
+    </row>
+    <row r="46" spans="10:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AP46" s="30"/>
+      <c r="AQ46" s="28"/>
+      <c r="AR46" s="28"/>
+      <c r="AS46" s="20"/>
+      <c r="AT46" s="28"/>
+      <c r="AU46" s="76"/>
+      <c r="AV46" s="76"/>
+      <c r="AW46" s="76"/>
+      <c r="AX46" s="76"/>
+      <c r="AY46" s="76"/>
+      <c r="AZ46" s="28"/>
+      <c r="BA46" s="28"/>
+      <c r="BB46" s="28"/>
+      <c r="BC46" s="28"/>
+      <c r="BD46" s="28"/>
+      <c r="BE46" s="76"/>
+      <c r="BF46" s="77"/>
+      <c r="BG46" s="76"/>
+      <c r="BH46" s="77"/>
+      <c r="BI46" s="77"/>
+      <c r="BJ46" s="28"/>
+      <c r="BK46" s="28"/>
+      <c r="BL46" s="28"/>
+      <c r="BM46" s="20"/>
+      <c r="BN46" s="28"/>
+      <c r="BO46" s="76"/>
+      <c r="BP46" s="76"/>
+      <c r="BQ46" s="76"/>
+      <c r="BR46" s="76"/>
+      <c r="BS46" s="76"/>
+      <c r="BT46" s="28"/>
+      <c r="BU46" s="28"/>
+      <c r="BV46" s="28"/>
+      <c r="BW46" s="28"/>
+      <c r="BX46" s="28"/>
+      <c r="BY46" s="76"/>
+      <c r="BZ46" s="77"/>
+      <c r="CA46" s="76"/>
+      <c r="CB46" s="77"/>
+      <c r="CC46" s="77"/>
+      <c r="CD46" s="28"/>
+      <c r="CE46" s="28"/>
+      <c r="CF46" s="84"/>
+    </row>
+    <row r="47" spans="10:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AP47" s="30"/>
+      <c r="AQ47" s="28"/>
+      <c r="AR47" s="28"/>
+      <c r="AS47" s="20"/>
+      <c r="AT47" s="28"/>
+      <c r="AU47" s="76"/>
+      <c r="AV47" s="76"/>
+      <c r="AW47" s="93"/>
+      <c r="AX47" s="76"/>
+      <c r="AY47" s="76"/>
+      <c r="AZ47" s="28"/>
+      <c r="BA47" s="28"/>
+      <c r="BB47" s="28"/>
+      <c r="BC47" s="28"/>
+      <c r="BD47" s="28"/>
+      <c r="BE47" s="76"/>
+      <c r="BF47" s="76"/>
+      <c r="BG47" s="76"/>
+      <c r="BH47" s="76"/>
+      <c r="BI47" s="76"/>
+      <c r="BJ47" s="28"/>
+      <c r="BK47" s="28"/>
+      <c r="BL47" s="28"/>
+      <c r="BM47" s="20"/>
+      <c r="BN47" s="28"/>
+      <c r="BO47" s="93"/>
+      <c r="BP47" s="76"/>
+      <c r="BQ47" s="77"/>
+      <c r="BR47" s="76"/>
+      <c r="BS47" s="76"/>
+      <c r="BT47" s="28"/>
+      <c r="BU47" s="28"/>
+      <c r="BV47" s="28"/>
+      <c r="BW47" s="28"/>
+      <c r="BX47" s="28"/>
+      <c r="BY47" s="76"/>
+      <c r="BZ47" s="76"/>
+      <c r="CA47" s="76"/>
+      <c r="CB47" s="76"/>
+      <c r="CC47" s="93"/>
+      <c r="CD47" s="28"/>
+      <c r="CE47" s="28"/>
+      <c r="CF47" s="84"/>
+    </row>
+    <row r="48" spans="10:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AP48" s="30"/>
+      <c r="AQ48" s="28"/>
+      <c r="AR48" s="28"/>
+      <c r="AS48" s="20"/>
+      <c r="AT48" s="28"/>
+      <c r="AU48" s="28"/>
+      <c r="AV48" s="28"/>
+      <c r="AW48" s="28"/>
+      <c r="AX48" s="28"/>
+      <c r="AY48" s="28"/>
+      <c r="AZ48" s="28"/>
+      <c r="BA48" s="28"/>
+      <c r="BB48" s="28"/>
+      <c r="BC48" s="28"/>
+      <c r="BD48" s="28"/>
+      <c r="BE48" s="28"/>
+      <c r="BF48" s="28"/>
+      <c r="BG48" s="28"/>
+      <c r="BH48" s="28"/>
+      <c r="BI48" s="28"/>
+      <c r="BJ48" s="28"/>
+      <c r="BK48" s="28"/>
+      <c r="BL48" s="28"/>
+      <c r="BM48" s="20"/>
+      <c r="BN48" s="28"/>
+      <c r="BO48" s="28"/>
+      <c r="BP48" s="28"/>
+      <c r="BQ48" s="28"/>
+      <c r="BR48" s="28"/>
+      <c r="BS48" s="28"/>
+      <c r="BT48" s="28"/>
+      <c r="BU48" s="28"/>
+      <c r="BV48" s="28"/>
+      <c r="BW48" s="28"/>
+      <c r="BX48" s="28"/>
+      <c r="BY48" s="28"/>
+      <c r="BZ48" s="28"/>
+      <c r="CA48" s="28"/>
+      <c r="CB48" s="28"/>
+      <c r="CC48" s="28"/>
+      <c r="CD48" s="28"/>
+      <c r="CE48" s="28"/>
+      <c r="CF48" s="84"/>
+    </row>
+    <row r="49" spans="42:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AP49" s="30"/>
+      <c r="AQ49" s="28"/>
+      <c r="AR49" s="28"/>
+      <c r="AS49" s="20"/>
+      <c r="AT49" s="28"/>
+      <c r="AU49" s="28"/>
+      <c r="AV49" s="28"/>
+      <c r="AW49" s="28"/>
+      <c r="AX49" s="28"/>
+      <c r="AY49" s="28"/>
+      <c r="AZ49" s="28"/>
+      <c r="BA49" s="28"/>
+      <c r="BB49" s="28"/>
+      <c r="BC49" s="28"/>
+      <c r="BD49" s="28"/>
+      <c r="BE49" s="28"/>
+      <c r="BF49" s="28"/>
+      <c r="BG49" s="28"/>
+      <c r="BH49" s="28"/>
+      <c r="BI49" s="28"/>
+      <c r="BJ49" s="28"/>
+      <c r="BK49" s="28"/>
+      <c r="BL49" s="28"/>
+      <c r="BM49" s="20"/>
+      <c r="BN49" s="28"/>
+      <c r="BO49" s="28"/>
+      <c r="BP49" s="28"/>
+      <c r="BQ49" s="28"/>
+      <c r="BR49" s="28"/>
+      <c r="BS49" s="28"/>
+      <c r="BT49" s="28"/>
+      <c r="BU49" s="28"/>
+      <c r="BV49" s="28"/>
+      <c r="BW49" s="28"/>
+      <c r="BX49" s="28"/>
+      <c r="BY49" s="28"/>
+      <c r="BZ49" s="28"/>
+      <c r="CA49" s="28"/>
+      <c r="CB49" s="28"/>
+      <c r="CC49" s="28"/>
+      <c r="CD49" s="28"/>
+      <c r="CE49" s="28"/>
+      <c r="CF49" s="84"/>
+    </row>
+    <row r="50" spans="42:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AP50" s="30"/>
+      <c r="AQ50" s="28"/>
+      <c r="AR50" s="28"/>
+      <c r="AS50" s="20"/>
+      <c r="AT50" s="81"/>
+      <c r="AU50" s="21"/>
+      <c r="AV50" s="21"/>
+      <c r="AW50" s="21"/>
+      <c r="AX50" s="21"/>
+      <c r="AY50" s="21"/>
+      <c r="AZ50" s="21"/>
+      <c r="BA50" s="21"/>
+      <c r="BB50" s="21"/>
+      <c r="BC50" s="21"/>
+      <c r="BD50" s="21"/>
+      <c r="BE50" s="82"/>
+      <c r="BF50" s="82"/>
+      <c r="BG50" s="82"/>
+      <c r="BH50" s="82"/>
+      <c r="BI50" s="82"/>
+      <c r="BJ50" s="83"/>
+      <c r="BK50" s="28"/>
+      <c r="BL50" s="28"/>
+      <c r="BM50" s="20"/>
+      <c r="BN50" s="81"/>
+      <c r="BO50" s="21"/>
+      <c r="BP50" s="21"/>
+      <c r="BQ50" s="21"/>
+      <c r="BR50" s="21"/>
+      <c r="BS50" s="21"/>
+      <c r="BT50" s="21"/>
+      <c r="BU50" s="21"/>
+      <c r="BV50" s="21"/>
+      <c r="BW50" s="21"/>
+      <c r="BX50" s="21"/>
+      <c r="BY50" s="82"/>
+      <c r="BZ50" s="82"/>
+      <c r="CA50" s="82"/>
+      <c r="CB50" s="82"/>
+      <c r="CC50" s="82"/>
+      <c r="CD50" s="83"/>
+      <c r="CE50" s="28"/>
+      <c r="CF50" s="84"/>
+    </row>
+    <row r="51" spans="42:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AP51" s="30"/>
+      <c r="AQ51" s="28"/>
+      <c r="AR51" s="28"/>
+      <c r="AS51" s="20"/>
+      <c r="AT51" s="23"/>
+      <c r="AU51" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV51" s="79"/>
+      <c r="AW51" s="79"/>
+      <c r="AX51" s="79"/>
+      <c r="AY51" s="80"/>
+      <c r="AZ51" s="20"/>
+      <c r="BA51" s="20"/>
+      <c r="BB51" s="94"/>
+      <c r="BC51" s="20"/>
+      <c r="BD51" s="28"/>
+      <c r="BE51" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF51" s="79"/>
+      <c r="BG51" s="79"/>
+      <c r="BH51" s="79"/>
+      <c r="BI51" s="80"/>
+      <c r="BJ51" s="84"/>
+      <c r="BK51" s="28"/>
+      <c r="BL51" s="28"/>
+      <c r="BM51" s="20"/>
+      <c r="BN51" s="23"/>
+      <c r="BO51" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="BP51" s="79"/>
+      <c r="BQ51" s="79"/>
+      <c r="BR51" s="79"/>
+      <c r="BS51" s="80"/>
+      <c r="BT51" s="20"/>
+      <c r="BU51" s="20"/>
+      <c r="BV51" s="94"/>
+      <c r="BW51" s="20"/>
+      <c r="BX51" s="28"/>
+      <c r="BY51" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="BZ51" s="79"/>
+      <c r="CA51" s="79"/>
+      <c r="CB51" s="79"/>
+      <c r="CC51" s="80"/>
+      <c r="CD51" s="84"/>
+      <c r="CE51" s="28"/>
+      <c r="CF51" s="84"/>
+    </row>
+    <row r="52" spans="42:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AP52" s="30"/>
+      <c r="AQ52" s="28"/>
+      <c r="AR52" s="28"/>
+      <c r="AS52" s="20"/>
+      <c r="AT52" s="25"/>
+      <c r="AU52" s="26"/>
+      <c r="AV52" s="26"/>
+      <c r="AW52" s="26"/>
+      <c r="AX52" s="26"/>
+      <c r="AY52" s="26"/>
+      <c r="AZ52" s="26"/>
+      <c r="BA52" s="26"/>
+      <c r="BB52" s="26"/>
+      <c r="BC52" s="26"/>
+      <c r="BD52" s="26"/>
+      <c r="BE52" s="85"/>
+      <c r="BF52" s="85"/>
+      <c r="BG52" s="85"/>
+      <c r="BH52" s="85"/>
+      <c r="BI52" s="85"/>
+      <c r="BJ52" s="86"/>
+      <c r="BK52" s="28"/>
+      <c r="BL52" s="28"/>
+      <c r="BM52" s="20"/>
+      <c r="BN52" s="25"/>
+      <c r="BO52" s="26"/>
+      <c r="BP52" s="26"/>
+      <c r="BQ52" s="26"/>
+      <c r="BR52" s="26"/>
+      <c r="BS52" s="26"/>
+      <c r="BT52" s="26"/>
+      <c r="BU52" s="26"/>
+      <c r="BV52" s="26"/>
+      <c r="BW52" s="26"/>
+      <c r="BX52" s="26"/>
+      <c r="BY52" s="85"/>
+      <c r="BZ52" s="85"/>
+      <c r="CA52" s="85"/>
+      <c r="CB52" s="85"/>
+      <c r="CC52" s="85"/>
+      <c r="CD52" s="86"/>
+      <c r="CE52" s="28"/>
+      <c r="CF52" s="84"/>
+    </row>
+    <row r="53" spans="42:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AP53" s="30"/>
+      <c r="AQ53" s="28"/>
+      <c r="AR53" s="28"/>
+      <c r="AS53" s="20"/>
+      <c r="AT53" s="20"/>
+      <c r="AU53" s="20"/>
+      <c r="AV53" s="20"/>
+      <c r="AW53" s="20"/>
+      <c r="AX53" s="20"/>
+      <c r="AY53" s="20"/>
+      <c r="AZ53" s="20"/>
+      <c r="BA53" s="20"/>
+      <c r="BB53" s="20"/>
+      <c r="BC53" s="20"/>
+      <c r="BD53" s="20"/>
+      <c r="BE53" s="28"/>
+      <c r="BF53" s="28"/>
+      <c r="BG53" s="28"/>
+      <c r="BH53" s="28"/>
+      <c r="BI53" s="28"/>
+      <c r="BJ53" s="28"/>
+      <c r="BK53" s="28"/>
+      <c r="BL53" s="28"/>
+      <c r="BM53" s="20"/>
+      <c r="BN53" s="20"/>
+      <c r="BO53" s="20"/>
+      <c r="BP53" s="20"/>
+      <c r="BQ53" s="20"/>
+      <c r="BR53" s="20"/>
+      <c r="BS53" s="20"/>
+      <c r="BT53" s="20"/>
+      <c r="BU53" s="20"/>
+      <c r="BV53" s="20"/>
+      <c r="BW53" s="20"/>
+      <c r="BX53" s="20"/>
+      <c r="BY53" s="28"/>
+      <c r="BZ53" s="28"/>
+      <c r="CA53" s="28"/>
+      <c r="CB53" s="28"/>
+      <c r="CC53" s="28"/>
+      <c r="CD53" s="28"/>
+      <c r="CE53" s="28"/>
+      <c r="CF53" s="84"/>
+    </row>
+    <row r="54" spans="42:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AP54" s="30"/>
+      <c r="AQ54" s="28"/>
+      <c r="AR54" s="28"/>
+      <c r="AS54" s="28"/>
+      <c r="AT54" s="28"/>
+      <c r="AU54" s="28"/>
+      <c r="AV54" s="28"/>
+      <c r="AW54" s="28"/>
+      <c r="AX54" s="28"/>
+      <c r="AY54" s="28"/>
+      <c r="AZ54" s="29"/>
+      <c r="BA54" s="82"/>
+      <c r="BB54" s="82"/>
+      <c r="BC54" s="82"/>
+      <c r="BD54" s="82"/>
+      <c r="BE54" s="82"/>
+      <c r="BF54" s="82"/>
+      <c r="BG54" s="82"/>
+      <c r="BH54" s="82"/>
+      <c r="BI54" s="82"/>
+      <c r="BJ54" s="82"/>
+      <c r="BK54" s="82"/>
+      <c r="BL54" s="82"/>
+      <c r="BM54" s="82"/>
+      <c r="BN54" s="82"/>
+      <c r="BO54" s="82"/>
+      <c r="BP54" s="82"/>
+      <c r="BQ54" s="82"/>
+      <c r="BR54" s="82"/>
+      <c r="BS54" s="82"/>
+      <c r="BT54" s="82"/>
+      <c r="BU54" s="82"/>
+      <c r="BV54" s="82"/>
+      <c r="BW54" s="82"/>
+      <c r="BX54" s="83"/>
+      <c r="BY54" s="28"/>
+      <c r="BZ54" s="28"/>
+      <c r="CA54" s="28"/>
+      <c r="CB54" s="28"/>
+      <c r="CC54" s="28"/>
+      <c r="CD54" s="28"/>
+      <c r="CE54" s="28"/>
+      <c r="CF54" s="84"/>
+    </row>
+    <row r="55" spans="42:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AP55" s="30"/>
+      <c r="AQ55" s="28"/>
+      <c r="AR55" s="28"/>
+      <c r="AS55" s="28"/>
+      <c r="AT55" s="28"/>
+      <c r="AU55" s="28"/>
+      <c r="AV55" s="28"/>
+      <c r="AW55" s="28"/>
+      <c r="AX55" s="28"/>
+      <c r="AY55" s="28"/>
+      <c r="AZ55" s="30"/>
+      <c r="BA55" s="87" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB55" s="88"/>
+      <c r="BC55" s="89"/>
+      <c r="BD55" s="28"/>
+      <c r="BE55" s="28"/>
+      <c r="BF55" s="28"/>
+      <c r="BG55" s="28"/>
+      <c r="BH55" s="28"/>
+      <c r="BI55" s="28"/>
+      <c r="BJ55" s="28"/>
+      <c r="BK55" s="28"/>
+      <c r="BL55" s="94"/>
+      <c r="BM55" s="28"/>
+      <c r="BN55" s="28"/>
+      <c r="BO55" s="28"/>
+      <c r="BP55" s="28"/>
+      <c r="BQ55" s="28"/>
+      <c r="BR55" s="28"/>
+      <c r="BS55" s="28"/>
+      <c r="BT55" s="28"/>
+      <c r="BU55" s="87" t="s">
+        <v>2</v>
+      </c>
+      <c r="BV55" s="88"/>
+      <c r="BW55" s="89"/>
+      <c r="BX55" s="84"/>
+      <c r="BY55" s="28"/>
+      <c r="BZ55" s="28"/>
+      <c r="CA55" s="28"/>
+      <c r="CB55" s="28"/>
+      <c r="CC55" s="28"/>
+      <c r="CD55" s="28"/>
+      <c r="CE55" s="28"/>
+      <c r="CF55" s="84"/>
+    </row>
+    <row r="56" spans="42:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AP56" s="30"/>
+      <c r="AQ56" s="28"/>
+      <c r="AR56" s="28"/>
+      <c r="AS56" s="28"/>
+      <c r="AT56" s="28"/>
+      <c r="AU56" s="28"/>
+      <c r="AV56" s="28"/>
+      <c r="AW56" s="28"/>
+      <c r="AX56" s="28"/>
+      <c r="AY56" s="28"/>
+      <c r="AZ56" s="30"/>
+      <c r="BA56" s="90"/>
+      <c r="BB56" s="91"/>
+      <c r="BC56" s="92"/>
+      <c r="BD56" s="28"/>
+      <c r="BE56" s="28"/>
+      <c r="BF56" s="28"/>
+      <c r="BG56" s="28"/>
+      <c r="BH56" s="28"/>
+      <c r="BI56" s="28"/>
+      <c r="BJ56" s="28"/>
+      <c r="BK56" s="28"/>
+      <c r="BL56" s="28"/>
+      <c r="BM56" s="28"/>
+      <c r="BN56" s="28"/>
+      <c r="BO56" s="28"/>
+      <c r="BP56" s="28"/>
+      <c r="BQ56" s="28"/>
+      <c r="BR56" s="28"/>
+      <c r="BS56" s="28"/>
+      <c r="BT56" s="28"/>
+      <c r="BU56" s="90"/>
+      <c r="BV56" s="91"/>
+      <c r="BW56" s="92"/>
+      <c r="BX56" s="84"/>
+      <c r="BY56" s="28"/>
+      <c r="BZ56" s="28"/>
+      <c r="CA56" s="28"/>
+      <c r="CB56" s="28"/>
+      <c r="CC56" s="28"/>
+      <c r="CD56" s="28"/>
+      <c r="CE56" s="28"/>
+      <c r="CF56" s="84"/>
+    </row>
+    <row r="57" spans="42:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AP57" s="30"/>
+      <c r="AQ57" s="28"/>
+      <c r="AR57" s="28"/>
+      <c r="AS57" s="28"/>
+      <c r="AT57" s="28"/>
+      <c r="AU57" s="28"/>
+      <c r="AV57" s="28"/>
+      <c r="AW57" s="28"/>
+      <c r="AX57" s="28"/>
+      <c r="AY57" s="28"/>
+      <c r="AZ57" s="31"/>
+      <c r="BA57" s="85"/>
+      <c r="BB57" s="85"/>
+      <c r="BC57" s="85"/>
+      <c r="BD57" s="85"/>
+      <c r="BE57" s="85"/>
+      <c r="BF57" s="85"/>
+      <c r="BG57" s="85"/>
+      <c r="BH57" s="85"/>
+      <c r="BI57" s="85"/>
+      <c r="BJ57" s="85"/>
+      <c r="BK57" s="85"/>
+      <c r="BL57" s="85"/>
+      <c r="BM57" s="85"/>
+      <c r="BN57" s="85"/>
+      <c r="BO57" s="85"/>
+      <c r="BP57" s="85"/>
+      <c r="BQ57" s="85"/>
+      <c r="BR57" s="85"/>
+      <c r="BS57" s="85"/>
+      <c r="BT57" s="85"/>
+      <c r="BU57" s="85"/>
+      <c r="BV57" s="85"/>
+      <c r="BW57" s="85"/>
+      <c r="BX57" s="86"/>
+      <c r="BY57" s="28"/>
+      <c r="BZ57" s="28"/>
+      <c r="CA57" s="28"/>
+      <c r="CB57" s="28"/>
+      <c r="CC57" s="28"/>
+      <c r="CD57" s="28"/>
+      <c r="CE57" s="28"/>
+      <c r="CF57" s="84"/>
+    </row>
+    <row r="58" spans="42:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AP58" s="30"/>
+      <c r="AQ58" s="28"/>
+      <c r="AR58" s="28"/>
+      <c r="AS58" s="28"/>
+      <c r="AT58" s="28"/>
+      <c r="AU58" s="28"/>
+      <c r="AV58" s="28"/>
+      <c r="AW58" s="28"/>
+      <c r="AX58" s="28"/>
+      <c r="AY58" s="28"/>
+      <c r="AZ58" s="28"/>
+      <c r="BA58" s="28"/>
+      <c r="BB58" s="28"/>
+      <c r="BC58" s="28"/>
+      <c r="BD58" s="28"/>
+      <c r="BE58" s="28"/>
+      <c r="BF58" s="28"/>
+      <c r="BG58" s="28"/>
+      <c r="BH58" s="28"/>
+      <c r="BI58" s="28"/>
+      <c r="BJ58" s="28"/>
+      <c r="BK58" s="28"/>
+      <c r="BL58" s="28"/>
+      <c r="BM58" s="28"/>
+      <c r="BN58" s="28"/>
+      <c r="BO58" s="28"/>
+      <c r="BP58" s="28"/>
+      <c r="BQ58" s="28"/>
+      <c r="BR58" s="28"/>
+      <c r="BS58" s="28"/>
+      <c r="BT58" s="28"/>
+      <c r="BU58" s="28"/>
+      <c r="BV58" s="28"/>
+      <c r="BW58" s="28"/>
+      <c r="BX58" s="28"/>
+      <c r="BY58" s="28"/>
+      <c r="BZ58" s="28"/>
+      <c r="CA58" s="28"/>
+      <c r="CB58" s="28"/>
+      <c r="CC58" s="28"/>
+      <c r="CD58" s="28"/>
+      <c r="CE58" s="28"/>
+      <c r="CF58" s="84"/>
+    </row>
+    <row r="59" spans="42:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AP59" s="30"/>
+      <c r="AQ59" s="28"/>
+      <c r="AR59" s="28"/>
+      <c r="AS59" s="28"/>
+      <c r="AT59" s="28"/>
+      <c r="AU59" s="28"/>
+      <c r="AV59" s="28"/>
+      <c r="AW59" s="28"/>
+      <c r="AX59" s="28"/>
+      <c r="AY59" s="28"/>
+      <c r="AZ59" s="28"/>
+      <c r="BA59" s="28"/>
+      <c r="BB59" s="28"/>
+      <c r="BC59" s="28"/>
+      <c r="BD59" s="28"/>
+      <c r="BE59" s="28"/>
+      <c r="BF59" s="28"/>
+      <c r="BG59" s="28"/>
+      <c r="BH59" s="28"/>
+      <c r="BI59" s="28"/>
+      <c r="BJ59" s="28"/>
+      <c r="BK59" s="87" t="s">
+        <v>2</v>
+      </c>
+      <c r="BL59" s="88"/>
+      <c r="BM59" s="89"/>
+      <c r="BN59" s="28"/>
+      <c r="BO59" s="28"/>
+      <c r="BP59" s="28"/>
+      <c r="BQ59" s="28"/>
+      <c r="BR59" s="28"/>
+      <c r="BS59" s="28"/>
+      <c r="BT59" s="28"/>
+      <c r="BU59" s="28"/>
+      <c r="BV59" s="28"/>
+      <c r="BW59" s="28"/>
+      <c r="BX59" s="28"/>
+      <c r="BY59" s="28"/>
+      <c r="BZ59" s="28"/>
+      <c r="CA59" s="28"/>
+      <c r="CB59" s="28"/>
+      <c r="CC59" s="28"/>
+      <c r="CD59" s="28"/>
+      <c r="CE59" s="28"/>
+      <c r="CF59" s="84"/>
+    </row>
+    <row r="60" spans="42:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AP60" s="30"/>
+      <c r="AQ60" s="28"/>
+      <c r="AR60" s="28"/>
+      <c r="AS60" s="28"/>
+      <c r="AT60" s="28"/>
+      <c r="AU60" s="28"/>
+      <c r="AV60" s="28"/>
+      <c r="AW60" s="28"/>
+      <c r="AX60" s="28"/>
+      <c r="AY60" s="28"/>
+      <c r="AZ60" s="28"/>
+      <c r="BA60" s="28"/>
+      <c r="BB60" s="28"/>
+      <c r="BC60" s="28"/>
+      <c r="BD60" s="28"/>
+      <c r="BE60" s="28"/>
+      <c r="BF60" s="28"/>
+      <c r="BG60" s="28"/>
+      <c r="BH60" s="28"/>
+      <c r="BI60" s="28"/>
+      <c r="BJ60" s="28"/>
+      <c r="BK60" s="90"/>
+      <c r="BL60" s="91"/>
+      <c r="BM60" s="92"/>
+      <c r="BN60" s="28"/>
+      <c r="BO60" s="28"/>
+      <c r="BP60" s="28"/>
+      <c r="BQ60" s="28"/>
+      <c r="BR60" s="28"/>
+      <c r="BS60" s="28"/>
+      <c r="BT60" s="28"/>
+      <c r="BU60" s="28"/>
+      <c r="BV60" s="28"/>
+      <c r="BW60" s="28"/>
+      <c r="BX60" s="28"/>
+      <c r="BY60" s="28"/>
+      <c r="BZ60" s="28"/>
+      <c r="CA60" s="28"/>
+      <c r="CB60" s="28"/>
+      <c r="CC60" s="28"/>
+      <c r="CD60" s="28"/>
+      <c r="CE60" s="28"/>
+      <c r="CF60" s="84"/>
+    </row>
+    <row r="61" spans="42:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AP61" s="30"/>
+      <c r="AQ61" s="28"/>
+      <c r="AR61" s="28"/>
+      <c r="AS61" s="28"/>
+      <c r="AT61" s="28"/>
+      <c r="AU61" s="28"/>
+      <c r="AV61" s="28"/>
+      <c r="AW61" s="28"/>
+      <c r="AX61" s="28"/>
+      <c r="AY61" s="28"/>
+      <c r="AZ61" s="28"/>
+      <c r="BA61" s="28"/>
+      <c r="BB61" s="28"/>
+      <c r="BC61" s="28"/>
+      <c r="BD61" s="28"/>
+      <c r="BE61" s="28"/>
+      <c r="BF61" s="28"/>
+      <c r="BG61" s="28"/>
+      <c r="BH61" s="28"/>
+      <c r="BI61" s="28"/>
+      <c r="BJ61" s="28"/>
+      <c r="BK61" s="28"/>
+      <c r="BL61" s="28"/>
+      <c r="BM61" s="28"/>
+      <c r="BN61" s="28"/>
+      <c r="BO61" s="28"/>
+      <c r="BP61" s="28"/>
+      <c r="BQ61" s="28"/>
+      <c r="BR61" s="28"/>
+      <c r="BS61" s="28"/>
+      <c r="BT61" s="28"/>
+      <c r="BU61" s="28"/>
+      <c r="BV61" s="28"/>
+      <c r="BW61" s="28"/>
+      <c r="BX61" s="28"/>
+      <c r="BY61" s="28"/>
+      <c r="BZ61" s="28"/>
+      <c r="CA61" s="28"/>
+      <c r="CB61" s="28"/>
+      <c r="CC61" s="28"/>
+      <c r="CD61" s="28"/>
+      <c r="CE61" s="28"/>
+      <c r="CF61" s="84"/>
+    </row>
+    <row r="62" spans="42:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AP62" s="31"/>
+      <c r="AQ62" s="85"/>
+      <c r="AR62" s="85"/>
+      <c r="AS62" s="85"/>
+      <c r="AT62" s="85"/>
+      <c r="AU62" s="85"/>
+      <c r="AV62" s="85"/>
+      <c r="AW62" s="85"/>
+      <c r="AX62" s="85"/>
+      <c r="AY62" s="85"/>
+      <c r="AZ62" s="85"/>
+      <c r="BA62" s="85"/>
+      <c r="BB62" s="85"/>
+      <c r="BC62" s="85"/>
+      <c r="BD62" s="85"/>
+      <c r="BE62" s="85"/>
+      <c r="BF62" s="85"/>
+      <c r="BG62" s="85"/>
+      <c r="BH62" s="85"/>
+      <c r="BI62" s="85"/>
+      <c r="BJ62" s="85"/>
+      <c r="BK62" s="85"/>
+      <c r="BL62" s="85"/>
+      <c r="BM62" s="85"/>
+      <c r="BN62" s="85"/>
+      <c r="BO62" s="85"/>
+      <c r="BP62" s="85"/>
+      <c r="BQ62" s="85"/>
+      <c r="BR62" s="85"/>
+      <c r="BS62" s="85"/>
+      <c r="BT62" s="85"/>
+      <c r="BU62" s="85"/>
+      <c r="BV62" s="85"/>
+      <c r="BW62" s="85"/>
+      <c r="BX62" s="85"/>
+      <c r="BY62" s="85"/>
+      <c r="BZ62" s="85"/>
+      <c r="CA62" s="85"/>
+      <c r="CB62" s="85"/>
+      <c r="CC62" s="85"/>
+      <c r="CD62" s="85"/>
+      <c r="CE62" s="85"/>
+      <c r="CF62" s="86"/>
     </row>
   </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="BK59:BM60"/>
+    <mergeCell ref="BI23:BO23"/>
+    <mergeCell ref="BA55:BC56"/>
+    <mergeCell ref="BO51:BS51"/>
+    <mergeCell ref="BY51:CC51"/>
+    <mergeCell ref="BU55:BW56"/>
+    <mergeCell ref="BN32:BR32"/>
+    <mergeCell ref="BX32:CB32"/>
+    <mergeCell ref="BT36:BV37"/>
+    <mergeCell ref="BJ40:BL41"/>
+    <mergeCell ref="AU51:AY51"/>
+    <mergeCell ref="BE51:BI51"/>
+    <mergeCell ref="BF6:BL6"/>
+    <mergeCell ref="AS32:AW32"/>
+    <mergeCell ref="BC32:BG32"/>
+    <mergeCell ref="AY36:BA37"/>
+    <mergeCell ref="AS17:AW17"/>
+    <mergeCell ref="BC17:BG17"/>
+    <mergeCell ref="AY20:BA21"/>
+    <mergeCell ref="BN17:BR17"/>
+    <mergeCell ref="BX17:CB17"/>
+    <mergeCell ref="BT20:BV21"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add note of NR2
</commit_message>
<xml_diff>
--- a/BNR/bayer.xlsx
+++ b/BNR/bayer.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>五个中的中值</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,6 +51,42 @@
   </si>
   <si>
     <t>多级中值混合滤波</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W33</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -997,7 +1033,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1076,50 +1112,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1152,6 +1152,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2893,10 +2932,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E2:CF62"/>
+  <dimension ref="E2:CF67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="AH61" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="AX66" sqref="AX66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2906,6 +2945,9 @@
     <col min="10" max="11" width="4.5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4.875" customWidth="1"/>
     <col min="18" max="19" width="4.375" customWidth="1"/>
+    <col min="46" max="46" width="4" customWidth="1"/>
+    <col min="47" max="47" width="4.125" customWidth="1"/>
+    <col min="48" max="48" width="4.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="11:82" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -2922,48 +2964,48 @@
       <c r="U6" s="5"/>
       <c r="V6" s="4"/>
       <c r="AP6" s="29"/>
-      <c r="AQ6" s="82"/>
-      <c r="AR6" s="82"/>
-      <c r="AS6" s="82"/>
-      <c r="AT6" s="82"/>
-      <c r="AU6" s="82"/>
-      <c r="AV6" s="82"/>
-      <c r="AW6" s="82"/>
-      <c r="AX6" s="82"/>
-      <c r="AY6" s="82"/>
-      <c r="AZ6" s="82"/>
-      <c r="BA6" s="82"/>
-      <c r="BB6" s="82"/>
-      <c r="BC6" s="82"/>
-      <c r="BD6" s="82"/>
-      <c r="BE6" s="82"/>
-      <c r="BF6" s="95" t="s">
+      <c r="AQ6" s="79"/>
+      <c r="AR6" s="79"/>
+      <c r="AS6" s="79"/>
+      <c r="AT6" s="79"/>
+      <c r="AU6" s="79"/>
+      <c r="AV6" s="79"/>
+      <c r="AW6" s="79"/>
+      <c r="AX6" s="79"/>
+      <c r="AY6" s="79"/>
+      <c r="AZ6" s="79"/>
+      <c r="BA6" s="79"/>
+      <c r="BB6" s="79"/>
+      <c r="BC6" s="79"/>
+      <c r="BD6" s="79"/>
+      <c r="BE6" s="79"/>
+      <c r="BF6" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="BG6" s="96"/>
-      <c r="BH6" s="96"/>
-      <c r="BI6" s="96"/>
-      <c r="BJ6" s="96"/>
-      <c r="BK6" s="96"/>
-      <c r="BL6" s="97"/>
-      <c r="BM6" s="82"/>
-      <c r="BN6" s="82"/>
-      <c r="BO6" s="82"/>
-      <c r="BP6" s="82"/>
-      <c r="BQ6" s="82"/>
-      <c r="BR6" s="82"/>
-      <c r="BS6" s="82"/>
-      <c r="BT6" s="82"/>
-      <c r="BU6" s="82"/>
-      <c r="BV6" s="82"/>
-      <c r="BW6" s="82"/>
-      <c r="BX6" s="82"/>
-      <c r="BY6" s="82"/>
-      <c r="BZ6" s="82"/>
-      <c r="CA6" s="82"/>
-      <c r="CB6" s="82"/>
-      <c r="CC6" s="82"/>
-      <c r="CD6" s="83"/>
+      <c r="BG6" s="105"/>
+      <c r="BH6" s="105"/>
+      <c r="BI6" s="105"/>
+      <c r="BJ6" s="105"/>
+      <c r="BK6" s="105"/>
+      <c r="BL6" s="106"/>
+      <c r="BM6" s="79"/>
+      <c r="BN6" s="79"/>
+      <c r="BO6" s="79"/>
+      <c r="BP6" s="79"/>
+      <c r="BQ6" s="79"/>
+      <c r="BR6" s="79"/>
+      <c r="BS6" s="79"/>
+      <c r="BT6" s="79"/>
+      <c r="BU6" s="79"/>
+      <c r="BV6" s="79"/>
+      <c r="BW6" s="79"/>
+      <c r="BX6" s="79"/>
+      <c r="BY6" s="79"/>
+      <c r="BZ6" s="79"/>
+      <c r="CA6" s="79"/>
+      <c r="CB6" s="79"/>
+      <c r="CC6" s="79"/>
+      <c r="CD6" s="80"/>
     </row>
     <row r="7" spans="11:82" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="P7" s="5"/>
@@ -3013,7 +3055,7 @@
       <c r="CA7" s="28"/>
       <c r="CB7" s="28"/>
       <c r="CC7" s="28"/>
-      <c r="CD7" s="84"/>
+      <c r="CD7" s="81"/>
     </row>
     <row r="8" spans="11:82" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P8" s="4"/>
@@ -3065,7 +3107,7 @@
       <c r="CA8" s="28"/>
       <c r="CB8" s="28"/>
       <c r="CC8" s="28"/>
-      <c r="CD8" s="84"/>
+      <c r="CD8" s="81"/>
     </row>
     <row r="9" spans="11:82" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P9" s="5"/>
@@ -3103,7 +3145,7 @@
       <c r="BM9" s="28"/>
       <c r="BN9" s="76"/>
       <c r="BO9" s="76"/>
-      <c r="BP9" s="93"/>
+      <c r="BP9" s="84"/>
       <c r="BQ9" s="76"/>
       <c r="BR9" s="76"/>
       <c r="BS9" s="28"/>
@@ -3111,13 +3153,13 @@
       <c r="BU9" s="28"/>
       <c r="BV9" s="28"/>
       <c r="BW9" s="28"/>
-      <c r="BX9" s="93"/>
+      <c r="BX9" s="84"/>
       <c r="BY9" s="76"/>
       <c r="BZ9" s="76"/>
       <c r="CA9" s="76"/>
-      <c r="CB9" s="93"/>
+      <c r="CB9" s="84"/>
       <c r="CC9" s="28"/>
-      <c r="CD9" s="84"/>
+      <c r="CD9" s="81"/>
     </row>
     <row r="10" spans="11:82" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P10" s="4"/>
@@ -3169,7 +3211,7 @@
       <c r="CA10" s="77"/>
       <c r="CB10" s="77"/>
       <c r="CC10" s="28"/>
-      <c r="CD10" s="84"/>
+      <c r="CD10" s="81"/>
     </row>
     <row r="11" spans="11:82" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P11" s="5"/>
@@ -3205,23 +3247,23 @@
       <c r="BK11" s="28"/>
       <c r="BL11" s="28"/>
       <c r="BM11" s="28"/>
-      <c r="BN11" s="93"/>
+      <c r="BN11" s="84"/>
       <c r="BO11" s="76"/>
-      <c r="BP11" s="93"/>
+      <c r="BP11" s="84"/>
       <c r="BQ11" s="76"/>
-      <c r="BR11" s="93"/>
+      <c r="BR11" s="84"/>
       <c r="BS11" s="28"/>
       <c r="BT11" s="28"/>
-      <c r="BU11" s="94"/>
+      <c r="BU11" s="85"/>
       <c r="BV11" s="28"/>
       <c r="BW11" s="28"/>
       <c r="BX11" s="76"/>
       <c r="BY11" s="76"/>
-      <c r="BZ11" s="93"/>
+      <c r="BZ11" s="84"/>
       <c r="CA11" s="76"/>
       <c r="CB11" s="76"/>
       <c r="CC11" s="28"/>
-      <c r="CD11" s="84"/>
+      <c r="CD11" s="81"/>
     </row>
     <row r="12" spans="11:82" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="P12" s="4"/>
@@ -3273,7 +3315,7 @@
       <c r="CA12" s="77"/>
       <c r="CB12" s="76"/>
       <c r="CC12" s="28"/>
-      <c r="CD12" s="84"/>
+      <c r="CD12" s="81"/>
     </row>
     <row r="13" spans="11:82" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R13" s="5"/>
@@ -3307,7 +3349,7 @@
       <c r="BM13" s="28"/>
       <c r="BN13" s="76"/>
       <c r="BO13" s="76"/>
-      <c r="BP13" s="93"/>
+      <c r="BP13" s="84"/>
       <c r="BQ13" s="76"/>
       <c r="BR13" s="76"/>
       <c r="BS13" s="28"/>
@@ -3315,13 +3357,13 @@
       <c r="BU13" s="28"/>
       <c r="BV13" s="28"/>
       <c r="BW13" s="28"/>
-      <c r="BX13" s="93"/>
+      <c r="BX13" s="84"/>
       <c r="BY13" s="76"/>
       <c r="BZ13" s="76"/>
       <c r="CA13" s="76"/>
-      <c r="CB13" s="93"/>
+      <c r="CB13" s="84"/>
       <c r="CC13" s="28"/>
-      <c r="CD13" s="84"/>
+      <c r="CD13" s="81"/>
     </row>
     <row r="14" spans="11:82" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R14" s="4"/>
@@ -3369,7 +3411,7 @@
       <c r="CA14" s="28"/>
       <c r="CB14" s="28"/>
       <c r="CC14" s="28"/>
-      <c r="CD14" s="84"/>
+      <c r="CD14" s="81"/>
     </row>
     <row r="15" spans="11:82" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AP15" s="30"/>
@@ -3412,7 +3454,7 @@
       <c r="CA15" s="28"/>
       <c r="CB15" s="28"/>
       <c r="CC15" s="28"/>
-      <c r="CD15" s="84"/>
+      <c r="CD15" s="81"/>
     </row>
     <row r="16" spans="11:82" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="K16" s="20"/>
@@ -3448,7 +3490,7 @@
       <c r="AO16" s="20"/>
       <c r="AP16" s="23"/>
       <c r="AQ16" s="20"/>
-      <c r="AR16" s="81"/>
+      <c r="AR16" s="78"/>
       <c r="AS16" s="21"/>
       <c r="AT16" s="21"/>
       <c r="AU16" s="21"/>
@@ -3459,17 +3501,17 @@
       <c r="AZ16" s="21"/>
       <c r="BA16" s="21"/>
       <c r="BB16" s="21"/>
-      <c r="BC16" s="82"/>
-      <c r="BD16" s="82"/>
-      <c r="BE16" s="82"/>
-      <c r="BF16" s="82"/>
-      <c r="BG16" s="82"/>
-      <c r="BH16" s="83"/>
+      <c r="BC16" s="79"/>
+      <c r="BD16" s="79"/>
+      <c r="BE16" s="79"/>
+      <c r="BF16" s="79"/>
+      <c r="BG16" s="79"/>
+      <c r="BH16" s="80"/>
       <c r="BI16" s="28"/>
       <c r="BJ16" s="28"/>
       <c r="BK16" s="28"/>
       <c r="BL16" s="20"/>
-      <c r="BM16" s="81"/>
+      <c r="BM16" s="78"/>
       <c r="BN16" s="21"/>
       <c r="BO16" s="21"/>
       <c r="BP16" s="21"/>
@@ -3480,13 +3522,13 @@
       <c r="BU16" s="21"/>
       <c r="BV16" s="21"/>
       <c r="BW16" s="21"/>
-      <c r="BX16" s="82"/>
-      <c r="BY16" s="82"/>
-      <c r="BZ16" s="82"/>
-      <c r="CA16" s="82"/>
-      <c r="CB16" s="82"/>
-      <c r="CC16" s="83"/>
-      <c r="CD16" s="84"/>
+      <c r="BX16" s="79"/>
+      <c r="BY16" s="79"/>
+      <c r="BZ16" s="79"/>
+      <c r="CA16" s="79"/>
+      <c r="CB16" s="79"/>
+      <c r="CC16" s="80"/>
+      <c r="CD16" s="81"/>
     </row>
     <row r="17" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J17" s="29"/>
@@ -3524,52 +3566,52 @@
       <c r="AP17" s="23"/>
       <c r="AQ17" s="20"/>
       <c r="AR17" s="23"/>
-      <c r="AS17" s="78" t="s">
+      <c r="AS17" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="AT17" s="79"/>
-      <c r="AU17" s="79"/>
-      <c r="AV17" s="79"/>
-      <c r="AW17" s="80"/>
+      <c r="AT17" s="108"/>
+      <c r="AU17" s="108"/>
+      <c r="AV17" s="108"/>
+      <c r="AW17" s="109"/>
       <c r="AX17" s="20"/>
       <c r="AY17" s="20"/>
       <c r="AZ17" s="5"/>
       <c r="BA17" s="20"/>
       <c r="BB17" s="28"/>
-      <c r="BC17" s="78" t="s">
+      <c r="BC17" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="BD17" s="79"/>
-      <c r="BE17" s="79"/>
-      <c r="BF17" s="79"/>
-      <c r="BG17" s="80"/>
-      <c r="BH17" s="84"/>
+      <c r="BD17" s="108"/>
+      <c r="BE17" s="108"/>
+      <c r="BF17" s="108"/>
+      <c r="BG17" s="109"/>
+      <c r="BH17" s="81"/>
       <c r="BI17" s="28"/>
       <c r="BJ17" s="28"/>
       <c r="BK17" s="28"/>
       <c r="BL17" s="20"/>
       <c r="BM17" s="23"/>
-      <c r="BN17" s="78" t="s">
+      <c r="BN17" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="BO17" s="79"/>
-      <c r="BP17" s="79"/>
-      <c r="BQ17" s="79"/>
-      <c r="BR17" s="80"/>
+      <c r="BO17" s="108"/>
+      <c r="BP17" s="108"/>
+      <c r="BQ17" s="108"/>
+      <c r="BR17" s="109"/>
       <c r="BS17" s="20"/>
       <c r="BT17" s="20"/>
-      <c r="BU17" s="94"/>
+      <c r="BU17" s="85"/>
       <c r="BV17" s="20"/>
       <c r="BW17" s="28"/>
-      <c r="BX17" s="78" t="s">
+      <c r="BX17" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="BY17" s="79"/>
-      <c r="BZ17" s="79"/>
-      <c r="CA17" s="79"/>
-      <c r="CB17" s="80"/>
-      <c r="CC17" s="84"/>
-      <c r="CD17" s="84"/>
+      <c r="BY17" s="108"/>
+      <c r="BZ17" s="108"/>
+      <c r="CA17" s="108"/>
+      <c r="CB17" s="109"/>
+      <c r="CC17" s="81"/>
+      <c r="CD17" s="81"/>
     </row>
     <row r="18" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J18" s="30"/>
@@ -3617,12 +3659,12 @@
       <c r="AZ18" s="26"/>
       <c r="BA18" s="26"/>
       <c r="BB18" s="26"/>
-      <c r="BC18" s="85"/>
-      <c r="BD18" s="85"/>
-      <c r="BE18" s="85"/>
-      <c r="BF18" s="85"/>
-      <c r="BG18" s="85"/>
-      <c r="BH18" s="86"/>
+      <c r="BC18" s="82"/>
+      <c r="BD18" s="82"/>
+      <c r="BE18" s="82"/>
+      <c r="BF18" s="82"/>
+      <c r="BG18" s="82"/>
+      <c r="BH18" s="83"/>
       <c r="BI18" s="28"/>
       <c r="BJ18" s="28"/>
       <c r="BK18" s="28"/>
@@ -3638,13 +3680,13 @@
       <c r="BU18" s="26"/>
       <c r="BV18" s="26"/>
       <c r="BW18" s="26"/>
-      <c r="BX18" s="85"/>
-      <c r="BY18" s="85"/>
-      <c r="BZ18" s="85"/>
-      <c r="CA18" s="85"/>
-      <c r="CB18" s="85"/>
-      <c r="CC18" s="86"/>
-      <c r="CD18" s="84"/>
+      <c r="BX18" s="82"/>
+      <c r="BY18" s="82"/>
+      <c r="BZ18" s="82"/>
+      <c r="CA18" s="82"/>
+      <c r="CB18" s="82"/>
+      <c r="CC18" s="83"/>
+      <c r="CD18" s="81"/>
     </row>
     <row r="19" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J19" s="30"/>
@@ -3719,7 +3761,7 @@
       <c r="CA19" s="28"/>
       <c r="CB19" s="28"/>
       <c r="CC19" s="28"/>
-      <c r="CD19" s="84"/>
+      <c r="CD19" s="81"/>
     </row>
     <row r="20" spans="10:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J20" s="30"/>
@@ -3763,11 +3805,11 @@
       <c r="AV20" s="20"/>
       <c r="AW20" s="20"/>
       <c r="AX20" s="20"/>
-      <c r="AY20" s="87" t="s">
+      <c r="AY20" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="AZ20" s="88"/>
-      <c r="BA20" s="89"/>
+      <c r="AZ20" s="99"/>
+      <c r="BA20" s="100"/>
       <c r="BB20" s="20"/>
       <c r="BC20" s="28"/>
       <c r="BD20" s="28"/>
@@ -3786,11 +3828,11 @@
       <c r="BQ20" s="20"/>
       <c r="BR20" s="20"/>
       <c r="BS20" s="20"/>
-      <c r="BT20" s="87" t="s">
+      <c r="BT20" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="BU20" s="88"/>
-      <c r="BV20" s="89"/>
+      <c r="BU20" s="99"/>
+      <c r="BV20" s="100"/>
       <c r="BW20" s="20"/>
       <c r="BX20" s="28"/>
       <c r="BY20" s="28"/>
@@ -3798,7 +3840,7 @@
       <c r="CA20" s="28"/>
       <c r="CB20" s="28"/>
       <c r="CC20" s="28"/>
-      <c r="CD20" s="84"/>
+      <c r="CD20" s="81"/>
     </row>
     <row r="21" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J21" s="31"/>
@@ -3842,9 +3884,9 @@
       <c r="AV21" s="20"/>
       <c r="AW21" s="20"/>
       <c r="AX21" s="20"/>
-      <c r="AY21" s="90"/>
-      <c r="AZ21" s="91"/>
-      <c r="BA21" s="92"/>
+      <c r="AY21" s="101"/>
+      <c r="AZ21" s="102"/>
+      <c r="BA21" s="103"/>
       <c r="BB21" s="20"/>
       <c r="BC21" s="28"/>
       <c r="BD21" s="28"/>
@@ -3863,9 +3905,9 @@
       <c r="BQ21" s="20"/>
       <c r="BR21" s="20"/>
       <c r="BS21" s="20"/>
-      <c r="BT21" s="90"/>
-      <c r="BU21" s="91"/>
-      <c r="BV21" s="92"/>
+      <c r="BT21" s="101"/>
+      <c r="BU21" s="102"/>
+      <c r="BV21" s="103"/>
       <c r="BW21" s="20"/>
       <c r="BX21" s="28"/>
       <c r="BY21" s="28"/>
@@ -3873,7 +3915,7 @@
       <c r="CA21" s="28"/>
       <c r="CB21" s="28"/>
       <c r="CC21" s="28"/>
-      <c r="CD21" s="84"/>
+      <c r="CD21" s="81"/>
     </row>
     <row r="22" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J22" s="34"/>
@@ -3948,7 +3990,7 @@
       <c r="CA22" s="28"/>
       <c r="CB22" s="28"/>
       <c r="CC22" s="28"/>
-      <c r="CD22" s="84"/>
+      <c r="CD22" s="81"/>
     </row>
     <row r="23" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J23" s="34"/>
@@ -3983,7 +4025,7 @@
       <c r="AM23" s="20"/>
       <c r="AN23" s="20"/>
       <c r="AO23" s="20"/>
-      <c r="AP23" s="81"/>
+      <c r="AP23" s="78"/>
       <c r="AQ23" s="21"/>
       <c r="AR23" s="21"/>
       <c r="AS23" s="21"/>
@@ -3996,38 +4038,38 @@
       <c r="AZ23" s="21"/>
       <c r="BA23" s="21"/>
       <c r="BB23" s="21"/>
-      <c r="BC23" s="82"/>
-      <c r="BD23" s="82"/>
-      <c r="BE23" s="82"/>
-      <c r="BF23" s="82"/>
-      <c r="BG23" s="82"/>
-      <c r="BH23" s="82"/>
-      <c r="BI23" s="95" t="s">
+      <c r="BC23" s="79"/>
+      <c r="BD23" s="79"/>
+      <c r="BE23" s="79"/>
+      <c r="BF23" s="79"/>
+      <c r="BG23" s="79"/>
+      <c r="BH23" s="79"/>
+      <c r="BI23" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="BJ23" s="96"/>
-      <c r="BK23" s="96"/>
-      <c r="BL23" s="96"/>
-      <c r="BM23" s="96"/>
-      <c r="BN23" s="96"/>
-      <c r="BO23" s="97"/>
-      <c r="BP23" s="82"/>
-      <c r="BQ23" s="82"/>
-      <c r="BR23" s="82"/>
-      <c r="BS23" s="82"/>
-      <c r="BT23" s="82"/>
-      <c r="BU23" s="82"/>
-      <c r="BV23" s="82"/>
-      <c r="BW23" s="82"/>
-      <c r="BX23" s="82"/>
-      <c r="BY23" s="82"/>
-      <c r="BZ23" s="82"/>
-      <c r="CA23" s="82"/>
-      <c r="CB23" s="82"/>
-      <c r="CC23" s="82"/>
-      <c r="CD23" s="82"/>
-      <c r="CE23" s="82"/>
-      <c r="CF23" s="83"/>
+      <c r="BJ23" s="105"/>
+      <c r="BK23" s="105"/>
+      <c r="BL23" s="105"/>
+      <c r="BM23" s="105"/>
+      <c r="BN23" s="105"/>
+      <c r="BO23" s="106"/>
+      <c r="BP23" s="79"/>
+      <c r="BQ23" s="79"/>
+      <c r="BR23" s="79"/>
+      <c r="BS23" s="79"/>
+      <c r="BT23" s="79"/>
+      <c r="BU23" s="79"/>
+      <c r="BV23" s="79"/>
+      <c r="BW23" s="79"/>
+      <c r="BX23" s="79"/>
+      <c r="BY23" s="79"/>
+      <c r="BZ23" s="79"/>
+      <c r="CA23" s="79"/>
+      <c r="CB23" s="79"/>
+      <c r="CC23" s="79"/>
+      <c r="CD23" s="79"/>
+      <c r="CE23" s="79"/>
+      <c r="CF23" s="80"/>
     </row>
     <row r="24" spans="10:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J24" s="34"/>
@@ -4104,7 +4146,7 @@
       <c r="CC24" s="28"/>
       <c r="CD24" s="28"/>
       <c r="CE24" s="28"/>
-      <c r="CF24" s="84"/>
+      <c r="CF24" s="81"/>
     </row>
     <row r="25" spans="10:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J25" s="34"/>
@@ -4181,7 +4223,7 @@
       <c r="CC25" s="28"/>
       <c r="CD25" s="28"/>
       <c r="CE25" s="28"/>
-      <c r="CF25" s="84"/>
+      <c r="CF25" s="81"/>
     </row>
     <row r="26" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J26" s="34"/>
@@ -4258,7 +4300,7 @@
       <c r="CC26" s="28"/>
       <c r="CD26" s="28"/>
       <c r="CE26" s="28"/>
-      <c r="CF26" s="84"/>
+      <c r="CF26" s="81"/>
     </row>
     <row r="27" spans="10:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J27" s="34"/>
@@ -4335,7 +4377,7 @@
       <c r="CC27" s="28"/>
       <c r="CD27" s="28"/>
       <c r="CE27" s="28"/>
-      <c r="CF27" s="84"/>
+      <c r="CF27" s="81"/>
     </row>
     <row r="28" spans="10:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J28" s="34"/>
@@ -4412,7 +4454,7 @@
       <c r="CC28" s="28"/>
       <c r="CD28" s="28"/>
       <c r="CE28" s="28"/>
-      <c r="CF28" s="84"/>
+      <c r="CF28" s="81"/>
     </row>
     <row r="29" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J29" s="34"/>
@@ -4489,7 +4531,7 @@
       <c r="CC29" s="28"/>
       <c r="CD29" s="28"/>
       <c r="CE29" s="28"/>
-      <c r="CF29" s="84"/>
+      <c r="CF29" s="81"/>
     </row>
     <row r="30" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J30" s="34"/>
@@ -4566,7 +4608,7 @@
       <c r="CC30" s="28"/>
       <c r="CD30" s="28"/>
       <c r="CE30" s="28"/>
-      <c r="CF30" s="84"/>
+      <c r="CF30" s="81"/>
     </row>
     <row r="31" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J31" s="34"/>
@@ -4603,7 +4645,7 @@
       <c r="AO31" s="20"/>
       <c r="AP31" s="23"/>
       <c r="AQ31" s="20"/>
-      <c r="AR31" s="81"/>
+      <c r="AR31" s="78"/>
       <c r="AS31" s="21"/>
       <c r="AT31" s="21"/>
       <c r="AU31" s="21"/>
@@ -4614,36 +4656,36 @@
       <c r="AZ31" s="21"/>
       <c r="BA31" s="21"/>
       <c r="BB31" s="21"/>
-      <c r="BC31" s="82"/>
-      <c r="BD31" s="82"/>
-      <c r="BE31" s="82"/>
-      <c r="BF31" s="82"/>
-      <c r="BG31" s="82"/>
-      <c r="BH31" s="83"/>
+      <c r="BC31" s="79"/>
+      <c r="BD31" s="79"/>
+      <c r="BE31" s="79"/>
+      <c r="BF31" s="79"/>
+      <c r="BG31" s="79"/>
+      <c r="BH31" s="80"/>
       <c r="BI31" s="28"/>
       <c r="BJ31" s="28"/>
       <c r="BK31" s="28"/>
       <c r="BL31" s="28"/>
       <c r="BM31" s="29"/>
-      <c r="BN31" s="82"/>
-      <c r="BO31" s="82"/>
-      <c r="BP31" s="82"/>
-      <c r="BQ31" s="82"/>
-      <c r="BR31" s="82"/>
-      <c r="BS31" s="82"/>
-      <c r="BT31" s="82"/>
-      <c r="BU31" s="82"/>
-      <c r="BV31" s="82"/>
-      <c r="BW31" s="82"/>
-      <c r="BX31" s="82"/>
-      <c r="BY31" s="82"/>
-      <c r="BZ31" s="82"/>
-      <c r="CA31" s="82"/>
-      <c r="CB31" s="82"/>
-      <c r="CC31" s="83"/>
+      <c r="BN31" s="79"/>
+      <c r="BO31" s="79"/>
+      <c r="BP31" s="79"/>
+      <c r="BQ31" s="79"/>
+      <c r="BR31" s="79"/>
+      <c r="BS31" s="79"/>
+      <c r="BT31" s="79"/>
+      <c r="BU31" s="79"/>
+      <c r="BV31" s="79"/>
+      <c r="BW31" s="79"/>
+      <c r="BX31" s="79"/>
+      <c r="BY31" s="79"/>
+      <c r="BZ31" s="79"/>
+      <c r="CA31" s="79"/>
+      <c r="CB31" s="79"/>
+      <c r="CC31" s="80"/>
       <c r="CD31" s="28"/>
       <c r="CE31" s="28"/>
-      <c r="CF31" s="84"/>
+      <c r="CF31" s="81"/>
     </row>
     <row r="32" spans="10:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J32" s="34"/>
@@ -4681,54 +4723,54 @@
       <c r="AP32" s="23"/>
       <c r="AQ32" s="20"/>
       <c r="AR32" s="23"/>
-      <c r="AS32" s="78" t="s">
+      <c r="AS32" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="AT32" s="79"/>
-      <c r="AU32" s="79"/>
-      <c r="AV32" s="79"/>
-      <c r="AW32" s="80"/>
+      <c r="AT32" s="108"/>
+      <c r="AU32" s="108"/>
+      <c r="AV32" s="108"/>
+      <c r="AW32" s="109"/>
       <c r="AX32" s="20"/>
       <c r="AY32" s="20"/>
       <c r="AZ32" s="5"/>
       <c r="BA32" s="20"/>
       <c r="BB32" s="28"/>
-      <c r="BC32" s="78" t="s">
+      <c r="BC32" s="107" t="s">
         <v>4</v>
       </c>
-      <c r="BD32" s="79"/>
-      <c r="BE32" s="79"/>
-      <c r="BF32" s="79"/>
-      <c r="BG32" s="80"/>
-      <c r="BH32" s="84"/>
+      <c r="BD32" s="108"/>
+      <c r="BE32" s="108"/>
+      <c r="BF32" s="108"/>
+      <c r="BG32" s="109"/>
+      <c r="BH32" s="81"/>
       <c r="BI32" s="28"/>
       <c r="BJ32" s="28"/>
       <c r="BK32" s="28"/>
       <c r="BL32" s="28"/>
       <c r="BM32" s="30"/>
-      <c r="BN32" s="78" t="s">
+      <c r="BN32" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="BO32" s="79"/>
-      <c r="BP32" s="79"/>
-      <c r="BQ32" s="79"/>
-      <c r="BR32" s="80"/>
+      <c r="BO32" s="108"/>
+      <c r="BP32" s="108"/>
+      <c r="BQ32" s="108"/>
+      <c r="BR32" s="109"/>
       <c r="BS32" s="28"/>
       <c r="BT32" s="28"/>
       <c r="BU32" s="5"/>
       <c r="BV32" s="28"/>
       <c r="BW32" s="28"/>
-      <c r="BX32" s="78" t="s">
+      <c r="BX32" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="BY32" s="79"/>
-      <c r="BZ32" s="79"/>
-      <c r="CA32" s="79"/>
-      <c r="CB32" s="80"/>
-      <c r="CC32" s="84"/>
+      <c r="BY32" s="108"/>
+      <c r="BZ32" s="108"/>
+      <c r="CA32" s="108"/>
+      <c r="CB32" s="109"/>
+      <c r="CC32" s="81"/>
       <c r="CD32" s="28"/>
       <c r="CE32" s="28"/>
-      <c r="CF32" s="84"/>
+      <c r="CF32" s="81"/>
     </row>
     <row r="33" spans="5:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J33" s="34"/>
@@ -4776,36 +4818,36 @@
       <c r="AZ33" s="26"/>
       <c r="BA33" s="26"/>
       <c r="BB33" s="26"/>
-      <c r="BC33" s="85"/>
-      <c r="BD33" s="85"/>
-      <c r="BE33" s="85"/>
-      <c r="BF33" s="85"/>
-      <c r="BG33" s="85"/>
-      <c r="BH33" s="86"/>
+      <c r="BC33" s="82"/>
+      <c r="BD33" s="82"/>
+      <c r="BE33" s="82"/>
+      <c r="BF33" s="82"/>
+      <c r="BG33" s="82"/>
+      <c r="BH33" s="83"/>
       <c r="BI33" s="28"/>
       <c r="BJ33" s="28"/>
       <c r="BK33" s="28"/>
       <c r="BL33" s="28"/>
       <c r="BM33" s="31"/>
-      <c r="BN33" s="85"/>
-      <c r="BO33" s="85"/>
-      <c r="BP33" s="85"/>
-      <c r="BQ33" s="85"/>
-      <c r="BR33" s="85"/>
-      <c r="BS33" s="85"/>
-      <c r="BT33" s="85"/>
-      <c r="BU33" s="85"/>
-      <c r="BV33" s="85"/>
-      <c r="BW33" s="85"/>
-      <c r="BX33" s="85"/>
-      <c r="BY33" s="85"/>
-      <c r="BZ33" s="85"/>
-      <c r="CA33" s="85"/>
-      <c r="CB33" s="85"/>
-      <c r="CC33" s="86"/>
+      <c r="BN33" s="82"/>
+      <c r="BO33" s="82"/>
+      <c r="BP33" s="82"/>
+      <c r="BQ33" s="82"/>
+      <c r="BR33" s="82"/>
+      <c r="BS33" s="82"/>
+      <c r="BT33" s="82"/>
+      <c r="BU33" s="82"/>
+      <c r="BV33" s="82"/>
+      <c r="BW33" s="82"/>
+      <c r="BX33" s="82"/>
+      <c r="BY33" s="82"/>
+      <c r="BZ33" s="82"/>
+      <c r="CA33" s="82"/>
+      <c r="CB33" s="82"/>
+      <c r="CC33" s="83"/>
       <c r="CD33" s="28"/>
       <c r="CE33" s="28"/>
-      <c r="CF33" s="84"/>
+      <c r="CF33" s="81"/>
     </row>
     <row r="34" spans="5:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J34" s="34"/>
@@ -4882,7 +4924,7 @@
       <c r="CC34" s="28"/>
       <c r="CD34" s="28"/>
       <c r="CE34" s="28"/>
-      <c r="CF34" s="84"/>
+      <c r="CF34" s="81"/>
     </row>
     <row r="35" spans="5:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J35" s="34"/>
@@ -4925,32 +4967,32 @@
       <c r="AU35" s="20"/>
       <c r="AV35" s="20"/>
       <c r="AW35" s="20"/>
-      <c r="AX35" s="81"/>
-      <c r="AY35" s="82"/>
-      <c r="AZ35" s="82"/>
-      <c r="BA35" s="82"/>
+      <c r="AX35" s="78"/>
+      <c r="AY35" s="79"/>
+      <c r="AZ35" s="79"/>
+      <c r="BA35" s="79"/>
       <c r="BB35" s="21"/>
-      <c r="BC35" s="82"/>
-      <c r="BD35" s="82"/>
-      <c r="BE35" s="82"/>
-      <c r="BF35" s="82"/>
-      <c r="BG35" s="82"/>
-      <c r="BH35" s="82"/>
-      <c r="BI35" s="82"/>
-      <c r="BJ35" s="82"/>
-      <c r="BK35" s="82"/>
-      <c r="BL35" s="82"/>
-      <c r="BM35" s="82"/>
-      <c r="BN35" s="82"/>
-      <c r="BO35" s="82"/>
-      <c r="BP35" s="82"/>
-      <c r="BQ35" s="82"/>
-      <c r="BR35" s="82"/>
-      <c r="BS35" s="82"/>
-      <c r="BT35" s="82"/>
-      <c r="BU35" s="82"/>
-      <c r="BV35" s="82"/>
-      <c r="BW35" s="83"/>
+      <c r="BC35" s="79"/>
+      <c r="BD35" s="79"/>
+      <c r="BE35" s="79"/>
+      <c r="BF35" s="79"/>
+      <c r="BG35" s="79"/>
+      <c r="BH35" s="79"/>
+      <c r="BI35" s="79"/>
+      <c r="BJ35" s="79"/>
+      <c r="BK35" s="79"/>
+      <c r="BL35" s="79"/>
+      <c r="BM35" s="79"/>
+      <c r="BN35" s="79"/>
+      <c r="BO35" s="79"/>
+      <c r="BP35" s="79"/>
+      <c r="BQ35" s="79"/>
+      <c r="BR35" s="79"/>
+      <c r="BS35" s="79"/>
+      <c r="BT35" s="79"/>
+      <c r="BU35" s="79"/>
+      <c r="BV35" s="79"/>
+      <c r="BW35" s="80"/>
       <c r="BX35" s="28"/>
       <c r="BY35" s="28"/>
       <c r="BZ35" s="28"/>
@@ -4959,7 +5001,7 @@
       <c r="CC35" s="28"/>
       <c r="CD35" s="28"/>
       <c r="CE35" s="28"/>
-      <c r="CF35" s="84"/>
+      <c r="CF35" s="81"/>
     </row>
     <row r="36" spans="5:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J36" s="34"/>
@@ -5003,11 +5045,11 @@
       <c r="AV36" s="20"/>
       <c r="AW36" s="20"/>
       <c r="AX36" s="23"/>
-      <c r="AY36" s="87" t="s">
+      <c r="AY36" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="AZ36" s="88"/>
-      <c r="BA36" s="89"/>
+      <c r="AZ36" s="99"/>
+      <c r="BA36" s="100"/>
       <c r="BB36" s="20"/>
       <c r="BC36" s="28"/>
       <c r="BD36" s="28"/>
@@ -5026,12 +5068,12 @@
       <c r="BQ36" s="28"/>
       <c r="BR36" s="28"/>
       <c r="BS36" s="28"/>
-      <c r="BT36" s="87" t="s">
+      <c r="BT36" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="BU36" s="88"/>
-      <c r="BV36" s="89"/>
-      <c r="BW36" s="84"/>
+      <c r="BU36" s="99"/>
+      <c r="BV36" s="100"/>
+      <c r="BW36" s="81"/>
       <c r="BX36" s="28"/>
       <c r="BY36" s="28"/>
       <c r="BZ36" s="28"/>
@@ -5040,7 +5082,7 @@
       <c r="CC36" s="28"/>
       <c r="CD36" s="28"/>
       <c r="CE36" s="28"/>
-      <c r="CF36" s="84"/>
+      <c r="CF36" s="81"/>
     </row>
     <row r="37" spans="5:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J37" s="34"/>
@@ -5084,9 +5126,9 @@
       <c r="AV37" s="20"/>
       <c r="AW37" s="20"/>
       <c r="AX37" s="23"/>
-      <c r="AY37" s="90"/>
-      <c r="AZ37" s="91"/>
-      <c r="BA37" s="92"/>
+      <c r="AY37" s="101"/>
+      <c r="AZ37" s="102"/>
+      <c r="BA37" s="103"/>
       <c r="BB37" s="20"/>
       <c r="BC37" s="28"/>
       <c r="BD37" s="28"/>
@@ -5105,10 +5147,10 @@
       <c r="BQ37" s="28"/>
       <c r="BR37" s="28"/>
       <c r="BS37" s="28"/>
-      <c r="BT37" s="90"/>
-      <c r="BU37" s="91"/>
-      <c r="BV37" s="92"/>
-      <c r="BW37" s="84"/>
+      <c r="BT37" s="101"/>
+      <c r="BU37" s="102"/>
+      <c r="BV37" s="103"/>
+      <c r="BW37" s="81"/>
       <c r="BX37" s="28"/>
       <c r="BY37" s="28"/>
       <c r="BZ37" s="28"/>
@@ -5117,7 +5159,7 @@
       <c r="CC37" s="28"/>
       <c r="CD37" s="28"/>
       <c r="CE37" s="28"/>
-      <c r="CF37" s="84"/>
+      <c r="CF37" s="81"/>
     </row>
     <row r="38" spans="5:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J38" s="34"/>
@@ -5161,31 +5203,31 @@
       <c r="AV38" s="20"/>
       <c r="AW38" s="20"/>
       <c r="AX38" s="25"/>
-      <c r="AY38" s="85"/>
-      <c r="AZ38" s="85"/>
-      <c r="BA38" s="85"/>
+      <c r="AY38" s="82"/>
+      <c r="AZ38" s="82"/>
+      <c r="BA38" s="82"/>
       <c r="BB38" s="26"/>
-      <c r="BC38" s="85"/>
-      <c r="BD38" s="98"/>
-      <c r="BE38" s="98"/>
-      <c r="BF38" s="98"/>
-      <c r="BG38" s="85"/>
-      <c r="BH38" s="85"/>
-      <c r="BI38" s="85"/>
-      <c r="BJ38" s="85"/>
-      <c r="BK38" s="85"/>
-      <c r="BL38" s="85"/>
-      <c r="BM38" s="85"/>
-      <c r="BN38" s="85"/>
-      <c r="BO38" s="85"/>
-      <c r="BP38" s="85"/>
-      <c r="BQ38" s="85"/>
-      <c r="BR38" s="85"/>
-      <c r="BS38" s="85"/>
-      <c r="BT38" s="85"/>
-      <c r="BU38" s="85"/>
-      <c r="BV38" s="85"/>
-      <c r="BW38" s="86"/>
+      <c r="BC38" s="82"/>
+      <c r="BD38" s="86"/>
+      <c r="BE38" s="86"/>
+      <c r="BF38" s="86"/>
+      <c r="BG38" s="82"/>
+      <c r="BH38" s="82"/>
+      <c r="BI38" s="82"/>
+      <c r="BJ38" s="82"/>
+      <c r="BK38" s="82"/>
+      <c r="BL38" s="82"/>
+      <c r="BM38" s="82"/>
+      <c r="BN38" s="82"/>
+      <c r="BO38" s="82"/>
+      <c r="BP38" s="82"/>
+      <c r="BQ38" s="82"/>
+      <c r="BR38" s="82"/>
+      <c r="BS38" s="82"/>
+      <c r="BT38" s="82"/>
+      <c r="BU38" s="82"/>
+      <c r="BV38" s="82"/>
+      <c r="BW38" s="83"/>
       <c r="BX38" s="28"/>
       <c r="BY38" s="28"/>
       <c r="BZ38" s="28"/>
@@ -5194,7 +5236,7 @@
       <c r="CC38" s="28"/>
       <c r="CD38" s="28"/>
       <c r="CE38" s="28"/>
-      <c r="CF38" s="84"/>
+      <c r="CF38" s="81"/>
     </row>
     <row r="39" spans="5:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J39" s="34"/>
@@ -5240,9 +5282,9 @@
       <c r="BA39" s="28"/>
       <c r="BB39" s="28"/>
       <c r="BC39" s="28"/>
-      <c r="BD39" s="100"/>
-      <c r="BE39" s="100"/>
-      <c r="BF39" s="100"/>
+      <c r="BD39" s="88"/>
+      <c r="BE39" s="88"/>
+      <c r="BF39" s="88"/>
       <c r="BG39" s="28"/>
       <c r="BH39" s="28"/>
       <c r="BI39" s="28"/>
@@ -5268,10 +5310,10 @@
       <c r="CC39" s="28"/>
       <c r="CD39" s="28"/>
       <c r="CE39" s="28"/>
-      <c r="CF39" s="84"/>
+      <c r="CF39" s="81"/>
     </row>
     <row r="40" spans="5:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E40" s="99"/>
+      <c r="E40" s="87"/>
       <c r="J40" s="34"/>
       <c r="K40" s="28"/>
       <c r="L40" s="28"/>
@@ -5321,11 +5363,11 @@
       <c r="BG40" s="28"/>
       <c r="BH40" s="28"/>
       <c r="BI40" s="28"/>
-      <c r="BJ40" s="87" t="s">
+      <c r="BJ40" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="BK40" s="88"/>
-      <c r="BL40" s="89"/>
+      <c r="BK40" s="99"/>
+      <c r="BL40" s="100"/>
       <c r="BM40" s="28"/>
       <c r="BN40" s="28"/>
       <c r="BO40" s="28"/>
@@ -5345,7 +5387,7 @@
       <c r="CC40" s="28"/>
       <c r="CD40" s="28"/>
       <c r="CE40" s="28"/>
-      <c r="CF40" s="84"/>
+      <c r="CF40" s="81"/>
     </row>
     <row r="41" spans="5:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J41" s="34"/>
@@ -5397,9 +5439,9 @@
       <c r="BG41" s="28"/>
       <c r="BH41" s="28"/>
       <c r="BI41" s="28"/>
-      <c r="BJ41" s="90"/>
-      <c r="BK41" s="91"/>
-      <c r="BL41" s="92"/>
+      <c r="BJ41" s="101"/>
+      <c r="BK41" s="102"/>
+      <c r="BL41" s="103"/>
       <c r="BM41" s="28"/>
       <c r="BN41" s="28"/>
       <c r="BO41" s="28"/>
@@ -5419,7 +5461,7 @@
       <c r="CC41" s="28"/>
       <c r="CD41" s="28"/>
       <c r="CE41" s="28"/>
-      <c r="CF41" s="84"/>
+      <c r="CF41" s="81"/>
     </row>
     <row r="42" spans="5:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J42" s="34"/>
@@ -5493,7 +5535,7 @@
       <c r="CC42" s="28"/>
       <c r="CD42" s="28"/>
       <c r="CE42" s="28"/>
-      <c r="CF42" s="84"/>
+      <c r="CF42" s="81"/>
     </row>
     <row r="43" spans="5:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J43" s="34"/>
@@ -5532,7 +5574,7 @@
       <c r="AT43" s="28"/>
       <c r="AU43" s="76"/>
       <c r="AV43" s="76"/>
-      <c r="AW43" s="93"/>
+      <c r="AW43" s="84"/>
       <c r="AX43" s="76"/>
       <c r="AY43" s="76"/>
       <c r="AZ43" s="28"/>
@@ -5554,20 +5596,20 @@
       <c r="BP43" s="76"/>
       <c r="BQ43" s="77"/>
       <c r="BR43" s="76"/>
-      <c r="BS43" s="93"/>
+      <c r="BS43" s="84"/>
       <c r="BT43" s="28"/>
       <c r="BU43" s="28"/>
       <c r="BV43" s="28"/>
       <c r="BW43" s="28"/>
       <c r="BX43" s="28"/>
-      <c r="BY43" s="93"/>
+      <c r="BY43" s="84"/>
       <c r="BZ43" s="76"/>
       <c r="CA43" s="76"/>
       <c r="CB43" s="76"/>
       <c r="CC43" s="76"/>
       <c r="CD43" s="28"/>
       <c r="CE43" s="28"/>
-      <c r="CF43" s="84"/>
+      <c r="CF43" s="81"/>
     </row>
     <row r="44" spans="5:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J44" s="37"/>
@@ -5641,7 +5683,7 @@
       <c r="CC44" s="76"/>
       <c r="CD44" s="28"/>
       <c r="CE44" s="28"/>
-      <c r="CF44" s="84"/>
+      <c r="CF44" s="81"/>
     </row>
     <row r="45" spans="5:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AP45" s="30"/>
@@ -5651,42 +5693,42 @@
       <c r="AT45" s="28"/>
       <c r="AU45" s="77"/>
       <c r="AV45" s="76"/>
-      <c r="AW45" s="93"/>
+      <c r="AW45" s="84"/>
       <c r="AX45" s="76"/>
       <c r="AY45" s="77"/>
       <c r="AZ45" s="28"/>
       <c r="BA45" s="28"/>
-      <c r="BB45" s="94"/>
+      <c r="BB45" s="85"/>
       <c r="BC45" s="28"/>
       <c r="BD45" s="28"/>
-      <c r="BE45" s="93"/>
+      <c r="BE45" s="84"/>
       <c r="BF45" s="76"/>
-      <c r="BG45" s="93"/>
+      <c r="BG45" s="84"/>
       <c r="BH45" s="76"/>
-      <c r="BI45" s="93"/>
+      <c r="BI45" s="84"/>
       <c r="BJ45" s="28"/>
       <c r="BK45" s="28"/>
-      <c r="BL45" s="94"/>
+      <c r="BL45" s="85"/>
       <c r="BM45" s="20"/>
       <c r="BN45" s="28"/>
       <c r="BO45" s="77"/>
       <c r="BP45" s="76"/>
-      <c r="BQ45" s="93"/>
+      <c r="BQ45" s="84"/>
       <c r="BR45" s="76"/>
       <c r="BS45" s="77"/>
       <c r="BT45" s="28"/>
       <c r="BU45" s="28"/>
-      <c r="BV45" s="94"/>
+      <c r="BV45" s="85"/>
       <c r="BW45" s="28"/>
       <c r="BX45" s="28"/>
       <c r="BY45" s="77"/>
       <c r="BZ45" s="76"/>
-      <c r="CA45" s="93"/>
+      <c r="CA45" s="84"/>
       <c r="CB45" s="76"/>
       <c r="CC45" s="77"/>
       <c r="CD45" s="28"/>
       <c r="CE45" s="28"/>
-      <c r="CF45" s="84"/>
+      <c r="CF45" s="81"/>
     </row>
     <row r="46" spans="5:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AP46" s="30"/>
@@ -5731,38 +5773,38 @@
       <c r="CC46" s="77"/>
       <c r="CD46" s="28"/>
       <c r="CE46" s="28"/>
-      <c r="CF46" s="84"/>
+      <c r="CF46" s="81"/>
     </row>
     <row r="47" spans="5:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F47" s="28"/>
-      <c r="G47" s="101">
+      <c r="G47" s="89">
         <v>10</v>
       </c>
-      <c r="H47" s="102">
+      <c r="H47" s="90">
         <v>9</v>
       </c>
-      <c r="I47" s="102">
+      <c r="I47" s="90">
         <v>4</v>
       </c>
-      <c r="J47" s="102">
+      <c r="J47" s="90">
         <v>7</v>
       </c>
-      <c r="K47" s="103">
+      <c r="K47" s="91">
         <v>7</v>
       </c>
-      <c r="O47" s="101">
+      <c r="O47" s="89">
         <v>10</v>
       </c>
-      <c r="P47" s="102">
+      <c r="P47" s="90">
         <v>9</v>
       </c>
-      <c r="Q47" s="102">
+      <c r="Q47" s="90">
         <v>4</v>
       </c>
-      <c r="R47" s="102">
+      <c r="R47" s="90">
         <v>7</v>
       </c>
-      <c r="S47" s="103">
+      <c r="S47" s="91">
         <v>7</v>
       </c>
       <c r="AP47" s="30"/>
@@ -5772,7 +5814,7 @@
       <c r="AT47" s="28"/>
       <c r="AU47" s="76"/>
       <c r="AV47" s="76"/>
-      <c r="AW47" s="93"/>
+      <c r="AW47" s="84"/>
       <c r="AX47" s="76"/>
       <c r="AY47" s="76"/>
       <c r="AZ47" s="28"/>
@@ -5790,7 +5832,7 @@
       <c r="BL47" s="28"/>
       <c r="BM47" s="20"/>
       <c r="BN47" s="28"/>
-      <c r="BO47" s="93"/>
+      <c r="BO47" s="84"/>
       <c r="BP47" s="76"/>
       <c r="BQ47" s="77"/>
       <c r="BR47" s="76"/>
@@ -5804,41 +5846,41 @@
       <c r="BZ47" s="76"/>
       <c r="CA47" s="76"/>
       <c r="CB47" s="76"/>
-      <c r="CC47" s="93"/>
+      <c r="CC47" s="84"/>
       <c r="CD47" s="28"/>
       <c r="CE47" s="28"/>
-      <c r="CF47" s="84"/>
+      <c r="CF47" s="81"/>
     </row>
     <row r="48" spans="5:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F48" s="28"/>
-      <c r="G48" s="104">
+      <c r="G48" s="92">
         <v>4</v>
       </c>
-      <c r="H48" s="109">
+      <c r="H48" s="97">
         <v>50</v>
       </c>
-      <c r="I48" s="109">
+      <c r="I48" s="97">
         <v>60</v>
       </c>
-      <c r="J48" s="109">
+      <c r="J48" s="97">
         <v>45</v>
       </c>
-      <c r="K48" s="105">
+      <c r="K48" s="93">
         <v>30</v>
       </c>
-      <c r="O48" s="104">
+      <c r="O48" s="92">
         <v>4</v>
       </c>
-      <c r="P48" s="109">
+      <c r="P48" s="97">
         <v>50</v>
       </c>
-      <c r="Q48" s="109">
+      <c r="Q48" s="97">
         <v>60</v>
       </c>
-      <c r="R48" s="109">
+      <c r="R48" s="97">
         <v>45</v>
       </c>
-      <c r="S48" s="105">
+      <c r="S48" s="93">
         <v>30</v>
       </c>
       <c r="AP48" s="30"/>
@@ -5883,38 +5925,38 @@
       <c r="CC48" s="28"/>
       <c r="CD48" s="28"/>
       <c r="CE48" s="28"/>
-      <c r="CF48" s="84"/>
+      <c r="CF48" s="81"/>
     </row>
     <row r="49" spans="6:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F49" s="28"/>
-      <c r="G49" s="104">
+      <c r="G49" s="92">
         <v>40</v>
       </c>
-      <c r="H49" s="109">
+      <c r="H49" s="97">
         <v>75</v>
       </c>
-      <c r="I49" s="109">
+      <c r="I49" s="97">
         <v>80</v>
       </c>
-      <c r="J49" s="109">
+      <c r="J49" s="97">
         <v>52</v>
       </c>
-      <c r="K49" s="105">
+      <c r="K49" s="93">
         <v>210</v>
       </c>
-      <c r="O49" s="104">
+      <c r="O49" s="92">
         <v>40</v>
       </c>
-      <c r="P49" s="109">
+      <c r="P49" s="97">
         <v>75</v>
       </c>
-      <c r="Q49" s="109">
+      <c r="Q49" s="97">
         <v>75</v>
       </c>
-      <c r="R49" s="109">
+      <c r="R49" s="97">
         <v>52</v>
       </c>
-      <c r="S49" s="105">
+      <c r="S49" s="93">
         <v>210</v>
       </c>
       <c r="AP49" s="30"/>
@@ -5959,45 +6001,45 @@
       <c r="CC49" s="28"/>
       <c r="CD49" s="28"/>
       <c r="CE49" s="28"/>
-      <c r="CF49" s="84"/>
+      <c r="CF49" s="81"/>
     </row>
     <row r="50" spans="6:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F50" s="28"/>
-      <c r="G50" s="104">
+      <c r="G50" s="92">
         <v>50</v>
       </c>
-      <c r="H50" s="109">
+      <c r="H50" s="97">
         <v>90</v>
       </c>
-      <c r="I50" s="109">
+      <c r="I50" s="97">
         <v>200</v>
       </c>
-      <c r="J50" s="109">
+      <c r="J50" s="97">
         <v>255</v>
       </c>
-      <c r="K50" s="105">
+      <c r="K50" s="93">
         <v>201</v>
       </c>
-      <c r="O50" s="104">
+      <c r="O50" s="92">
         <v>50</v>
       </c>
-      <c r="P50" s="109">
+      <c r="P50" s="97">
         <v>90</v>
       </c>
-      <c r="Q50" s="109">
+      <c r="Q50" s="97">
         <v>200</v>
       </c>
-      <c r="R50" s="109">
+      <c r="R50" s="97">
         <v>255</v>
       </c>
-      <c r="S50" s="105">
+      <c r="S50" s="93">
         <v>201</v>
       </c>
       <c r="AP50" s="30"/>
       <c r="AQ50" s="28"/>
       <c r="AR50" s="28"/>
       <c r="AS50" s="20"/>
-      <c r="AT50" s="81"/>
+      <c r="AT50" s="78"/>
       <c r="AU50" s="21"/>
       <c r="AV50" s="21"/>
       <c r="AW50" s="21"/>
@@ -6008,16 +6050,16 @@
       <c r="BB50" s="21"/>
       <c r="BC50" s="21"/>
       <c r="BD50" s="21"/>
-      <c r="BE50" s="82"/>
-      <c r="BF50" s="82"/>
-      <c r="BG50" s="82"/>
-      <c r="BH50" s="82"/>
-      <c r="BI50" s="82"/>
-      <c r="BJ50" s="83"/>
+      <c r="BE50" s="79"/>
+      <c r="BF50" s="79"/>
+      <c r="BG50" s="79"/>
+      <c r="BH50" s="79"/>
+      <c r="BI50" s="79"/>
+      <c r="BJ50" s="80"/>
       <c r="BK50" s="28"/>
       <c r="BL50" s="28"/>
       <c r="BM50" s="20"/>
-      <c r="BN50" s="81"/>
+      <c r="BN50" s="78"/>
       <c r="BO50" s="21"/>
       <c r="BP50" s="21"/>
       <c r="BQ50" s="21"/>
@@ -6028,45 +6070,45 @@
       <c r="BV50" s="21"/>
       <c r="BW50" s="21"/>
       <c r="BX50" s="21"/>
-      <c r="BY50" s="82"/>
-      <c r="BZ50" s="82"/>
-      <c r="CA50" s="82"/>
-      <c r="CB50" s="82"/>
-      <c r="CC50" s="82"/>
-      <c r="CD50" s="83"/>
+      <c r="BY50" s="79"/>
+      <c r="BZ50" s="79"/>
+      <c r="CA50" s="79"/>
+      <c r="CB50" s="79"/>
+      <c r="CC50" s="79"/>
+      <c r="CD50" s="80"/>
       <c r="CE50" s="28"/>
-      <c r="CF50" s="84"/>
+      <c r="CF50" s="81"/>
     </row>
     <row r="51" spans="6:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F51" s="28"/>
-      <c r="G51" s="106">
+      <c r="G51" s="94">
         <v>60</v>
       </c>
-      <c r="H51" s="107">
+      <c r="H51" s="95">
         <v>44</v>
       </c>
-      <c r="I51" s="107">
+      <c r="I51" s="95">
         <v>85</v>
       </c>
-      <c r="J51" s="107">
+      <c r="J51" s="95">
         <v>89</v>
       </c>
-      <c r="K51" s="108">
+      <c r="K51" s="96">
         <v>90</v>
       </c>
-      <c r="O51" s="106">
+      <c r="O51" s="94">
         <v>60</v>
       </c>
-      <c r="P51" s="107">
+      <c r="P51" s="95">
         <v>44</v>
       </c>
-      <c r="Q51" s="107">
+      <c r="Q51" s="95">
         <v>85</v>
       </c>
-      <c r="R51" s="107">
+      <c r="R51" s="95">
         <v>89</v>
       </c>
-      <c r="S51" s="108">
+      <c r="S51" s="96">
         <v>90</v>
       </c>
       <c r="AP51" s="30"/>
@@ -6074,52 +6116,52 @@
       <c r="AR51" s="28"/>
       <c r="AS51" s="20"/>
       <c r="AT51" s="23"/>
-      <c r="AU51" s="78" t="s">
+      <c r="AU51" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="AV51" s="79"/>
-      <c r="AW51" s="79"/>
-      <c r="AX51" s="79"/>
-      <c r="AY51" s="80"/>
+      <c r="AV51" s="108"/>
+      <c r="AW51" s="108"/>
+      <c r="AX51" s="108"/>
+      <c r="AY51" s="109"/>
       <c r="AZ51" s="20"/>
       <c r="BA51" s="20"/>
-      <c r="BB51" s="94"/>
+      <c r="BB51" s="85"/>
       <c r="BC51" s="20"/>
       <c r="BD51" s="28"/>
-      <c r="BE51" s="78" t="s">
+      <c r="BE51" s="107" t="s">
         <v>4</v>
       </c>
-      <c r="BF51" s="79"/>
-      <c r="BG51" s="79"/>
-      <c r="BH51" s="79"/>
-      <c r="BI51" s="80"/>
-      <c r="BJ51" s="84"/>
+      <c r="BF51" s="108"/>
+      <c r="BG51" s="108"/>
+      <c r="BH51" s="108"/>
+      <c r="BI51" s="109"/>
+      <c r="BJ51" s="81"/>
       <c r="BK51" s="28"/>
       <c r="BL51" s="28"/>
       <c r="BM51" s="20"/>
       <c r="BN51" s="23"/>
-      <c r="BO51" s="78" t="s">
+      <c r="BO51" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="BP51" s="79"/>
-      <c r="BQ51" s="79"/>
-      <c r="BR51" s="79"/>
-      <c r="BS51" s="80"/>
+      <c r="BP51" s="108"/>
+      <c r="BQ51" s="108"/>
+      <c r="BR51" s="108"/>
+      <c r="BS51" s="109"/>
       <c r="BT51" s="20"/>
       <c r="BU51" s="20"/>
-      <c r="BV51" s="94"/>
+      <c r="BV51" s="85"/>
       <c r="BW51" s="20"/>
       <c r="BX51" s="28"/>
-      <c r="BY51" s="78" t="s">
+      <c r="BY51" s="107" t="s">
         <v>4</v>
       </c>
-      <c r="BZ51" s="79"/>
-      <c r="CA51" s="79"/>
-      <c r="CB51" s="79"/>
-      <c r="CC51" s="80"/>
-      <c r="CD51" s="84"/>
+      <c r="BZ51" s="108"/>
+      <c r="CA51" s="108"/>
+      <c r="CB51" s="108"/>
+      <c r="CC51" s="109"/>
+      <c r="CD51" s="81"/>
       <c r="CE51" s="28"/>
-      <c r="CF51" s="84"/>
+      <c r="CF51" s="81"/>
     </row>
     <row r="52" spans="6:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F52" s="28"/>
@@ -6143,12 +6185,12 @@
       <c r="BB52" s="26"/>
       <c r="BC52" s="26"/>
       <c r="BD52" s="26"/>
-      <c r="BE52" s="85"/>
-      <c r="BF52" s="85"/>
-      <c r="BG52" s="85"/>
-      <c r="BH52" s="85"/>
-      <c r="BI52" s="85"/>
-      <c r="BJ52" s="86"/>
+      <c r="BE52" s="82"/>
+      <c r="BF52" s="82"/>
+      <c r="BG52" s="82"/>
+      <c r="BH52" s="82"/>
+      <c r="BI52" s="82"/>
+      <c r="BJ52" s="83"/>
       <c r="BK52" s="28"/>
       <c r="BL52" s="28"/>
       <c r="BM52" s="20"/>
@@ -6163,14 +6205,14 @@
       <c r="BV52" s="26"/>
       <c r="BW52" s="26"/>
       <c r="BX52" s="26"/>
-      <c r="BY52" s="85"/>
-      <c r="BZ52" s="85"/>
-      <c r="CA52" s="85"/>
-      <c r="CB52" s="85"/>
-      <c r="CC52" s="85"/>
-      <c r="CD52" s="86"/>
+      <c r="BY52" s="82"/>
+      <c r="BZ52" s="82"/>
+      <c r="CA52" s="82"/>
+      <c r="CB52" s="82"/>
+      <c r="CC52" s="82"/>
+      <c r="CD52" s="83"/>
       <c r="CE52" s="28"/>
-      <c r="CF52" s="84"/>
+      <c r="CF52" s="81"/>
     </row>
     <row r="53" spans="6:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AP53" s="30"/>
@@ -6215,7 +6257,7 @@
       <c r="CC53" s="28"/>
       <c r="CD53" s="28"/>
       <c r="CE53" s="28"/>
-      <c r="CF53" s="84"/>
+      <c r="CF53" s="81"/>
     </row>
     <row r="54" spans="6:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AP54" s="30"/>
@@ -6229,30 +6271,30 @@
       <c r="AX54" s="28"/>
       <c r="AY54" s="28"/>
       <c r="AZ54" s="29"/>
-      <c r="BA54" s="82"/>
-      <c r="BB54" s="82"/>
-      <c r="BC54" s="82"/>
-      <c r="BD54" s="82"/>
-      <c r="BE54" s="82"/>
-      <c r="BF54" s="82"/>
-      <c r="BG54" s="82"/>
-      <c r="BH54" s="82"/>
-      <c r="BI54" s="82"/>
-      <c r="BJ54" s="82"/>
-      <c r="BK54" s="82"/>
-      <c r="BL54" s="82"/>
-      <c r="BM54" s="82"/>
-      <c r="BN54" s="82"/>
-      <c r="BO54" s="82"/>
-      <c r="BP54" s="82"/>
-      <c r="BQ54" s="82"/>
-      <c r="BR54" s="82"/>
-      <c r="BS54" s="82"/>
-      <c r="BT54" s="82"/>
-      <c r="BU54" s="82"/>
-      <c r="BV54" s="82"/>
-      <c r="BW54" s="82"/>
-      <c r="BX54" s="83"/>
+      <c r="BA54" s="79"/>
+      <c r="BB54" s="79"/>
+      <c r="BC54" s="79"/>
+      <c r="BD54" s="79"/>
+      <c r="BE54" s="79"/>
+      <c r="BF54" s="79"/>
+      <c r="BG54" s="79"/>
+      <c r="BH54" s="79"/>
+      <c r="BI54" s="79"/>
+      <c r="BJ54" s="79"/>
+      <c r="BK54" s="79"/>
+      <c r="BL54" s="79"/>
+      <c r="BM54" s="79"/>
+      <c r="BN54" s="79"/>
+      <c r="BO54" s="79"/>
+      <c r="BP54" s="79"/>
+      <c r="BQ54" s="79"/>
+      <c r="BR54" s="79"/>
+      <c r="BS54" s="79"/>
+      <c r="BT54" s="79"/>
+      <c r="BU54" s="79"/>
+      <c r="BV54" s="79"/>
+      <c r="BW54" s="79"/>
+      <c r="BX54" s="80"/>
       <c r="BY54" s="28"/>
       <c r="BZ54" s="28"/>
       <c r="CA54" s="28"/>
@@ -6260,7 +6302,7 @@
       <c r="CC54" s="28"/>
       <c r="CD54" s="28"/>
       <c r="CE54" s="28"/>
-      <c r="CF54" s="84"/>
+      <c r="CF54" s="81"/>
     </row>
     <row r="55" spans="6:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AP55" s="30"/>
@@ -6274,11 +6316,11 @@
       <c r="AX55" s="28"/>
       <c r="AY55" s="28"/>
       <c r="AZ55" s="30"/>
-      <c r="BA55" s="87" t="s">
+      <c r="BA55" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="BB55" s="88"/>
-      <c r="BC55" s="89"/>
+      <c r="BB55" s="99"/>
+      <c r="BC55" s="100"/>
       <c r="BD55" s="28"/>
       <c r="BE55" s="28"/>
       <c r="BF55" s="28"/>
@@ -6287,7 +6329,7 @@
       <c r="BI55" s="28"/>
       <c r="BJ55" s="28"/>
       <c r="BK55" s="28"/>
-      <c r="BL55" s="94"/>
+      <c r="BL55" s="85"/>
       <c r="BM55" s="28"/>
       <c r="BN55" s="28"/>
       <c r="BO55" s="28"/>
@@ -6296,12 +6338,12 @@
       <c r="BR55" s="28"/>
       <c r="BS55" s="28"/>
       <c r="BT55" s="28"/>
-      <c r="BU55" s="87" t="s">
+      <c r="BU55" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="BV55" s="88"/>
-      <c r="BW55" s="89"/>
-      <c r="BX55" s="84"/>
+      <c r="BV55" s="99"/>
+      <c r="BW55" s="100"/>
+      <c r="BX55" s="81"/>
       <c r="BY55" s="28"/>
       <c r="BZ55" s="28"/>
       <c r="CA55" s="28"/>
@@ -6309,7 +6351,7 @@
       <c r="CC55" s="28"/>
       <c r="CD55" s="28"/>
       <c r="CE55" s="28"/>
-      <c r="CF55" s="84"/>
+      <c r="CF55" s="81"/>
     </row>
     <row r="56" spans="6:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AP56" s="30"/>
@@ -6323,9 +6365,9 @@
       <c r="AX56" s="28"/>
       <c r="AY56" s="28"/>
       <c r="AZ56" s="30"/>
-      <c r="BA56" s="90"/>
-      <c r="BB56" s="91"/>
-      <c r="BC56" s="92"/>
+      <c r="BA56" s="101"/>
+      <c r="BB56" s="102"/>
+      <c r="BC56" s="103"/>
       <c r="BD56" s="28"/>
       <c r="BE56" s="28"/>
       <c r="BF56" s="28"/>
@@ -6343,10 +6385,10 @@
       <c r="BR56" s="28"/>
       <c r="BS56" s="28"/>
       <c r="BT56" s="28"/>
-      <c r="BU56" s="90"/>
-      <c r="BV56" s="91"/>
-      <c r="BW56" s="92"/>
-      <c r="BX56" s="84"/>
+      <c r="BU56" s="101"/>
+      <c r="BV56" s="102"/>
+      <c r="BW56" s="103"/>
+      <c r="BX56" s="81"/>
       <c r="BY56" s="28"/>
       <c r="BZ56" s="28"/>
       <c r="CA56" s="28"/>
@@ -6354,7 +6396,7 @@
       <c r="CC56" s="28"/>
       <c r="CD56" s="28"/>
       <c r="CE56" s="28"/>
-      <c r="CF56" s="84"/>
+      <c r="CF56" s="81"/>
     </row>
     <row r="57" spans="6:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AP57" s="30"/>
@@ -6368,30 +6410,30 @@
       <c r="AX57" s="28"/>
       <c r="AY57" s="28"/>
       <c r="AZ57" s="31"/>
-      <c r="BA57" s="85"/>
-      <c r="BB57" s="85"/>
-      <c r="BC57" s="85"/>
-      <c r="BD57" s="85"/>
-      <c r="BE57" s="85"/>
-      <c r="BF57" s="85"/>
-      <c r="BG57" s="85"/>
-      <c r="BH57" s="85"/>
-      <c r="BI57" s="85"/>
-      <c r="BJ57" s="85"/>
-      <c r="BK57" s="85"/>
-      <c r="BL57" s="85"/>
-      <c r="BM57" s="85"/>
-      <c r="BN57" s="85"/>
-      <c r="BO57" s="85"/>
-      <c r="BP57" s="85"/>
-      <c r="BQ57" s="85"/>
-      <c r="BR57" s="85"/>
-      <c r="BS57" s="85"/>
-      <c r="BT57" s="85"/>
-      <c r="BU57" s="85"/>
-      <c r="BV57" s="85"/>
-      <c r="BW57" s="85"/>
-      <c r="BX57" s="86"/>
+      <c r="BA57" s="82"/>
+      <c r="BB57" s="82"/>
+      <c r="BC57" s="82"/>
+      <c r="BD57" s="82"/>
+      <c r="BE57" s="82"/>
+      <c r="BF57" s="82"/>
+      <c r="BG57" s="82"/>
+      <c r="BH57" s="82"/>
+      <c r="BI57" s="82"/>
+      <c r="BJ57" s="82"/>
+      <c r="BK57" s="82"/>
+      <c r="BL57" s="82"/>
+      <c r="BM57" s="82"/>
+      <c r="BN57" s="82"/>
+      <c r="BO57" s="82"/>
+      <c r="BP57" s="82"/>
+      <c r="BQ57" s="82"/>
+      <c r="BR57" s="82"/>
+      <c r="BS57" s="82"/>
+      <c r="BT57" s="82"/>
+      <c r="BU57" s="82"/>
+      <c r="BV57" s="82"/>
+      <c r="BW57" s="82"/>
+      <c r="BX57" s="83"/>
       <c r="BY57" s="28"/>
       <c r="BZ57" s="28"/>
       <c r="CA57" s="28"/>
@@ -6399,7 +6441,7 @@
       <c r="CC57" s="28"/>
       <c r="CD57" s="28"/>
       <c r="CE57" s="28"/>
-      <c r="CF57" s="84"/>
+      <c r="CF57" s="81"/>
     </row>
     <row r="58" spans="6:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AP58" s="30"/>
@@ -6444,7 +6486,7 @@
       <c r="CC58" s="28"/>
       <c r="CD58" s="28"/>
       <c r="CE58" s="28"/>
-      <c r="CF58" s="84"/>
+      <c r="CF58" s="81"/>
     </row>
     <row r="59" spans="6:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AP59" s="30"/>
@@ -6468,11 +6510,11 @@
       <c r="BH59" s="28"/>
       <c r="BI59" s="28"/>
       <c r="BJ59" s="28"/>
-      <c r="BK59" s="87" t="s">
+      <c r="BK59" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="BL59" s="88"/>
-      <c r="BM59" s="89"/>
+      <c r="BL59" s="99"/>
+      <c r="BM59" s="100"/>
       <c r="BN59" s="28"/>
       <c r="BO59" s="28"/>
       <c r="BP59" s="28"/>
@@ -6491,7 +6533,7 @@
       <c r="CC59" s="28"/>
       <c r="CD59" s="28"/>
       <c r="CE59" s="28"/>
-      <c r="CF59" s="84"/>
+      <c r="CF59" s="81"/>
     </row>
     <row r="60" spans="6:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AP60" s="30"/>
@@ -6515,9 +6557,9 @@
       <c r="BH60" s="28"/>
       <c r="BI60" s="28"/>
       <c r="BJ60" s="28"/>
-      <c r="BK60" s="90"/>
-      <c r="BL60" s="91"/>
-      <c r="BM60" s="92"/>
+      <c r="BK60" s="101"/>
+      <c r="BL60" s="102"/>
+      <c r="BM60" s="103"/>
       <c r="BN60" s="28"/>
       <c r="BO60" s="28"/>
       <c r="BP60" s="28"/>
@@ -6536,7 +6578,7 @@
       <c r="CC60" s="28"/>
       <c r="CD60" s="28"/>
       <c r="CE60" s="28"/>
-      <c r="CF60" s="84"/>
+      <c r="CF60" s="81"/>
     </row>
     <row r="61" spans="6:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AP61" s="30"/>
@@ -6581,55 +6623,100 @@
       <c r="CC61" s="28"/>
       <c r="CD61" s="28"/>
       <c r="CE61" s="28"/>
-      <c r="CF61" s="84"/>
+      <c r="CF61" s="81"/>
     </row>
     <row r="62" spans="6:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AP62" s="31"/>
-      <c r="AQ62" s="85"/>
-      <c r="AR62" s="85"/>
-      <c r="AS62" s="85"/>
-      <c r="AT62" s="85"/>
-      <c r="AU62" s="85"/>
-      <c r="AV62" s="85"/>
-      <c r="AW62" s="85"/>
-      <c r="AX62" s="85"/>
-      <c r="AY62" s="85"/>
-      <c r="AZ62" s="85"/>
-      <c r="BA62" s="85"/>
-      <c r="BB62" s="85"/>
-      <c r="BC62" s="85"/>
-      <c r="BD62" s="85"/>
-      <c r="BE62" s="85"/>
-      <c r="BF62" s="85"/>
-      <c r="BG62" s="85"/>
-      <c r="BH62" s="85"/>
-      <c r="BI62" s="85"/>
-      <c r="BJ62" s="85"/>
-      <c r="BK62" s="85"/>
-      <c r="BL62" s="85"/>
-      <c r="BM62" s="85"/>
-      <c r="BN62" s="85"/>
-      <c r="BO62" s="85"/>
-      <c r="BP62" s="85"/>
-      <c r="BQ62" s="85"/>
-      <c r="BR62" s="85"/>
-      <c r="BS62" s="85"/>
-      <c r="BT62" s="85"/>
-      <c r="BU62" s="85"/>
-      <c r="BV62" s="85"/>
-      <c r="BW62" s="85"/>
-      <c r="BX62" s="85"/>
-      <c r="BY62" s="85"/>
-      <c r="BZ62" s="85"/>
-      <c r="CA62" s="85"/>
-      <c r="CB62" s="85"/>
-      <c r="CC62" s="85"/>
-      <c r="CD62" s="85"/>
-      <c r="CE62" s="85"/>
-      <c r="CF62" s="86"/>
+      <c r="AQ62" s="82"/>
+      <c r="AR62" s="82"/>
+      <c r="AS62" s="82"/>
+      <c r="AT62" s="82"/>
+      <c r="AU62" s="82"/>
+      <c r="AV62" s="82"/>
+      <c r="AW62" s="82"/>
+      <c r="AX62" s="82"/>
+      <c r="AY62" s="82"/>
+      <c r="AZ62" s="82"/>
+      <c r="BA62" s="82"/>
+      <c r="BB62" s="82"/>
+      <c r="BC62" s="82"/>
+      <c r="BD62" s="82"/>
+      <c r="BE62" s="82"/>
+      <c r="BF62" s="82"/>
+      <c r="BG62" s="82"/>
+      <c r="BH62" s="82"/>
+      <c r="BI62" s="82"/>
+      <c r="BJ62" s="82"/>
+      <c r="BK62" s="82"/>
+      <c r="BL62" s="82"/>
+      <c r="BM62" s="82"/>
+      <c r="BN62" s="82"/>
+      <c r="BO62" s="82"/>
+      <c r="BP62" s="82"/>
+      <c r="BQ62" s="82"/>
+      <c r="BR62" s="82"/>
+      <c r="BS62" s="82"/>
+      <c r="BT62" s="82"/>
+      <c r="BU62" s="82"/>
+      <c r="BV62" s="82"/>
+      <c r="BW62" s="82"/>
+      <c r="BX62" s="82"/>
+      <c r="BY62" s="82"/>
+      <c r="BZ62" s="82"/>
+      <c r="CA62" s="82"/>
+      <c r="CB62" s="82"/>
+      <c r="CC62" s="82"/>
+      <c r="CD62" s="82"/>
+      <c r="CE62" s="82"/>
+      <c r="CF62" s="83"/>
+    </row>
+    <row r="65" spans="46:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AT65" s="110" t="s">
+        <v>7</v>
+      </c>
+      <c r="AU65" s="110" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV65" s="110" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="46:48" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AT66" s="110" t="s">
+        <v>10</v>
+      </c>
+      <c r="AU66" s="110" t="s">
+        <v>11</v>
+      </c>
+      <c r="AV66" s="110" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="46:48" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AT67" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="AU67" s="110" t="s">
+        <v>14</v>
+      </c>
+      <c r="AV67" s="110" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="BN17:BR17"/>
+    <mergeCell ref="BX17:CB17"/>
+    <mergeCell ref="BT20:BV21"/>
+    <mergeCell ref="AU51:AY51"/>
+    <mergeCell ref="BE51:BI51"/>
+    <mergeCell ref="BF6:BL6"/>
+    <mergeCell ref="AS32:AW32"/>
+    <mergeCell ref="BC32:BG32"/>
+    <mergeCell ref="AY36:BA37"/>
+    <mergeCell ref="AS17:AW17"/>
+    <mergeCell ref="BC17:BG17"/>
+    <mergeCell ref="AY20:BA21"/>
     <mergeCell ref="BK59:BM60"/>
     <mergeCell ref="BI23:BO23"/>
     <mergeCell ref="BA55:BC56"/>
@@ -6640,18 +6727,6 @@
     <mergeCell ref="BX32:CB32"/>
     <mergeCell ref="BT36:BV37"/>
     <mergeCell ref="BJ40:BL41"/>
-    <mergeCell ref="AU51:AY51"/>
-    <mergeCell ref="BE51:BI51"/>
-    <mergeCell ref="BF6:BL6"/>
-    <mergeCell ref="AS32:AW32"/>
-    <mergeCell ref="BC32:BG32"/>
-    <mergeCell ref="AY36:BA37"/>
-    <mergeCell ref="AS17:AW17"/>
-    <mergeCell ref="BC17:BG17"/>
-    <mergeCell ref="AY20:BA21"/>
-    <mergeCell ref="BN17:BR17"/>
-    <mergeCell ref="BX17:CB17"/>
-    <mergeCell ref="BT20:BV21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
BNR2 video is OK
</commit_message>
<xml_diff>
--- a/BNR/bayer.xlsx
+++ b/BNR/bayer.xlsx
@@ -1154,6 +1154,18 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1179,18 +1191,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2932,10 +2932,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E2:CF67"/>
+  <dimension ref="E2:CH111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH61" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="AX66" sqref="AX66"/>
+    <sheetView tabSelected="1" topLeftCell="BI94" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="CI102" sqref="CI102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2943,7 +2943,7 @@
     <col min="7" max="8" width="3.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.25" customWidth="1"/>
     <col min="10" max="11" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.875" customWidth="1"/>
+    <col min="17" max="17" width="3.875" customWidth="1"/>
     <col min="18" max="19" width="4.375" customWidth="1"/>
     <col min="46" max="46" width="4" customWidth="1"/>
     <col min="47" max="47" width="4.125" customWidth="1"/>
@@ -2979,15 +2979,15 @@
       <c r="BC6" s="79"/>
       <c r="BD6" s="79"/>
       <c r="BE6" s="79"/>
-      <c r="BF6" s="104" t="s">
+      <c r="BF6" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="BG6" s="105"/>
-      <c r="BH6" s="105"/>
-      <c r="BI6" s="105"/>
-      <c r="BJ6" s="105"/>
-      <c r="BK6" s="105"/>
-      <c r="BL6" s="106"/>
+      <c r="BG6" s="109"/>
+      <c r="BH6" s="109"/>
+      <c r="BI6" s="109"/>
+      <c r="BJ6" s="109"/>
+      <c r="BK6" s="109"/>
+      <c r="BL6" s="110"/>
       <c r="BM6" s="79"/>
       <c r="BN6" s="79"/>
       <c r="BO6" s="79"/>
@@ -3566,50 +3566,50 @@
       <c r="AP17" s="23"/>
       <c r="AQ17" s="20"/>
       <c r="AR17" s="23"/>
-      <c r="AS17" s="107" t="s">
+      <c r="AS17" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="AT17" s="108"/>
-      <c r="AU17" s="108"/>
-      <c r="AV17" s="108"/>
-      <c r="AW17" s="109"/>
+      <c r="AT17" s="100"/>
+      <c r="AU17" s="100"/>
+      <c r="AV17" s="100"/>
+      <c r="AW17" s="101"/>
       <c r="AX17" s="20"/>
       <c r="AY17" s="20"/>
       <c r="AZ17" s="5"/>
       <c r="BA17" s="20"/>
       <c r="BB17" s="28"/>
-      <c r="BC17" s="107" t="s">
+      <c r="BC17" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="BD17" s="108"/>
-      <c r="BE17" s="108"/>
-      <c r="BF17" s="108"/>
-      <c r="BG17" s="109"/>
+      <c r="BD17" s="100"/>
+      <c r="BE17" s="100"/>
+      <c r="BF17" s="100"/>
+      <c r="BG17" s="101"/>
       <c r="BH17" s="81"/>
       <c r="BI17" s="28"/>
       <c r="BJ17" s="28"/>
       <c r="BK17" s="28"/>
       <c r="BL17" s="20"/>
       <c r="BM17" s="23"/>
-      <c r="BN17" s="107" t="s">
+      <c r="BN17" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="BO17" s="108"/>
-      <c r="BP17" s="108"/>
-      <c r="BQ17" s="108"/>
-      <c r="BR17" s="109"/>
+      <c r="BO17" s="100"/>
+      <c r="BP17" s="100"/>
+      <c r="BQ17" s="100"/>
+      <c r="BR17" s="101"/>
       <c r="BS17" s="20"/>
       <c r="BT17" s="20"/>
       <c r="BU17" s="85"/>
       <c r="BV17" s="20"/>
       <c r="BW17" s="28"/>
-      <c r="BX17" s="107" t="s">
+      <c r="BX17" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="BY17" s="108"/>
-      <c r="BZ17" s="108"/>
-      <c r="CA17" s="108"/>
-      <c r="CB17" s="109"/>
+      <c r="BY17" s="100"/>
+      <c r="BZ17" s="100"/>
+      <c r="CA17" s="100"/>
+      <c r="CB17" s="101"/>
       <c r="CC17" s="81"/>
       <c r="CD17" s="81"/>
     </row>
@@ -3805,11 +3805,11 @@
       <c r="AV20" s="20"/>
       <c r="AW20" s="20"/>
       <c r="AX20" s="20"/>
-      <c r="AY20" s="98" t="s">
+      <c r="AY20" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="AZ20" s="99"/>
-      <c r="BA20" s="100"/>
+      <c r="AZ20" s="103"/>
+      <c r="BA20" s="104"/>
       <c r="BB20" s="20"/>
       <c r="BC20" s="28"/>
       <c r="BD20" s="28"/>
@@ -3828,11 +3828,11 @@
       <c r="BQ20" s="20"/>
       <c r="BR20" s="20"/>
       <c r="BS20" s="20"/>
-      <c r="BT20" s="98" t="s">
+      <c r="BT20" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="BU20" s="99"/>
-      <c r="BV20" s="100"/>
+      <c r="BU20" s="103"/>
+      <c r="BV20" s="104"/>
       <c r="BW20" s="20"/>
       <c r="BX20" s="28"/>
       <c r="BY20" s="28"/>
@@ -3884,9 +3884,9 @@
       <c r="AV21" s="20"/>
       <c r="AW21" s="20"/>
       <c r="AX21" s="20"/>
-      <c r="AY21" s="101"/>
-      <c r="AZ21" s="102"/>
-      <c r="BA21" s="103"/>
+      <c r="AY21" s="105"/>
+      <c r="AZ21" s="106"/>
+      <c r="BA21" s="107"/>
       <c r="BB21" s="20"/>
       <c r="BC21" s="28"/>
       <c r="BD21" s="28"/>
@@ -3905,9 +3905,9 @@
       <c r="BQ21" s="20"/>
       <c r="BR21" s="20"/>
       <c r="BS21" s="20"/>
-      <c r="BT21" s="101"/>
-      <c r="BU21" s="102"/>
-      <c r="BV21" s="103"/>
+      <c r="BT21" s="105"/>
+      <c r="BU21" s="106"/>
+      <c r="BV21" s="107"/>
       <c r="BW21" s="20"/>
       <c r="BX21" s="28"/>
       <c r="BY21" s="28"/>
@@ -4044,15 +4044,15 @@
       <c r="BF23" s="79"/>
       <c r="BG23" s="79"/>
       <c r="BH23" s="79"/>
-      <c r="BI23" s="104" t="s">
+      <c r="BI23" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="BJ23" s="105"/>
-      <c r="BK23" s="105"/>
-      <c r="BL23" s="105"/>
-      <c r="BM23" s="105"/>
-      <c r="BN23" s="105"/>
-      <c r="BO23" s="106"/>
+      <c r="BJ23" s="109"/>
+      <c r="BK23" s="109"/>
+      <c r="BL23" s="109"/>
+      <c r="BM23" s="109"/>
+      <c r="BN23" s="109"/>
+      <c r="BO23" s="110"/>
       <c r="BP23" s="79"/>
       <c r="BQ23" s="79"/>
       <c r="BR23" s="79"/>
@@ -4723,50 +4723,50 @@
       <c r="AP32" s="23"/>
       <c r="AQ32" s="20"/>
       <c r="AR32" s="23"/>
-      <c r="AS32" s="107" t="s">
+      <c r="AS32" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="AT32" s="108"/>
-      <c r="AU32" s="108"/>
-      <c r="AV32" s="108"/>
-      <c r="AW32" s="109"/>
+      <c r="AT32" s="100"/>
+      <c r="AU32" s="100"/>
+      <c r="AV32" s="100"/>
+      <c r="AW32" s="101"/>
       <c r="AX32" s="20"/>
       <c r="AY32" s="20"/>
       <c r="AZ32" s="5"/>
       <c r="BA32" s="20"/>
       <c r="BB32" s="28"/>
-      <c r="BC32" s="107" t="s">
+      <c r="BC32" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="BD32" s="108"/>
-      <c r="BE32" s="108"/>
-      <c r="BF32" s="108"/>
-      <c r="BG32" s="109"/>
+      <c r="BD32" s="100"/>
+      <c r="BE32" s="100"/>
+      <c r="BF32" s="100"/>
+      <c r="BG32" s="101"/>
       <c r="BH32" s="81"/>
       <c r="BI32" s="28"/>
       <c r="BJ32" s="28"/>
       <c r="BK32" s="28"/>
       <c r="BL32" s="28"/>
       <c r="BM32" s="30"/>
-      <c r="BN32" s="107" t="s">
+      <c r="BN32" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="BO32" s="108"/>
-      <c r="BP32" s="108"/>
-      <c r="BQ32" s="108"/>
-      <c r="BR32" s="109"/>
+      <c r="BO32" s="100"/>
+      <c r="BP32" s="100"/>
+      <c r="BQ32" s="100"/>
+      <c r="BR32" s="101"/>
       <c r="BS32" s="28"/>
       <c r="BT32" s="28"/>
       <c r="BU32" s="5"/>
       <c r="BV32" s="28"/>
       <c r="BW32" s="28"/>
-      <c r="BX32" s="107" t="s">
+      <c r="BX32" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="BY32" s="108"/>
-      <c r="BZ32" s="108"/>
-      <c r="CA32" s="108"/>
-      <c r="CB32" s="109"/>
+      <c r="BY32" s="100"/>
+      <c r="BZ32" s="100"/>
+      <c r="CA32" s="100"/>
+      <c r="CB32" s="101"/>
       <c r="CC32" s="81"/>
       <c r="CD32" s="28"/>
       <c r="CE32" s="28"/>
@@ -5045,11 +5045,11 @@
       <c r="AV36" s="20"/>
       <c r="AW36" s="20"/>
       <c r="AX36" s="23"/>
-      <c r="AY36" s="98" t="s">
+      <c r="AY36" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="AZ36" s="99"/>
-      <c r="BA36" s="100"/>
+      <c r="AZ36" s="103"/>
+      <c r="BA36" s="104"/>
       <c r="BB36" s="20"/>
       <c r="BC36" s="28"/>
       <c r="BD36" s="28"/>
@@ -5068,11 +5068,11 @@
       <c r="BQ36" s="28"/>
       <c r="BR36" s="28"/>
       <c r="BS36" s="28"/>
-      <c r="BT36" s="98" t="s">
+      <c r="BT36" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="BU36" s="99"/>
-      <c r="BV36" s="100"/>
+      <c r="BU36" s="103"/>
+      <c r="BV36" s="104"/>
       <c r="BW36" s="81"/>
       <c r="BX36" s="28"/>
       <c r="BY36" s="28"/>
@@ -5126,9 +5126,9 @@
       <c r="AV37" s="20"/>
       <c r="AW37" s="20"/>
       <c r="AX37" s="23"/>
-      <c r="AY37" s="101"/>
-      <c r="AZ37" s="102"/>
-      <c r="BA37" s="103"/>
+      <c r="AY37" s="105"/>
+      <c r="AZ37" s="106"/>
+      <c r="BA37" s="107"/>
       <c r="BB37" s="20"/>
       <c r="BC37" s="28"/>
       <c r="BD37" s="28"/>
@@ -5147,9 +5147,9 @@
       <c r="BQ37" s="28"/>
       <c r="BR37" s="28"/>
       <c r="BS37" s="28"/>
-      <c r="BT37" s="101"/>
-      <c r="BU37" s="102"/>
-      <c r="BV37" s="103"/>
+      <c r="BT37" s="105"/>
+      <c r="BU37" s="106"/>
+      <c r="BV37" s="107"/>
       <c r="BW37" s="81"/>
       <c r="BX37" s="28"/>
       <c r="BY37" s="28"/>
@@ -5363,11 +5363,11 @@
       <c r="BG40" s="28"/>
       <c r="BH40" s="28"/>
       <c r="BI40" s="28"/>
-      <c r="BJ40" s="98" t="s">
+      <c r="BJ40" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="BK40" s="99"/>
-      <c r="BL40" s="100"/>
+      <c r="BK40" s="103"/>
+      <c r="BL40" s="104"/>
       <c r="BM40" s="28"/>
       <c r="BN40" s="28"/>
       <c r="BO40" s="28"/>
@@ -5439,9 +5439,9 @@
       <c r="BG41" s="28"/>
       <c r="BH41" s="28"/>
       <c r="BI41" s="28"/>
-      <c r="BJ41" s="101"/>
-      <c r="BK41" s="102"/>
-      <c r="BL41" s="103"/>
+      <c r="BJ41" s="105"/>
+      <c r="BK41" s="106"/>
+      <c r="BL41" s="107"/>
       <c r="BM41" s="28"/>
       <c r="BN41" s="28"/>
       <c r="BO41" s="28"/>
@@ -6116,49 +6116,49 @@
       <c r="AR51" s="28"/>
       <c r="AS51" s="20"/>
       <c r="AT51" s="23"/>
-      <c r="AU51" s="107" t="s">
+      <c r="AU51" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="AV51" s="108"/>
-      <c r="AW51" s="108"/>
-      <c r="AX51" s="108"/>
-      <c r="AY51" s="109"/>
+      <c r="AV51" s="100"/>
+      <c r="AW51" s="100"/>
+      <c r="AX51" s="100"/>
+      <c r="AY51" s="101"/>
       <c r="AZ51" s="20"/>
       <c r="BA51" s="20"/>
       <c r="BB51" s="85"/>
       <c r="BC51" s="20"/>
       <c r="BD51" s="28"/>
-      <c r="BE51" s="107" t="s">
+      <c r="BE51" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="BF51" s="108"/>
-      <c r="BG51" s="108"/>
-      <c r="BH51" s="108"/>
-      <c r="BI51" s="109"/>
+      <c r="BF51" s="100"/>
+      <c r="BG51" s="100"/>
+      <c r="BH51" s="100"/>
+      <c r="BI51" s="101"/>
       <c r="BJ51" s="81"/>
       <c r="BK51" s="28"/>
       <c r="BL51" s="28"/>
       <c r="BM51" s="20"/>
       <c r="BN51" s="23"/>
-      <c r="BO51" s="107" t="s">
+      <c r="BO51" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="BP51" s="108"/>
-      <c r="BQ51" s="108"/>
-      <c r="BR51" s="108"/>
-      <c r="BS51" s="109"/>
+      <c r="BP51" s="100"/>
+      <c r="BQ51" s="100"/>
+      <c r="BR51" s="100"/>
+      <c r="BS51" s="101"/>
       <c r="BT51" s="20"/>
       <c r="BU51" s="20"/>
       <c r="BV51" s="85"/>
       <c r="BW51" s="20"/>
       <c r="BX51" s="28"/>
-      <c r="BY51" s="107" t="s">
+      <c r="BY51" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="BZ51" s="108"/>
-      <c r="CA51" s="108"/>
-      <c r="CB51" s="108"/>
-      <c r="CC51" s="109"/>
+      <c r="BZ51" s="100"/>
+      <c r="CA51" s="100"/>
+      <c r="CB51" s="100"/>
+      <c r="CC51" s="101"/>
       <c r="CD51" s="81"/>
       <c r="CE51" s="28"/>
       <c r="CF51" s="81"/>
@@ -6316,11 +6316,11 @@
       <c r="AX55" s="28"/>
       <c r="AY55" s="28"/>
       <c r="AZ55" s="30"/>
-      <c r="BA55" s="98" t="s">
+      <c r="BA55" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="BB55" s="99"/>
-      <c r="BC55" s="100"/>
+      <c r="BB55" s="103"/>
+      <c r="BC55" s="104"/>
       <c r="BD55" s="28"/>
       <c r="BE55" s="28"/>
       <c r="BF55" s="28"/>
@@ -6338,11 +6338,11 @@
       <c r="BR55" s="28"/>
       <c r="BS55" s="28"/>
       <c r="BT55" s="28"/>
-      <c r="BU55" s="98" t="s">
+      <c r="BU55" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="BV55" s="99"/>
-      <c r="BW55" s="100"/>
+      <c r="BV55" s="103"/>
+      <c r="BW55" s="104"/>
       <c r="BX55" s="81"/>
       <c r="BY55" s="28"/>
       <c r="BZ55" s="28"/>
@@ -6365,9 +6365,9 @@
       <c r="AX56" s="28"/>
       <c r="AY56" s="28"/>
       <c r="AZ56" s="30"/>
-      <c r="BA56" s="101"/>
-      <c r="BB56" s="102"/>
-      <c r="BC56" s="103"/>
+      <c r="BA56" s="105"/>
+      <c r="BB56" s="106"/>
+      <c r="BC56" s="107"/>
       <c r="BD56" s="28"/>
       <c r="BE56" s="28"/>
       <c r="BF56" s="28"/>
@@ -6385,9 +6385,9 @@
       <c r="BR56" s="28"/>
       <c r="BS56" s="28"/>
       <c r="BT56" s="28"/>
-      <c r="BU56" s="101"/>
-      <c r="BV56" s="102"/>
-      <c r="BW56" s="103"/>
+      <c r="BU56" s="105"/>
+      <c r="BV56" s="106"/>
+      <c r="BW56" s="107"/>
       <c r="BX56" s="81"/>
       <c r="BY56" s="28"/>
       <c r="BZ56" s="28"/>
@@ -6510,11 +6510,11 @@
       <c r="BH59" s="28"/>
       <c r="BI59" s="28"/>
       <c r="BJ59" s="28"/>
-      <c r="BK59" s="98" t="s">
+      <c r="BK59" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="BL59" s="99"/>
-      <c r="BM59" s="100"/>
+      <c r="BL59" s="103"/>
+      <c r="BM59" s="104"/>
       <c r="BN59" s="28"/>
       <c r="BO59" s="28"/>
       <c r="BP59" s="28"/>
@@ -6557,9 +6557,9 @@
       <c r="BH60" s="28"/>
       <c r="BI60" s="28"/>
       <c r="BJ60" s="28"/>
-      <c r="BK60" s="101"/>
-      <c r="BL60" s="102"/>
-      <c r="BM60" s="103"/>
+      <c r="BK60" s="105"/>
+      <c r="BL60" s="106"/>
+      <c r="BM60" s="107"/>
       <c r="BN60" s="28"/>
       <c r="BO60" s="28"/>
       <c r="BP60" s="28"/>
@@ -6670,53 +6670,578 @@
       <c r="CE62" s="82"/>
       <c r="CF62" s="83"/>
     </row>
-    <row r="65" spans="46:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AT65" s="110" t="s">
+    <row r="65" spans="46:86" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AT65" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="AU65" s="110" t="s">
+      <c r="AU65" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="AV65" s="110" t="s">
+      <c r="AV65" s="98" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="46:48" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AT66" s="110" t="s">
+    <row r="66" spans="46:86" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AT66" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="AU66" s="110" t="s">
+      <c r="AU66" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="AV66" s="110" t="s">
+      <c r="AV66" s="98" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="46:48" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AT67" s="110" t="s">
+    <row r="67" spans="46:86" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AT67" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="AU67" s="110" t="s">
+      <c r="AU67" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="AV67" s="110" t="s">
+      <c r="AV67" s="98" t="s">
         <v>15</v>
       </c>
+    </row>
+    <row r="69" spans="46:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BM69" s="1"/>
+      <c r="BN69" s="2"/>
+      <c r="BO69" s="1"/>
+      <c r="BP69" s="2"/>
+      <c r="BQ69" s="1"/>
+      <c r="BR69" s="2"/>
+      <c r="BS69" s="1"/>
+      <c r="BT69" s="2"/>
+      <c r="BU69" s="1"/>
+      <c r="BV69" s="2"/>
+      <c r="BY69" s="1"/>
+      <c r="BZ69" s="2"/>
+      <c r="CA69" s="1"/>
+      <c r="CB69" s="2"/>
+      <c r="CC69" s="1"/>
+      <c r="CD69" s="2"/>
+      <c r="CE69" s="1"/>
+      <c r="CF69" s="2"/>
+      <c r="CG69" s="1"/>
+      <c r="CH69" s="2"/>
+    </row>
+    <row r="70" spans="46:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BM70" s="2"/>
+      <c r="BN70" s="3"/>
+      <c r="BO70" s="2"/>
+      <c r="BP70" s="3"/>
+      <c r="BQ70" s="2"/>
+      <c r="BR70" s="3"/>
+      <c r="BS70" s="2"/>
+      <c r="BT70" s="3"/>
+      <c r="BU70" s="2"/>
+      <c r="BV70" s="3"/>
+      <c r="BY70" s="2"/>
+      <c r="BZ70" s="3"/>
+      <c r="CA70" s="2"/>
+      <c r="CB70" s="3"/>
+      <c r="CC70" s="2"/>
+      <c r="CD70" s="3"/>
+      <c r="CE70" s="2"/>
+      <c r="CF70" s="3"/>
+      <c r="CG70" s="2"/>
+      <c r="CH70" s="3"/>
+    </row>
+    <row r="71" spans="46:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BM71" s="1"/>
+      <c r="BN71" s="2"/>
+      <c r="BO71" s="1"/>
+      <c r="BP71" s="2"/>
+      <c r="BQ71" s="1"/>
+      <c r="BR71" s="2"/>
+      <c r="BS71" s="1"/>
+      <c r="BT71" s="2"/>
+      <c r="BU71" s="1"/>
+      <c r="BV71" s="2"/>
+      <c r="BY71" s="1"/>
+      <c r="BZ71" s="2"/>
+      <c r="CA71" s="1"/>
+      <c r="CB71" s="2"/>
+      <c r="CC71" s="1"/>
+      <c r="CD71" s="2"/>
+      <c r="CE71" s="1"/>
+      <c r="CF71" s="2"/>
+      <c r="CG71" s="1"/>
+      <c r="CH71" s="2"/>
+    </row>
+    <row r="72" spans="46:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BM72" s="2"/>
+      <c r="BN72" s="3"/>
+      <c r="BO72" s="2"/>
+      <c r="BP72" s="3"/>
+      <c r="BQ72" s="2"/>
+      <c r="BR72" s="3"/>
+      <c r="BS72" s="2"/>
+      <c r="BT72" s="3"/>
+      <c r="BU72" s="2"/>
+      <c r="BV72" s="3"/>
+      <c r="BY72" s="2"/>
+      <c r="BZ72" s="3"/>
+      <c r="CA72" s="2"/>
+      <c r="CB72" s="3"/>
+      <c r="CC72" s="2"/>
+      <c r="CD72" s="3"/>
+      <c r="CE72" s="2"/>
+      <c r="CF72" s="3"/>
+      <c r="CG72" s="2"/>
+      <c r="CH72" s="3"/>
+    </row>
+    <row r="73" spans="46:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BM73" s="1"/>
+      <c r="BN73" s="2"/>
+      <c r="BO73" s="1"/>
+      <c r="BP73" s="2"/>
+      <c r="BQ73" s="1"/>
+      <c r="BR73" s="2"/>
+      <c r="BS73" s="1"/>
+      <c r="BT73" s="2"/>
+      <c r="BU73" s="1"/>
+      <c r="BV73" s="2"/>
+      <c r="BY73" s="1"/>
+      <c r="BZ73" s="2"/>
+      <c r="CA73" s="1"/>
+      <c r="CB73" s="2"/>
+      <c r="CC73" s="1"/>
+      <c r="CD73" s="2"/>
+      <c r="CE73" s="1"/>
+      <c r="CF73" s="2"/>
+      <c r="CG73" s="1"/>
+      <c r="CH73" s="2"/>
+    </row>
+    <row r="74" spans="46:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BM74" s="2"/>
+      <c r="BN74" s="3"/>
+      <c r="BO74" s="2"/>
+      <c r="BP74" s="3"/>
+      <c r="BQ74" s="2"/>
+      <c r="BR74" s="3"/>
+      <c r="BS74" s="2"/>
+      <c r="BT74" s="3"/>
+      <c r="BU74" s="2"/>
+      <c r="BV74" s="3"/>
+      <c r="BY74" s="2"/>
+      <c r="BZ74" s="3"/>
+      <c r="CA74" s="2"/>
+      <c r="CB74" s="3"/>
+      <c r="CC74" s="2"/>
+      <c r="CD74" s="3"/>
+      <c r="CE74" s="2"/>
+      <c r="CF74" s="3"/>
+      <c r="CG74" s="2"/>
+      <c r="CH74" s="3"/>
+    </row>
+    <row r="75" spans="46:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BM75" s="1"/>
+      <c r="BN75" s="2"/>
+      <c r="BO75" s="1"/>
+      <c r="BP75" s="2"/>
+      <c r="BQ75" s="1"/>
+      <c r="BR75" s="2"/>
+      <c r="BS75" s="1"/>
+      <c r="BT75" s="2"/>
+      <c r="BU75" s="1"/>
+      <c r="BV75" s="2"/>
+      <c r="BY75" s="1"/>
+      <c r="BZ75" s="2"/>
+      <c r="CA75" s="1"/>
+      <c r="CB75" s="2"/>
+      <c r="CC75" s="1"/>
+      <c r="CD75" s="2"/>
+      <c r="CE75" s="1"/>
+      <c r="CF75" s="2"/>
+      <c r="CG75" s="1"/>
+      <c r="CH75" s="2"/>
+    </row>
+    <row r="76" spans="46:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BM76" s="2"/>
+      <c r="BN76" s="3"/>
+      <c r="BO76" s="2"/>
+      <c r="BP76" s="3"/>
+      <c r="BQ76" s="2"/>
+      <c r="BR76" s="3"/>
+      <c r="BS76" s="2"/>
+      <c r="BT76" s="3"/>
+      <c r="BU76" s="2"/>
+      <c r="BV76" s="3"/>
+      <c r="BY76" s="2"/>
+      <c r="BZ76" s="3"/>
+      <c r="CA76" s="2"/>
+      <c r="CB76" s="3"/>
+      <c r="CC76" s="2"/>
+      <c r="CD76" s="3"/>
+      <c r="CE76" s="2"/>
+      <c r="CF76" s="3"/>
+      <c r="CG76" s="2"/>
+      <c r="CH76" s="3"/>
+    </row>
+    <row r="77" spans="46:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BM77" s="1"/>
+      <c r="BN77" s="2"/>
+      <c r="BO77" s="1"/>
+      <c r="BP77" s="2"/>
+      <c r="BQ77" s="1"/>
+      <c r="BR77" s="2"/>
+      <c r="BS77" s="1"/>
+      <c r="BT77" s="2"/>
+      <c r="BU77" s="1"/>
+      <c r="BV77" s="2"/>
+      <c r="BY77" s="1"/>
+      <c r="BZ77" s="2"/>
+      <c r="CA77" s="1"/>
+      <c r="CB77" s="2"/>
+      <c r="CC77" s="1"/>
+      <c r="CD77" s="2"/>
+      <c r="CE77" s="1"/>
+      <c r="CF77" s="2"/>
+      <c r="CG77" s="1"/>
+      <c r="CH77" s="2"/>
+    </row>
+    <row r="78" spans="46:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BM78" s="2"/>
+      <c r="BN78" s="3"/>
+      <c r="BO78" s="2"/>
+      <c r="BP78" s="3"/>
+      <c r="BQ78" s="2"/>
+      <c r="BR78" s="3"/>
+      <c r="BS78" s="2"/>
+      <c r="BT78" s="3"/>
+      <c r="BU78" s="2"/>
+      <c r="BV78" s="3"/>
+      <c r="BY78" s="2"/>
+      <c r="BZ78" s="3"/>
+      <c r="CA78" s="2"/>
+      <c r="CB78" s="3"/>
+      <c r="CC78" s="2"/>
+      <c r="CD78" s="3"/>
+      <c r="CE78" s="2"/>
+      <c r="CF78" s="3"/>
+      <c r="CG78" s="2"/>
+      <c r="CH78" s="3"/>
+    </row>
+    <row r="80" spans="46:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BZ80" s="2"/>
+      <c r="CA80" s="1"/>
+      <c r="CB80" s="2"/>
+      <c r="CC80" s="1"/>
+      <c r="CD80" s="2"/>
+      <c r="CE80" s="1"/>
+      <c r="CF80" s="2"/>
+      <c r="CG80" s="1"/>
+      <c r="CH80" s="2"/>
+    </row>
+    <row r="81" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BZ81" s="3"/>
+      <c r="CA81" s="2"/>
+      <c r="CB81" s="3"/>
+      <c r="CC81" s="2"/>
+      <c r="CD81" s="3"/>
+      <c r="CE81" s="2"/>
+      <c r="CF81" s="3"/>
+      <c r="CG81" s="2"/>
+      <c r="CH81" s="3"/>
+    </row>
+    <row r="82" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BZ82" s="2"/>
+      <c r="CA82" s="1"/>
+      <c r="CB82" s="2"/>
+      <c r="CC82" s="1"/>
+      <c r="CD82" s="2"/>
+      <c r="CE82" s="1"/>
+      <c r="CF82" s="2"/>
+      <c r="CG82" s="1"/>
+      <c r="CH82" s="2"/>
+    </row>
+    <row r="83" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BZ83" s="3"/>
+      <c r="CA83" s="2"/>
+      <c r="CB83" s="3"/>
+      <c r="CC83" s="2"/>
+      <c r="CD83" s="3"/>
+      <c r="CE83" s="2"/>
+      <c r="CF83" s="3"/>
+      <c r="CG83" s="2"/>
+      <c r="CH83" s="3"/>
+    </row>
+    <row r="84" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BZ84" s="2"/>
+      <c r="CA84" s="1"/>
+      <c r="CB84" s="2"/>
+      <c r="CC84" s="1"/>
+      <c r="CD84" s="2"/>
+      <c r="CE84" s="1"/>
+      <c r="CF84" s="2"/>
+      <c r="CG84" s="1"/>
+      <c r="CH84" s="2"/>
+    </row>
+    <row r="85" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BZ85" s="3"/>
+      <c r="CA85" s="2"/>
+      <c r="CB85" s="3"/>
+      <c r="CC85" s="2"/>
+      <c r="CD85" s="3"/>
+      <c r="CE85" s="2"/>
+      <c r="CF85" s="3"/>
+      <c r="CG85" s="2"/>
+      <c r="CH85" s="3"/>
+    </row>
+    <row r="86" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BZ86" s="2"/>
+      <c r="CA86" s="1"/>
+      <c r="CB86" s="2"/>
+      <c r="CC86" s="1"/>
+      <c r="CD86" s="2"/>
+      <c r="CE86" s="1"/>
+      <c r="CF86" s="2"/>
+      <c r="CG86" s="1"/>
+      <c r="CH86" s="2"/>
+    </row>
+    <row r="87" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BZ87" s="3"/>
+      <c r="CA87" s="2"/>
+      <c r="CB87" s="3"/>
+      <c r="CC87" s="2"/>
+      <c r="CD87" s="3"/>
+      <c r="CE87" s="2"/>
+      <c r="CF87" s="3"/>
+      <c r="CG87" s="2"/>
+      <c r="CH87" s="3"/>
+    </row>
+    <row r="88" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BZ88" s="2"/>
+      <c r="CA88" s="1"/>
+      <c r="CB88" s="2"/>
+      <c r="CC88" s="1"/>
+      <c r="CD88" s="2"/>
+      <c r="CE88" s="1"/>
+      <c r="CF88" s="2"/>
+      <c r="CG88" s="1"/>
+      <c r="CH88" s="2"/>
+    </row>
+    <row r="89" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BZ89" s="3"/>
+      <c r="CA89" s="2"/>
+      <c r="CB89" s="3"/>
+      <c r="CC89" s="2"/>
+      <c r="CD89" s="3"/>
+      <c r="CE89" s="2"/>
+      <c r="CF89" s="3"/>
+      <c r="CG89" s="2"/>
+      <c r="CH89" s="3"/>
+    </row>
+    <row r="92" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BY92" s="2"/>
+      <c r="BZ92" s="3"/>
+      <c r="CA92" s="2"/>
+      <c r="CB92" s="3"/>
+      <c r="CC92" s="2"/>
+      <c r="CD92" s="3"/>
+      <c r="CE92" s="2"/>
+      <c r="CF92" s="3"/>
+      <c r="CG92" s="2"/>
+      <c r="CH92" s="3"/>
+    </row>
+    <row r="93" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BY93" s="1"/>
+      <c r="BZ93" s="2"/>
+      <c r="CA93" s="1"/>
+      <c r="CB93" s="2"/>
+      <c r="CC93" s="1"/>
+      <c r="CD93" s="2"/>
+      <c r="CE93" s="1"/>
+      <c r="CF93" s="2"/>
+      <c r="CG93" s="1"/>
+      <c r="CH93" s="2"/>
+    </row>
+    <row r="94" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BY94" s="2"/>
+      <c r="BZ94" s="3"/>
+      <c r="CA94" s="2"/>
+      <c r="CB94" s="3"/>
+      <c r="CC94" s="2"/>
+      <c r="CD94" s="3"/>
+      <c r="CE94" s="2"/>
+      <c r="CF94" s="3"/>
+      <c r="CG94" s="2"/>
+      <c r="CH94" s="3"/>
+    </row>
+    <row r="95" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BY95" s="1"/>
+      <c r="BZ95" s="2"/>
+      <c r="CA95" s="1"/>
+      <c r="CB95" s="2"/>
+      <c r="CC95" s="1"/>
+      <c r="CD95" s="2"/>
+      <c r="CE95" s="1"/>
+      <c r="CF95" s="2"/>
+      <c r="CG95" s="1"/>
+      <c r="CH95" s="2"/>
+    </row>
+    <row r="96" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BY96" s="2"/>
+      <c r="BZ96" s="3"/>
+      <c r="CA96" s="2"/>
+      <c r="CB96" s="3"/>
+      <c r="CC96" s="2"/>
+      <c r="CD96" s="3"/>
+      <c r="CE96" s="2"/>
+      <c r="CF96" s="3"/>
+      <c r="CG96" s="2"/>
+      <c r="CH96" s="3"/>
+    </row>
+    <row r="97" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BY97" s="1"/>
+      <c r="BZ97" s="2"/>
+      <c r="CA97" s="1"/>
+      <c r="CB97" s="2"/>
+      <c r="CC97" s="1"/>
+      <c r="CD97" s="2"/>
+      <c r="CE97" s="1"/>
+      <c r="CF97" s="2"/>
+      <c r="CG97" s="1"/>
+      <c r="CH97" s="2"/>
+    </row>
+    <row r="98" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BY98" s="2"/>
+      <c r="BZ98" s="3"/>
+      <c r="CA98" s="2"/>
+      <c r="CB98" s="3"/>
+      <c r="CC98" s="2"/>
+      <c r="CD98" s="3"/>
+      <c r="CE98" s="2"/>
+      <c r="CF98" s="3"/>
+      <c r="CG98" s="2"/>
+      <c r="CH98" s="3"/>
+    </row>
+    <row r="99" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BY99" s="1"/>
+      <c r="BZ99" s="2"/>
+      <c r="CA99" s="1"/>
+      <c r="CB99" s="2"/>
+      <c r="CC99" s="1"/>
+      <c r="CD99" s="2"/>
+      <c r="CE99" s="1"/>
+      <c r="CF99" s="2"/>
+      <c r="CG99" s="1"/>
+      <c r="CH99" s="2"/>
+    </row>
+    <row r="100" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BY100" s="2"/>
+      <c r="BZ100" s="3"/>
+      <c r="CA100" s="2"/>
+      <c r="CB100" s="3"/>
+      <c r="CC100" s="2"/>
+      <c r="CD100" s="3"/>
+      <c r="CE100" s="2"/>
+      <c r="CF100" s="3"/>
+      <c r="CG100" s="2"/>
+      <c r="CH100" s="3"/>
+    </row>
+    <row r="103" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BZ103" s="3"/>
+      <c r="CA103" s="2"/>
+      <c r="CB103" s="3"/>
+      <c r="CC103" s="2"/>
+      <c r="CD103" s="3"/>
+      <c r="CE103" s="2"/>
+      <c r="CF103" s="3"/>
+      <c r="CG103" s="2"/>
+      <c r="CH103" s="3"/>
+    </row>
+    <row r="104" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BZ104" s="2"/>
+      <c r="CA104" s="1"/>
+      <c r="CB104" s="2"/>
+      <c r="CC104" s="1"/>
+      <c r="CD104" s="2"/>
+      <c r="CE104" s="1"/>
+      <c r="CF104" s="2"/>
+      <c r="CG104" s="1"/>
+      <c r="CH104" s="2"/>
+    </row>
+    <row r="105" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BZ105" s="3"/>
+      <c r="CA105" s="2"/>
+      <c r="CB105" s="3"/>
+      <c r="CC105" s="2"/>
+      <c r="CD105" s="3"/>
+      <c r="CE105" s="2"/>
+      <c r="CF105" s="3"/>
+      <c r="CG105" s="2"/>
+      <c r="CH105" s="3"/>
+    </row>
+    <row r="106" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BZ106" s="2"/>
+      <c r="CA106" s="1"/>
+      <c r="CB106" s="2"/>
+      <c r="CC106" s="1"/>
+      <c r="CD106" s="2"/>
+      <c r="CE106" s="1"/>
+      <c r="CF106" s="2"/>
+      <c r="CG106" s="1"/>
+      <c r="CH106" s="2"/>
+    </row>
+    <row r="107" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BZ107" s="3"/>
+      <c r="CA107" s="2"/>
+      <c r="CB107" s="3"/>
+      <c r="CC107" s="2"/>
+      <c r="CD107" s="3"/>
+      <c r="CE107" s="2"/>
+      <c r="CF107" s="3"/>
+      <c r="CG107" s="2"/>
+      <c r="CH107" s="3"/>
+    </row>
+    <row r="108" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BZ108" s="2"/>
+      <c r="CA108" s="1"/>
+      <c r="CB108" s="2"/>
+      <c r="CC108" s="1"/>
+      <c r="CD108" s="2"/>
+      <c r="CE108" s="1"/>
+      <c r="CF108" s="2"/>
+      <c r="CG108" s="1"/>
+      <c r="CH108" s="2"/>
+    </row>
+    <row r="109" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BZ109" s="3"/>
+      <c r="CA109" s="2"/>
+      <c r="CB109" s="3"/>
+      <c r="CC109" s="2"/>
+      <c r="CD109" s="3"/>
+      <c r="CE109" s="2"/>
+      <c r="CF109" s="3"/>
+      <c r="CG109" s="2"/>
+      <c r="CH109" s="3"/>
+    </row>
+    <row r="110" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BZ110" s="2"/>
+      <c r="CA110" s="1"/>
+      <c r="CB110" s="2"/>
+      <c r="CC110" s="1"/>
+      <c r="CD110" s="2"/>
+      <c r="CE110" s="1"/>
+      <c r="CF110" s="2"/>
+      <c r="CG110" s="1"/>
+      <c r="CH110" s="2"/>
+    </row>
+    <row r="111" spans="77:86" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BZ111" s="3"/>
+      <c r="CA111" s="2"/>
+      <c r="CB111" s="3"/>
+      <c r="CC111" s="2"/>
+      <c r="CD111" s="3"/>
+      <c r="CE111" s="2"/>
+      <c r="CF111" s="3"/>
+      <c r="CG111" s="2"/>
+      <c r="CH111" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="BN17:BR17"/>
-    <mergeCell ref="BX17:CB17"/>
-    <mergeCell ref="BT20:BV21"/>
-    <mergeCell ref="AU51:AY51"/>
-    <mergeCell ref="BE51:BI51"/>
-    <mergeCell ref="BF6:BL6"/>
-    <mergeCell ref="AS32:AW32"/>
-    <mergeCell ref="BC32:BG32"/>
-    <mergeCell ref="AY36:BA37"/>
-    <mergeCell ref="AS17:AW17"/>
-    <mergeCell ref="BC17:BG17"/>
-    <mergeCell ref="AY20:BA21"/>
     <mergeCell ref="BK59:BM60"/>
     <mergeCell ref="BI23:BO23"/>
     <mergeCell ref="BA55:BC56"/>
@@ -6727,6 +7252,18 @@
     <mergeCell ref="BX32:CB32"/>
     <mergeCell ref="BT36:BV37"/>
     <mergeCell ref="BJ40:BL41"/>
+    <mergeCell ref="BF6:BL6"/>
+    <mergeCell ref="AS32:AW32"/>
+    <mergeCell ref="BC32:BG32"/>
+    <mergeCell ref="AY36:BA37"/>
+    <mergeCell ref="AS17:AW17"/>
+    <mergeCell ref="BC17:BG17"/>
+    <mergeCell ref="AY20:BA21"/>
+    <mergeCell ref="BN17:BR17"/>
+    <mergeCell ref="BX17:CB17"/>
+    <mergeCell ref="BT20:BV21"/>
+    <mergeCell ref="AU51:AY51"/>
+    <mergeCell ref="BE51:BI51"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
start blog of BNR
</commit_message>
<xml_diff>
--- a/BNR/bayer.xlsx
+++ b/BNR/bayer.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="1335" windowWidth="21600" windowHeight="14385"/>
+    <workbookView xWindow="1650" yWindow="1335" windowWidth="21600" windowHeight="14385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -166,7 +167,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="66">
+  <borders count="74">
     <border>
       <left/>
       <right/>
@@ -1029,11 +1030,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1157,15 +1238,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1193,6 +1265,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="71" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="66" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="67" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2934,7 +3025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E2:CH111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BI94" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="B165" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="CI102" sqref="CI102"/>
     </sheetView>
   </sheetViews>
@@ -2979,15 +3070,15 @@
       <c r="BC6" s="79"/>
       <c r="BD6" s="79"/>
       <c r="BE6" s="79"/>
-      <c r="BF6" s="108" t="s">
+      <c r="BF6" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="BG6" s="109"/>
-      <c r="BH6" s="109"/>
-      <c r="BI6" s="109"/>
-      <c r="BJ6" s="109"/>
-      <c r="BK6" s="109"/>
-      <c r="BL6" s="110"/>
+      <c r="BG6" s="106"/>
+      <c r="BH6" s="106"/>
+      <c r="BI6" s="106"/>
+      <c r="BJ6" s="106"/>
+      <c r="BK6" s="106"/>
+      <c r="BL6" s="107"/>
       <c r="BM6" s="79"/>
       <c r="BN6" s="79"/>
       <c r="BO6" s="79"/>
@@ -3566,50 +3657,50 @@
       <c r="AP17" s="23"/>
       <c r="AQ17" s="20"/>
       <c r="AR17" s="23"/>
-      <c r="AS17" s="99" t="s">
+      <c r="AS17" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="AT17" s="100"/>
-      <c r="AU17" s="100"/>
-      <c r="AV17" s="100"/>
-      <c r="AW17" s="101"/>
+      <c r="AT17" s="109"/>
+      <c r="AU17" s="109"/>
+      <c r="AV17" s="109"/>
+      <c r="AW17" s="110"/>
       <c r="AX17" s="20"/>
       <c r="AY17" s="20"/>
       <c r="AZ17" s="5"/>
       <c r="BA17" s="20"/>
       <c r="BB17" s="28"/>
-      <c r="BC17" s="99" t="s">
+      <c r="BC17" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="BD17" s="100"/>
-      <c r="BE17" s="100"/>
-      <c r="BF17" s="100"/>
-      <c r="BG17" s="101"/>
+      <c r="BD17" s="109"/>
+      <c r="BE17" s="109"/>
+      <c r="BF17" s="109"/>
+      <c r="BG17" s="110"/>
       <c r="BH17" s="81"/>
       <c r="BI17" s="28"/>
       <c r="BJ17" s="28"/>
       <c r="BK17" s="28"/>
       <c r="BL17" s="20"/>
       <c r="BM17" s="23"/>
-      <c r="BN17" s="99" t="s">
+      <c r="BN17" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="BO17" s="100"/>
-      <c r="BP17" s="100"/>
-      <c r="BQ17" s="100"/>
-      <c r="BR17" s="101"/>
+      <c r="BO17" s="109"/>
+      <c r="BP17" s="109"/>
+      <c r="BQ17" s="109"/>
+      <c r="BR17" s="110"/>
       <c r="BS17" s="20"/>
       <c r="BT17" s="20"/>
       <c r="BU17" s="85"/>
       <c r="BV17" s="20"/>
       <c r="BW17" s="28"/>
-      <c r="BX17" s="99" t="s">
+      <c r="BX17" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="BY17" s="100"/>
-      <c r="BZ17" s="100"/>
-      <c r="CA17" s="100"/>
-      <c r="CB17" s="101"/>
+      <c r="BY17" s="109"/>
+      <c r="BZ17" s="109"/>
+      <c r="CA17" s="109"/>
+      <c r="CB17" s="110"/>
       <c r="CC17" s="81"/>
       <c r="CD17" s="81"/>
     </row>
@@ -3805,11 +3896,11 @@
       <c r="AV20" s="20"/>
       <c r="AW20" s="20"/>
       <c r="AX20" s="20"/>
-      <c r="AY20" s="102" t="s">
+      <c r="AY20" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="AZ20" s="103"/>
-      <c r="BA20" s="104"/>
+      <c r="AZ20" s="100"/>
+      <c r="BA20" s="101"/>
       <c r="BB20" s="20"/>
       <c r="BC20" s="28"/>
       <c r="BD20" s="28"/>
@@ -3828,11 +3919,11 @@
       <c r="BQ20" s="20"/>
       <c r="BR20" s="20"/>
       <c r="BS20" s="20"/>
-      <c r="BT20" s="102" t="s">
+      <c r="BT20" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="BU20" s="103"/>
-      <c r="BV20" s="104"/>
+      <c r="BU20" s="100"/>
+      <c r="BV20" s="101"/>
       <c r="BW20" s="20"/>
       <c r="BX20" s="28"/>
       <c r="BY20" s="28"/>
@@ -3884,9 +3975,9 @@
       <c r="AV21" s="20"/>
       <c r="AW21" s="20"/>
       <c r="AX21" s="20"/>
-      <c r="AY21" s="105"/>
-      <c r="AZ21" s="106"/>
-      <c r="BA21" s="107"/>
+      <c r="AY21" s="102"/>
+      <c r="AZ21" s="103"/>
+      <c r="BA21" s="104"/>
       <c r="BB21" s="20"/>
       <c r="BC21" s="28"/>
       <c r="BD21" s="28"/>
@@ -3905,9 +3996,9 @@
       <c r="BQ21" s="20"/>
       <c r="BR21" s="20"/>
       <c r="BS21" s="20"/>
-      <c r="BT21" s="105"/>
-      <c r="BU21" s="106"/>
-      <c r="BV21" s="107"/>
+      <c r="BT21" s="102"/>
+      <c r="BU21" s="103"/>
+      <c r="BV21" s="104"/>
       <c r="BW21" s="20"/>
       <c r="BX21" s="28"/>
       <c r="BY21" s="28"/>
@@ -4044,15 +4135,15 @@
       <c r="BF23" s="79"/>
       <c r="BG23" s="79"/>
       <c r="BH23" s="79"/>
-      <c r="BI23" s="108" t="s">
+      <c r="BI23" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="BJ23" s="109"/>
-      <c r="BK23" s="109"/>
-      <c r="BL23" s="109"/>
-      <c r="BM23" s="109"/>
-      <c r="BN23" s="109"/>
-      <c r="BO23" s="110"/>
+      <c r="BJ23" s="106"/>
+      <c r="BK23" s="106"/>
+      <c r="BL23" s="106"/>
+      <c r="BM23" s="106"/>
+      <c r="BN23" s="106"/>
+      <c r="BO23" s="107"/>
       <c r="BP23" s="79"/>
       <c r="BQ23" s="79"/>
       <c r="BR23" s="79"/>
@@ -4723,50 +4814,50 @@
       <c r="AP32" s="23"/>
       <c r="AQ32" s="20"/>
       <c r="AR32" s="23"/>
-      <c r="AS32" s="99" t="s">
+      <c r="AS32" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="AT32" s="100"/>
-      <c r="AU32" s="100"/>
-      <c r="AV32" s="100"/>
-      <c r="AW32" s="101"/>
+      <c r="AT32" s="109"/>
+      <c r="AU32" s="109"/>
+      <c r="AV32" s="109"/>
+      <c r="AW32" s="110"/>
       <c r="AX32" s="20"/>
       <c r="AY32" s="20"/>
       <c r="AZ32" s="5"/>
       <c r="BA32" s="20"/>
       <c r="BB32" s="28"/>
-      <c r="BC32" s="99" t="s">
+      <c r="BC32" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="BD32" s="100"/>
-      <c r="BE32" s="100"/>
-      <c r="BF32" s="100"/>
-      <c r="BG32" s="101"/>
+      <c r="BD32" s="109"/>
+      <c r="BE32" s="109"/>
+      <c r="BF32" s="109"/>
+      <c r="BG32" s="110"/>
       <c r="BH32" s="81"/>
       <c r="BI32" s="28"/>
       <c r="BJ32" s="28"/>
       <c r="BK32" s="28"/>
       <c r="BL32" s="28"/>
       <c r="BM32" s="30"/>
-      <c r="BN32" s="99" t="s">
+      <c r="BN32" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="BO32" s="100"/>
-      <c r="BP32" s="100"/>
-      <c r="BQ32" s="100"/>
-      <c r="BR32" s="101"/>
+      <c r="BO32" s="109"/>
+      <c r="BP32" s="109"/>
+      <c r="BQ32" s="109"/>
+      <c r="BR32" s="110"/>
       <c r="BS32" s="28"/>
       <c r="BT32" s="28"/>
       <c r="BU32" s="5"/>
       <c r="BV32" s="28"/>
       <c r="BW32" s="28"/>
-      <c r="BX32" s="99" t="s">
+      <c r="BX32" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="BY32" s="100"/>
-      <c r="BZ32" s="100"/>
-      <c r="CA32" s="100"/>
-      <c r="CB32" s="101"/>
+      <c r="BY32" s="109"/>
+      <c r="BZ32" s="109"/>
+      <c r="CA32" s="109"/>
+      <c r="CB32" s="110"/>
       <c r="CC32" s="81"/>
       <c r="CD32" s="28"/>
       <c r="CE32" s="28"/>
@@ -5045,11 +5136,11 @@
       <c r="AV36" s="20"/>
       <c r="AW36" s="20"/>
       <c r="AX36" s="23"/>
-      <c r="AY36" s="102" t="s">
+      <c r="AY36" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="AZ36" s="103"/>
-      <c r="BA36" s="104"/>
+      <c r="AZ36" s="100"/>
+      <c r="BA36" s="101"/>
       <c r="BB36" s="20"/>
       <c r="BC36" s="28"/>
       <c r="BD36" s="28"/>
@@ -5068,11 +5159,11 @@
       <c r="BQ36" s="28"/>
       <c r="BR36" s="28"/>
       <c r="BS36" s="28"/>
-      <c r="BT36" s="102" t="s">
+      <c r="BT36" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="BU36" s="103"/>
-      <c r="BV36" s="104"/>
+      <c r="BU36" s="100"/>
+      <c r="BV36" s="101"/>
       <c r="BW36" s="81"/>
       <c r="BX36" s="28"/>
       <c r="BY36" s="28"/>
@@ -5126,9 +5217,9 @@
       <c r="AV37" s="20"/>
       <c r="AW37" s="20"/>
       <c r="AX37" s="23"/>
-      <c r="AY37" s="105"/>
-      <c r="AZ37" s="106"/>
-      <c r="BA37" s="107"/>
+      <c r="AY37" s="102"/>
+      <c r="AZ37" s="103"/>
+      <c r="BA37" s="104"/>
       <c r="BB37" s="20"/>
       <c r="BC37" s="28"/>
       <c r="BD37" s="28"/>
@@ -5147,9 +5238,9 @@
       <c r="BQ37" s="28"/>
       <c r="BR37" s="28"/>
       <c r="BS37" s="28"/>
-      <c r="BT37" s="105"/>
-      <c r="BU37" s="106"/>
-      <c r="BV37" s="107"/>
+      <c r="BT37" s="102"/>
+      <c r="BU37" s="103"/>
+      <c r="BV37" s="104"/>
       <c r="BW37" s="81"/>
       <c r="BX37" s="28"/>
       <c r="BY37" s="28"/>
@@ -5363,11 +5454,11 @@
       <c r="BG40" s="28"/>
       <c r="BH40" s="28"/>
       <c r="BI40" s="28"/>
-      <c r="BJ40" s="102" t="s">
+      <c r="BJ40" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="BK40" s="103"/>
-      <c r="BL40" s="104"/>
+      <c r="BK40" s="100"/>
+      <c r="BL40" s="101"/>
       <c r="BM40" s="28"/>
       <c r="BN40" s="28"/>
       <c r="BO40" s="28"/>
@@ -5439,9 +5530,9 @@
       <c r="BG41" s="28"/>
       <c r="BH41" s="28"/>
       <c r="BI41" s="28"/>
-      <c r="BJ41" s="105"/>
-      <c r="BK41" s="106"/>
-      <c r="BL41" s="107"/>
+      <c r="BJ41" s="102"/>
+      <c r="BK41" s="103"/>
+      <c r="BL41" s="104"/>
       <c r="BM41" s="28"/>
       <c r="BN41" s="28"/>
       <c r="BO41" s="28"/>
@@ -6116,49 +6207,49 @@
       <c r="AR51" s="28"/>
       <c r="AS51" s="20"/>
       <c r="AT51" s="23"/>
-      <c r="AU51" s="99" t="s">
+      <c r="AU51" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="AV51" s="100"/>
-      <c r="AW51" s="100"/>
-      <c r="AX51" s="100"/>
-      <c r="AY51" s="101"/>
+      <c r="AV51" s="109"/>
+      <c r="AW51" s="109"/>
+      <c r="AX51" s="109"/>
+      <c r="AY51" s="110"/>
       <c r="AZ51" s="20"/>
       <c r="BA51" s="20"/>
       <c r="BB51" s="85"/>
       <c r="BC51" s="20"/>
       <c r="BD51" s="28"/>
-      <c r="BE51" s="99" t="s">
+      <c r="BE51" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="BF51" s="100"/>
-      <c r="BG51" s="100"/>
-      <c r="BH51" s="100"/>
-      <c r="BI51" s="101"/>
+      <c r="BF51" s="109"/>
+      <c r="BG51" s="109"/>
+      <c r="BH51" s="109"/>
+      <c r="BI51" s="110"/>
       <c r="BJ51" s="81"/>
       <c r="BK51" s="28"/>
       <c r="BL51" s="28"/>
       <c r="BM51" s="20"/>
       <c r="BN51" s="23"/>
-      <c r="BO51" s="99" t="s">
+      <c r="BO51" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="BP51" s="100"/>
-      <c r="BQ51" s="100"/>
-      <c r="BR51" s="100"/>
-      <c r="BS51" s="101"/>
+      <c r="BP51" s="109"/>
+      <c r="BQ51" s="109"/>
+      <c r="BR51" s="109"/>
+      <c r="BS51" s="110"/>
       <c r="BT51" s="20"/>
       <c r="BU51" s="20"/>
       <c r="BV51" s="85"/>
       <c r="BW51" s="20"/>
       <c r="BX51" s="28"/>
-      <c r="BY51" s="99" t="s">
+      <c r="BY51" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="BZ51" s="100"/>
-      <c r="CA51" s="100"/>
-      <c r="CB51" s="100"/>
-      <c r="CC51" s="101"/>
+      <c r="BZ51" s="109"/>
+      <c r="CA51" s="109"/>
+      <c r="CB51" s="109"/>
+      <c r="CC51" s="110"/>
       <c r="CD51" s="81"/>
       <c r="CE51" s="28"/>
       <c r="CF51" s="81"/>
@@ -6316,11 +6407,11 @@
       <c r="AX55" s="28"/>
       <c r="AY55" s="28"/>
       <c r="AZ55" s="30"/>
-      <c r="BA55" s="102" t="s">
+      <c r="BA55" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="BB55" s="103"/>
-      <c r="BC55" s="104"/>
+      <c r="BB55" s="100"/>
+      <c r="BC55" s="101"/>
       <c r="BD55" s="28"/>
       <c r="BE55" s="28"/>
       <c r="BF55" s="28"/>
@@ -6338,11 +6429,11 @@
       <c r="BR55" s="28"/>
       <c r="BS55" s="28"/>
       <c r="BT55" s="28"/>
-      <c r="BU55" s="102" t="s">
+      <c r="BU55" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="BV55" s="103"/>
-      <c r="BW55" s="104"/>
+      <c r="BV55" s="100"/>
+      <c r="BW55" s="101"/>
       <c r="BX55" s="81"/>
       <c r="BY55" s="28"/>
       <c r="BZ55" s="28"/>
@@ -6365,9 +6456,9 @@
       <c r="AX56" s="28"/>
       <c r="AY56" s="28"/>
       <c r="AZ56" s="30"/>
-      <c r="BA56" s="105"/>
-      <c r="BB56" s="106"/>
-      <c r="BC56" s="107"/>
+      <c r="BA56" s="102"/>
+      <c r="BB56" s="103"/>
+      <c r="BC56" s="104"/>
       <c r="BD56" s="28"/>
       <c r="BE56" s="28"/>
       <c r="BF56" s="28"/>
@@ -6385,9 +6476,9 @@
       <c r="BR56" s="28"/>
       <c r="BS56" s="28"/>
       <c r="BT56" s="28"/>
-      <c r="BU56" s="105"/>
-      <c r="BV56" s="106"/>
-      <c r="BW56" s="107"/>
+      <c r="BU56" s="102"/>
+      <c r="BV56" s="103"/>
+      <c r="BW56" s="104"/>
       <c r="BX56" s="81"/>
       <c r="BY56" s="28"/>
       <c r="BZ56" s="28"/>
@@ -6510,11 +6601,11 @@
       <c r="BH59" s="28"/>
       <c r="BI59" s="28"/>
       <c r="BJ59" s="28"/>
-      <c r="BK59" s="102" t="s">
+      <c r="BK59" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="BL59" s="103"/>
-      <c r="BM59" s="104"/>
+      <c r="BL59" s="100"/>
+      <c r="BM59" s="101"/>
       <c r="BN59" s="28"/>
       <c r="BO59" s="28"/>
       <c r="BP59" s="28"/>
@@ -6557,9 +6648,9 @@
       <c r="BH60" s="28"/>
       <c r="BI60" s="28"/>
       <c r="BJ60" s="28"/>
-      <c r="BK60" s="105"/>
-      <c r="BL60" s="106"/>
-      <c r="BM60" s="107"/>
+      <c r="BK60" s="102"/>
+      <c r="BL60" s="103"/>
+      <c r="BM60" s="104"/>
       <c r="BN60" s="28"/>
       <c r="BO60" s="28"/>
       <c r="BP60" s="28"/>
@@ -7242,6 +7333,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="BN17:BR17"/>
+    <mergeCell ref="BX17:CB17"/>
+    <mergeCell ref="BT20:BV21"/>
+    <mergeCell ref="AU51:AY51"/>
+    <mergeCell ref="BE51:BI51"/>
+    <mergeCell ref="BF6:BL6"/>
+    <mergeCell ref="AS32:AW32"/>
+    <mergeCell ref="BC32:BG32"/>
+    <mergeCell ref="AY36:BA37"/>
+    <mergeCell ref="AS17:AW17"/>
+    <mergeCell ref="BC17:BG17"/>
+    <mergeCell ref="AY20:BA21"/>
     <mergeCell ref="BK59:BM60"/>
     <mergeCell ref="BI23:BO23"/>
     <mergeCell ref="BA55:BC56"/>
@@ -7252,22 +7355,1252 @@
     <mergeCell ref="BX32:CB32"/>
     <mergeCell ref="BT36:BV37"/>
     <mergeCell ref="BJ40:BL41"/>
-    <mergeCell ref="BF6:BL6"/>
-    <mergeCell ref="AS32:AW32"/>
-    <mergeCell ref="BC32:BG32"/>
-    <mergeCell ref="AY36:BA37"/>
-    <mergeCell ref="AS17:AW17"/>
-    <mergeCell ref="BC17:BG17"/>
-    <mergeCell ref="AY20:BA21"/>
-    <mergeCell ref="BN17:BR17"/>
-    <mergeCell ref="BX17:CB17"/>
-    <mergeCell ref="BT20:BV21"/>
-    <mergeCell ref="AU51:AY51"/>
-    <mergeCell ref="BE51:BI51"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="X2:BE36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="T2" workbookViewId="0">
+      <selection activeCell="AD11" sqref="AD11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="24:57" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X3" s="118"/>
+      <c r="Y3" s="111"/>
+      <c r="Z3" s="119"/>
+      <c r="AA3" s="111"/>
+      <c r="AB3" s="119"/>
+      <c r="AC3" s="112"/>
+      <c r="AD3" s="120"/>
+      <c r="AE3" s="79"/>
+      <c r="AF3" s="120"/>
+      <c r="AG3" s="79"/>
+      <c r="AH3" s="120"/>
+      <c r="AI3" s="79"/>
+      <c r="AJ3" s="120"/>
+      <c r="AK3" s="79"/>
+      <c r="AL3" s="120"/>
+      <c r="AM3" s="79"/>
+      <c r="AN3" s="120"/>
+      <c r="AO3" s="79"/>
+      <c r="AP3" s="120"/>
+      <c r="AQ3" s="79"/>
+      <c r="AR3" s="120"/>
+      <c r="AS3" s="79"/>
+      <c r="AT3" s="120"/>
+      <c r="AU3" s="79"/>
+      <c r="AV3" s="120"/>
+      <c r="AW3" s="79"/>
+      <c r="AX3" s="120"/>
+      <c r="AY3" s="79"/>
+      <c r="AZ3" s="118"/>
+      <c r="BA3" s="111"/>
+      <c r="BB3" s="111"/>
+      <c r="BC3" s="111"/>
+      <c r="BD3" s="111"/>
+      <c r="BE3" s="112"/>
+    </row>
+    <row r="4" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X4" s="113"/>
+      <c r="Y4" s="28"/>
+      <c r="Z4" s="28"/>
+      <c r="AA4" s="28"/>
+      <c r="AB4" s="28"/>
+      <c r="AC4" s="114"/>
+      <c r="AD4" s="28"/>
+      <c r="AE4" s="28"/>
+      <c r="AF4" s="28"/>
+      <c r="AG4" s="28"/>
+      <c r="AH4" s="28"/>
+      <c r="AI4" s="28"/>
+      <c r="AJ4" s="28"/>
+      <c r="AK4" s="28"/>
+      <c r="AL4" s="28"/>
+      <c r="AM4" s="28"/>
+      <c r="AN4" s="28"/>
+      <c r="AO4" s="28"/>
+      <c r="AP4" s="28"/>
+      <c r="AQ4" s="28"/>
+      <c r="AR4" s="28"/>
+      <c r="AS4" s="28"/>
+      <c r="AT4" s="28"/>
+      <c r="AU4" s="28"/>
+      <c r="AV4" s="28"/>
+      <c r="AW4" s="28"/>
+      <c r="AX4" s="28"/>
+      <c r="AY4" s="28"/>
+      <c r="AZ4" s="113"/>
+      <c r="BA4" s="28"/>
+      <c r="BB4" s="28"/>
+      <c r="BC4" s="28"/>
+      <c r="BD4" s="28"/>
+      <c r="BE4" s="114"/>
+    </row>
+    <row r="5" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X5" s="113"/>
+      <c r="Y5" s="28"/>
+      <c r="Z5" s="28"/>
+      <c r="AA5" s="28"/>
+      <c r="AB5" s="28"/>
+      <c r="AC5" s="114"/>
+      <c r="AD5" s="28"/>
+      <c r="AE5" s="28"/>
+      <c r="AF5" s="28"/>
+      <c r="AG5" s="28"/>
+      <c r="AH5" s="28"/>
+      <c r="AI5" s="28"/>
+      <c r="AJ5" s="28"/>
+      <c r="AK5" s="28"/>
+      <c r="AL5" s="28"/>
+      <c r="AM5" s="28"/>
+      <c r="AN5" s="28"/>
+      <c r="AO5" s="28"/>
+      <c r="AP5" s="28"/>
+      <c r="AQ5" s="28"/>
+      <c r="AR5" s="28"/>
+      <c r="AS5" s="28"/>
+      <c r="AT5" s="28"/>
+      <c r="AU5" s="28"/>
+      <c r="AV5" s="28"/>
+      <c r="AW5" s="28"/>
+      <c r="AX5" s="28"/>
+      <c r="AY5" s="28"/>
+      <c r="AZ5" s="113"/>
+      <c r="BA5" s="28"/>
+      <c r="BB5" s="28"/>
+      <c r="BC5" s="28"/>
+      <c r="BD5" s="28"/>
+      <c r="BE5" s="114"/>
+    </row>
+    <row r="6" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X6" s="113"/>
+      <c r="Y6" s="28"/>
+      <c r="Z6" s="28"/>
+      <c r="AA6" s="28"/>
+      <c r="AB6" s="28"/>
+      <c r="AC6" s="114"/>
+      <c r="AD6" s="28"/>
+      <c r="AE6" s="28"/>
+      <c r="AF6" s="28"/>
+      <c r="AG6" s="28"/>
+      <c r="AH6" s="28"/>
+      <c r="AI6" s="28"/>
+      <c r="AJ6" s="28"/>
+      <c r="AK6" s="28"/>
+      <c r="AL6" s="28"/>
+      <c r="AM6" s="28"/>
+      <c r="AN6" s="28"/>
+      <c r="AO6" s="28"/>
+      <c r="AP6" s="28"/>
+      <c r="AQ6" s="28"/>
+      <c r="AR6" s="28"/>
+      <c r="AS6" s="28"/>
+      <c r="AT6" s="28"/>
+      <c r="AU6" s="28"/>
+      <c r="AV6" s="28"/>
+      <c r="AW6" s="28"/>
+      <c r="AX6" s="28"/>
+      <c r="AY6" s="28"/>
+      <c r="AZ6" s="113"/>
+      <c r="BA6" s="28"/>
+      <c r="BB6" s="28"/>
+      <c r="BC6" s="28"/>
+      <c r="BD6" s="28"/>
+      <c r="BE6" s="114"/>
+    </row>
+    <row r="7" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X7" s="113"/>
+      <c r="Y7" s="28"/>
+      <c r="Z7" s="28"/>
+      <c r="AA7" s="28"/>
+      <c r="AB7" s="28"/>
+      <c r="AC7" s="114"/>
+      <c r="AD7" s="28"/>
+      <c r="AE7" s="28"/>
+      <c r="AF7" s="28"/>
+      <c r="AG7" s="28"/>
+      <c r="AH7" s="28"/>
+      <c r="AI7" s="28"/>
+      <c r="AJ7" s="28"/>
+      <c r="AK7" s="28"/>
+      <c r="AL7" s="28"/>
+      <c r="AM7" s="28"/>
+      <c r="AN7" s="28"/>
+      <c r="AO7" s="28"/>
+      <c r="AP7" s="28"/>
+      <c r="AQ7" s="28"/>
+      <c r="AR7" s="28"/>
+      <c r="AS7" s="28"/>
+      <c r="AT7" s="28"/>
+      <c r="AU7" s="28"/>
+      <c r="AV7" s="28"/>
+      <c r="AW7" s="28"/>
+      <c r="AX7" s="28"/>
+      <c r="AY7" s="28"/>
+      <c r="AZ7" s="113"/>
+      <c r="BA7" s="28"/>
+      <c r="BB7" s="28"/>
+      <c r="BC7" s="28"/>
+      <c r="BD7" s="28"/>
+      <c r="BE7" s="114"/>
+    </row>
+    <row r="8" spans="24:57" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X8" s="115"/>
+      <c r="Y8" s="116"/>
+      <c r="Z8" s="116"/>
+      <c r="AA8" s="116"/>
+      <c r="AB8" s="116"/>
+      <c r="AC8" s="117"/>
+      <c r="AD8" s="28"/>
+      <c r="AE8" s="28"/>
+      <c r="AF8" s="28"/>
+      <c r="AG8" s="28"/>
+      <c r="AH8" s="28"/>
+      <c r="AI8" s="28"/>
+      <c r="AJ8" s="28"/>
+      <c r="AK8" s="28"/>
+      <c r="AL8" s="28"/>
+      <c r="AM8" s="28"/>
+      <c r="AN8" s="28"/>
+      <c r="AO8" s="28"/>
+      <c r="AP8" s="28"/>
+      <c r="AQ8" s="28"/>
+      <c r="AR8" s="28"/>
+      <c r="AS8" s="28"/>
+      <c r="AT8" s="28"/>
+      <c r="AU8" s="28"/>
+      <c r="AV8" s="28"/>
+      <c r="AW8" s="28"/>
+      <c r="AX8" s="28"/>
+      <c r="AY8" s="28"/>
+      <c r="AZ8" s="115"/>
+      <c r="BA8" s="116"/>
+      <c r="BB8" s="116"/>
+      <c r="BC8" s="116"/>
+      <c r="BD8" s="116"/>
+      <c r="BE8" s="117"/>
+    </row>
+    <row r="9" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X9" s="30"/>
+      <c r="Y9" s="28"/>
+      <c r="Z9" s="28"/>
+      <c r="AA9" s="28"/>
+      <c r="AB9" s="28"/>
+      <c r="AC9" s="28"/>
+      <c r="AD9" s="28"/>
+      <c r="AE9" s="28"/>
+      <c r="AF9" s="28"/>
+      <c r="AG9" s="28"/>
+      <c r="AH9" s="28"/>
+      <c r="AI9" s="28"/>
+      <c r="AJ9" s="28"/>
+      <c r="AK9" s="28"/>
+      <c r="AL9" s="28"/>
+      <c r="AM9" s="28"/>
+      <c r="AN9" s="28"/>
+      <c r="AO9" s="28"/>
+      <c r="AP9" s="28"/>
+      <c r="AQ9" s="28"/>
+      <c r="AR9" s="28"/>
+      <c r="AS9" s="28"/>
+      <c r="AT9" s="28"/>
+      <c r="AU9" s="28"/>
+      <c r="AV9" s="28"/>
+      <c r="AW9" s="28"/>
+      <c r="AX9" s="28"/>
+      <c r="AY9" s="28"/>
+      <c r="AZ9" s="28"/>
+      <c r="BA9" s="28"/>
+      <c r="BB9" s="28"/>
+      <c r="BC9" s="28"/>
+      <c r="BD9" s="28"/>
+      <c r="BE9" s="81"/>
+    </row>
+    <row r="10" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X10" s="30"/>
+      <c r="Y10" s="28"/>
+      <c r="Z10" s="28"/>
+      <c r="AA10" s="28"/>
+      <c r="AB10" s="28"/>
+      <c r="AC10" s="28"/>
+      <c r="AD10" s="28"/>
+      <c r="AE10" s="28"/>
+      <c r="AF10" s="28"/>
+      <c r="AG10" s="28"/>
+      <c r="AH10" s="28"/>
+      <c r="AI10" s="28"/>
+      <c r="AJ10" s="28"/>
+      <c r="AK10" s="28"/>
+      <c r="AL10" s="28"/>
+      <c r="AM10" s="28"/>
+      <c r="AN10" s="28"/>
+      <c r="AO10" s="28"/>
+      <c r="AP10" s="28"/>
+      <c r="AQ10" s="28"/>
+      <c r="AR10" s="28"/>
+      <c r="AS10" s="28"/>
+      <c r="AT10" s="28"/>
+      <c r="AU10" s="28"/>
+      <c r="AV10" s="28"/>
+      <c r="AW10" s="28"/>
+      <c r="AX10" s="28"/>
+      <c r="AY10" s="28"/>
+      <c r="AZ10" s="28"/>
+      <c r="BA10" s="28"/>
+      <c r="BB10" s="28"/>
+      <c r="BC10" s="28"/>
+      <c r="BD10" s="28"/>
+      <c r="BE10" s="81"/>
+    </row>
+    <row r="11" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X11" s="30"/>
+      <c r="Y11" s="28"/>
+      <c r="Z11" s="28"/>
+      <c r="AA11" s="28"/>
+      <c r="AB11" s="28"/>
+      <c r="AC11" s="28"/>
+      <c r="AD11" s="28"/>
+      <c r="AE11" s="28"/>
+      <c r="AF11" s="28"/>
+      <c r="AG11" s="28"/>
+      <c r="AH11" s="28"/>
+      <c r="AI11" s="28"/>
+      <c r="AJ11" s="28"/>
+      <c r="AK11" s="28"/>
+      <c r="AL11" s="28"/>
+      <c r="AM11" s="28"/>
+      <c r="AN11" s="28"/>
+      <c r="AO11" s="28"/>
+      <c r="AP11" s="28"/>
+      <c r="AQ11" s="28"/>
+      <c r="AR11" s="28"/>
+      <c r="AS11" s="28"/>
+      <c r="AT11" s="28"/>
+      <c r="AU11" s="28"/>
+      <c r="AV11" s="28"/>
+      <c r="AW11" s="28"/>
+      <c r="AX11" s="28"/>
+      <c r="AY11" s="28"/>
+      <c r="AZ11" s="28"/>
+      <c r="BA11" s="28"/>
+      <c r="BB11" s="28"/>
+      <c r="BC11" s="28"/>
+      <c r="BD11" s="28"/>
+      <c r="BE11" s="81"/>
+    </row>
+    <row r="12" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X12" s="30"/>
+      <c r="Y12" s="28"/>
+      <c r="Z12" s="28"/>
+      <c r="AA12" s="28"/>
+      <c r="AB12" s="28"/>
+      <c r="AC12" s="28"/>
+      <c r="AD12" s="28"/>
+      <c r="AE12" s="28"/>
+      <c r="AF12" s="28"/>
+      <c r="AG12" s="28"/>
+      <c r="AH12" s="28"/>
+      <c r="AI12" s="28"/>
+      <c r="AJ12" s="28"/>
+      <c r="AK12" s="28"/>
+      <c r="AL12" s="28"/>
+      <c r="AM12" s="28"/>
+      <c r="AN12" s="28"/>
+      <c r="AO12" s="28"/>
+      <c r="AP12" s="28"/>
+      <c r="AQ12" s="28"/>
+      <c r="AR12" s="28"/>
+      <c r="AS12" s="28"/>
+      <c r="AT12" s="28"/>
+      <c r="AU12" s="28"/>
+      <c r="AV12" s="28"/>
+      <c r="AW12" s="28"/>
+      <c r="AX12" s="28"/>
+      <c r="AY12" s="28"/>
+      <c r="AZ12" s="28"/>
+      <c r="BA12" s="28"/>
+      <c r="BB12" s="28"/>
+      <c r="BC12" s="28"/>
+      <c r="BD12" s="28"/>
+      <c r="BE12" s="81"/>
+    </row>
+    <row r="13" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X13" s="30"/>
+      <c r="Y13" s="28"/>
+      <c r="Z13" s="28"/>
+      <c r="AA13" s="28"/>
+      <c r="AB13" s="28"/>
+      <c r="AC13" s="28"/>
+      <c r="AD13" s="28"/>
+      <c r="AE13" s="28"/>
+      <c r="AF13" s="28"/>
+      <c r="AG13" s="28"/>
+      <c r="AH13" s="28"/>
+      <c r="AI13" s="28"/>
+      <c r="AJ13" s="28"/>
+      <c r="AK13" s="28"/>
+      <c r="AL13" s="28"/>
+      <c r="AM13" s="28"/>
+      <c r="AN13" s="28"/>
+      <c r="AO13" s="28"/>
+      <c r="AP13" s="28"/>
+      <c r="AQ13" s="28"/>
+      <c r="AR13" s="28"/>
+      <c r="AS13" s="28"/>
+      <c r="AT13" s="28"/>
+      <c r="AU13" s="28"/>
+      <c r="AV13" s="28"/>
+      <c r="AW13" s="28"/>
+      <c r="AX13" s="28"/>
+      <c r="AY13" s="28"/>
+      <c r="AZ13" s="28"/>
+      <c r="BA13" s="28"/>
+      <c r="BB13" s="28"/>
+      <c r="BC13" s="28"/>
+      <c r="BD13" s="28"/>
+      <c r="BE13" s="81"/>
+    </row>
+    <row r="14" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X14" s="30"/>
+      <c r="Y14" s="28"/>
+      <c r="Z14" s="28"/>
+      <c r="AA14" s="28"/>
+      <c r="AB14" s="28"/>
+      <c r="AC14" s="28"/>
+      <c r="AD14" s="28"/>
+      <c r="AE14" s="28"/>
+      <c r="AF14" s="28"/>
+      <c r="AG14" s="28"/>
+      <c r="AH14" s="28"/>
+      <c r="AI14" s="28"/>
+      <c r="AJ14" s="28"/>
+      <c r="AK14" s="28"/>
+      <c r="AL14" s="28"/>
+      <c r="AM14" s="28"/>
+      <c r="AN14" s="28"/>
+      <c r="AO14" s="28"/>
+      <c r="AP14" s="28"/>
+      <c r="AQ14" s="28"/>
+      <c r="AR14" s="28"/>
+      <c r="AS14" s="28"/>
+      <c r="AT14" s="28"/>
+      <c r="AU14" s="28"/>
+      <c r="AV14" s="28"/>
+      <c r="AW14" s="28"/>
+      <c r="AX14" s="28"/>
+      <c r="AY14" s="28"/>
+      <c r="AZ14" s="28"/>
+      <c r="BA14" s="28"/>
+      <c r="BB14" s="28"/>
+      <c r="BC14" s="28"/>
+      <c r="BD14" s="28"/>
+      <c r="BE14" s="81"/>
+    </row>
+    <row r="15" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X15" s="30"/>
+      <c r="Y15" s="28"/>
+      <c r="Z15" s="28"/>
+      <c r="AA15" s="28"/>
+      <c r="AB15" s="28"/>
+      <c r="AC15" s="28"/>
+      <c r="AD15" s="28"/>
+      <c r="AE15" s="28"/>
+      <c r="AF15" s="28"/>
+      <c r="AG15" s="28"/>
+      <c r="AH15" s="28"/>
+      <c r="AI15" s="28"/>
+      <c r="AJ15" s="28"/>
+      <c r="AK15" s="28"/>
+      <c r="AL15" s="28"/>
+      <c r="AM15" s="28"/>
+      <c r="AN15" s="28"/>
+      <c r="AO15" s="28"/>
+      <c r="AP15" s="28"/>
+      <c r="AQ15" s="28"/>
+      <c r="AR15" s="28"/>
+      <c r="AS15" s="28"/>
+      <c r="AT15" s="28"/>
+      <c r="AU15" s="28"/>
+      <c r="AV15" s="28"/>
+      <c r="AW15" s="28"/>
+      <c r="AX15" s="28"/>
+      <c r="AY15" s="28"/>
+      <c r="AZ15" s="28"/>
+      <c r="BA15" s="28"/>
+      <c r="BB15" s="28"/>
+      <c r="BC15" s="28"/>
+      <c r="BD15" s="28"/>
+      <c r="BE15" s="81"/>
+    </row>
+    <row r="16" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X16" s="30"/>
+      <c r="Y16" s="28"/>
+      <c r="Z16" s="28"/>
+      <c r="AA16" s="28"/>
+      <c r="AB16" s="28"/>
+      <c r="AC16" s="28"/>
+      <c r="AD16" s="28"/>
+      <c r="AE16" s="28"/>
+      <c r="AF16" s="28"/>
+      <c r="AG16" s="28"/>
+      <c r="AH16" s="28"/>
+      <c r="AI16" s="28"/>
+      <c r="AJ16" s="28"/>
+      <c r="AK16" s="28"/>
+      <c r="AL16" s="28"/>
+      <c r="AM16" s="28"/>
+      <c r="AN16" s="28"/>
+      <c r="AO16" s="28"/>
+      <c r="AP16" s="28"/>
+      <c r="AQ16" s="28"/>
+      <c r="AR16" s="28"/>
+      <c r="AS16" s="28"/>
+      <c r="AT16" s="28"/>
+      <c r="AU16" s="28"/>
+      <c r="AV16" s="28"/>
+      <c r="AW16" s="28"/>
+      <c r="AX16" s="28"/>
+      <c r="AY16" s="28"/>
+      <c r="AZ16" s="28"/>
+      <c r="BA16" s="28"/>
+      <c r="BB16" s="28"/>
+      <c r="BC16" s="28"/>
+      <c r="BD16" s="28"/>
+      <c r="BE16" s="81"/>
+    </row>
+    <row r="17" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X17" s="30"/>
+      <c r="Y17" s="28"/>
+      <c r="Z17" s="28"/>
+      <c r="AA17" s="28"/>
+      <c r="AB17" s="28"/>
+      <c r="AC17" s="28"/>
+      <c r="AD17" s="28"/>
+      <c r="AE17" s="28"/>
+      <c r="AF17" s="28"/>
+      <c r="AG17" s="28"/>
+      <c r="AH17" s="28"/>
+      <c r="AI17" s="28"/>
+      <c r="AJ17" s="28"/>
+      <c r="AK17" s="28"/>
+      <c r="AL17" s="28"/>
+      <c r="AM17" s="28"/>
+      <c r="AN17" s="28"/>
+      <c r="AO17" s="28"/>
+      <c r="AP17" s="28"/>
+      <c r="AQ17" s="28"/>
+      <c r="AR17" s="28"/>
+      <c r="AS17" s="28"/>
+      <c r="AT17" s="28"/>
+      <c r="AU17" s="28"/>
+      <c r="AV17" s="28"/>
+      <c r="AW17" s="28"/>
+      <c r="AX17" s="28"/>
+      <c r="AY17" s="28"/>
+      <c r="AZ17" s="28"/>
+      <c r="BA17" s="28"/>
+      <c r="BB17" s="28"/>
+      <c r="BC17" s="28"/>
+      <c r="BD17" s="28"/>
+      <c r="BE17" s="81"/>
+    </row>
+    <row r="18" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X18" s="30"/>
+      <c r="Y18" s="28"/>
+      <c r="Z18" s="28"/>
+      <c r="AA18" s="28"/>
+      <c r="AB18" s="28"/>
+      <c r="AC18" s="28"/>
+      <c r="AD18" s="28"/>
+      <c r="AE18" s="28"/>
+      <c r="AF18" s="28"/>
+      <c r="AG18" s="28"/>
+      <c r="AH18" s="28"/>
+      <c r="AI18" s="28"/>
+      <c r="AJ18" s="28"/>
+      <c r="AK18" s="28"/>
+      <c r="AL18" s="28"/>
+      <c r="AM18" s="28"/>
+      <c r="AN18" s="28"/>
+      <c r="AO18" s="28"/>
+      <c r="AP18" s="28"/>
+      <c r="AQ18" s="28"/>
+      <c r="AR18" s="28"/>
+      <c r="AS18" s="28"/>
+      <c r="AT18" s="28"/>
+      <c r="AU18" s="28"/>
+      <c r="AV18" s="28"/>
+      <c r="AW18" s="28"/>
+      <c r="AX18" s="28"/>
+      <c r="AY18" s="28"/>
+      <c r="AZ18" s="28"/>
+      <c r="BA18" s="28"/>
+      <c r="BB18" s="28"/>
+      <c r="BC18" s="28"/>
+      <c r="BD18" s="28"/>
+      <c r="BE18" s="81"/>
+    </row>
+    <row r="19" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X19" s="30"/>
+      <c r="Y19" s="28"/>
+      <c r="Z19" s="28"/>
+      <c r="AA19" s="28"/>
+      <c r="AB19" s="28"/>
+      <c r="AC19" s="28"/>
+      <c r="AD19" s="28"/>
+      <c r="AE19" s="28"/>
+      <c r="AF19" s="28"/>
+      <c r="AG19" s="28"/>
+      <c r="AH19" s="28"/>
+      <c r="AI19" s="28"/>
+      <c r="AJ19" s="28"/>
+      <c r="AK19" s="28"/>
+      <c r="AL19" s="28"/>
+      <c r="AM19" s="28"/>
+      <c r="AN19" s="28"/>
+      <c r="AO19" s="28"/>
+      <c r="AP19" s="28"/>
+      <c r="AQ19" s="28"/>
+      <c r="AR19" s="28"/>
+      <c r="AS19" s="28"/>
+      <c r="AT19" s="28"/>
+      <c r="AU19" s="28"/>
+      <c r="AV19" s="28"/>
+      <c r="AW19" s="28"/>
+      <c r="AX19" s="28"/>
+      <c r="AY19" s="28"/>
+      <c r="AZ19" s="28"/>
+      <c r="BA19" s="28"/>
+      <c r="BB19" s="28"/>
+      <c r="BC19" s="28"/>
+      <c r="BD19" s="28"/>
+      <c r="BE19" s="81"/>
+    </row>
+    <row r="20" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X20" s="30"/>
+      <c r="Y20" s="28"/>
+      <c r="Z20" s="28"/>
+      <c r="AA20" s="28"/>
+      <c r="AB20" s="28"/>
+      <c r="AC20" s="28"/>
+      <c r="AD20" s="28"/>
+      <c r="AE20" s="28"/>
+      <c r="AF20" s="28"/>
+      <c r="AG20" s="28"/>
+      <c r="AH20" s="28"/>
+      <c r="AI20" s="28"/>
+      <c r="AJ20" s="28"/>
+      <c r="AK20" s="28"/>
+      <c r="AL20" s="28"/>
+      <c r="AM20" s="28"/>
+      <c r="AN20" s="28"/>
+      <c r="AO20" s="28"/>
+      <c r="AP20" s="28"/>
+      <c r="AQ20" s="28"/>
+      <c r="AR20" s="28"/>
+      <c r="AS20" s="28"/>
+      <c r="AT20" s="28"/>
+      <c r="AU20" s="28"/>
+      <c r="AV20" s="28"/>
+      <c r="AW20" s="28"/>
+      <c r="AX20" s="28"/>
+      <c r="AY20" s="28"/>
+      <c r="AZ20" s="28"/>
+      <c r="BA20" s="28"/>
+      <c r="BB20" s="28"/>
+      <c r="BC20" s="28"/>
+      <c r="BD20" s="28"/>
+      <c r="BE20" s="81"/>
+    </row>
+    <row r="21" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X21" s="30"/>
+      <c r="Y21" s="28"/>
+      <c r="Z21" s="28"/>
+      <c r="AA21" s="28"/>
+      <c r="AB21" s="28"/>
+      <c r="AC21" s="28"/>
+      <c r="AD21" s="28"/>
+      <c r="AE21" s="28"/>
+      <c r="AF21" s="28"/>
+      <c r="AG21" s="28"/>
+      <c r="AH21" s="28"/>
+      <c r="AI21" s="28"/>
+      <c r="AJ21" s="28"/>
+      <c r="AK21" s="28"/>
+      <c r="AL21" s="28"/>
+      <c r="AM21" s="28"/>
+      <c r="AN21" s="28"/>
+      <c r="AO21" s="28"/>
+      <c r="AP21" s="28"/>
+      <c r="AQ21" s="28"/>
+      <c r="AR21" s="28"/>
+      <c r="AS21" s="28"/>
+      <c r="AT21" s="28"/>
+      <c r="AU21" s="28"/>
+      <c r="AV21" s="28"/>
+      <c r="AW21" s="28"/>
+      <c r="AX21" s="28"/>
+      <c r="AY21" s="28"/>
+      <c r="AZ21" s="28"/>
+      <c r="BA21" s="28"/>
+      <c r="BB21" s="28"/>
+      <c r="BC21" s="28"/>
+      <c r="BD21" s="28"/>
+      <c r="BE21" s="81"/>
+    </row>
+    <row r="22" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X22" s="30"/>
+      <c r="Y22" s="28"/>
+      <c r="Z22" s="28"/>
+      <c r="AA22" s="28"/>
+      <c r="AB22" s="28"/>
+      <c r="AC22" s="28"/>
+      <c r="AD22" s="28"/>
+      <c r="AE22" s="28"/>
+      <c r="AF22" s="28"/>
+      <c r="AG22" s="28"/>
+      <c r="AH22" s="28"/>
+      <c r="AI22" s="28"/>
+      <c r="AJ22" s="28"/>
+      <c r="AK22" s="28"/>
+      <c r="AL22" s="28"/>
+      <c r="AM22" s="28"/>
+      <c r="AN22" s="28"/>
+      <c r="AO22" s="28"/>
+      <c r="AP22" s="28"/>
+      <c r="AQ22" s="28"/>
+      <c r="AR22" s="28"/>
+      <c r="AS22" s="28"/>
+      <c r="AT22" s="28"/>
+      <c r="AU22" s="28"/>
+      <c r="AV22" s="28"/>
+      <c r="AW22" s="28"/>
+      <c r="AX22" s="28"/>
+      <c r="AY22" s="28"/>
+      <c r="AZ22" s="28"/>
+      <c r="BA22" s="28"/>
+      <c r="BB22" s="28"/>
+      <c r="BC22" s="28"/>
+      <c r="BD22" s="28"/>
+      <c r="BE22" s="81"/>
+    </row>
+    <row r="23" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X23" s="30"/>
+      <c r="Y23" s="28"/>
+      <c r="Z23" s="28"/>
+      <c r="AA23" s="28"/>
+      <c r="AB23" s="28"/>
+      <c r="AC23" s="28"/>
+      <c r="AD23" s="28"/>
+      <c r="AE23" s="28"/>
+      <c r="AF23" s="28"/>
+      <c r="AG23" s="28"/>
+      <c r="AH23" s="28"/>
+      <c r="AI23" s="28"/>
+      <c r="AJ23" s="28"/>
+      <c r="AK23" s="28"/>
+      <c r="AL23" s="28"/>
+      <c r="AM23" s="28"/>
+      <c r="AN23" s="28"/>
+      <c r="AO23" s="28"/>
+      <c r="AP23" s="28"/>
+      <c r="AQ23" s="28"/>
+      <c r="AR23" s="28"/>
+      <c r="AS23" s="28"/>
+      <c r="AT23" s="28"/>
+      <c r="AU23" s="28"/>
+      <c r="AV23" s="28"/>
+      <c r="AW23" s="28"/>
+      <c r="AX23" s="28"/>
+      <c r="AY23" s="28"/>
+      <c r="AZ23" s="28"/>
+      <c r="BA23" s="28"/>
+      <c r="BB23" s="28"/>
+      <c r="BC23" s="28"/>
+      <c r="BD23" s="28"/>
+      <c r="BE23" s="81"/>
+    </row>
+    <row r="24" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X24" s="30"/>
+      <c r="Y24" s="28"/>
+      <c r="Z24" s="28"/>
+      <c r="AA24" s="28"/>
+      <c r="AB24" s="28"/>
+      <c r="AC24" s="28"/>
+      <c r="AD24" s="28"/>
+      <c r="AE24" s="28"/>
+      <c r="AF24" s="28"/>
+      <c r="AG24" s="28"/>
+      <c r="AH24" s="28"/>
+      <c r="AI24" s="28"/>
+      <c r="AJ24" s="28"/>
+      <c r="AK24" s="28"/>
+      <c r="AL24" s="28"/>
+      <c r="AM24" s="28"/>
+      <c r="AN24" s="28"/>
+      <c r="AO24" s="28"/>
+      <c r="AP24" s="28"/>
+      <c r="AQ24" s="28"/>
+      <c r="AR24" s="28"/>
+      <c r="AS24" s="28"/>
+      <c r="AT24" s="28"/>
+      <c r="AU24" s="28"/>
+      <c r="AV24" s="28"/>
+      <c r="AW24" s="28"/>
+      <c r="AX24" s="28"/>
+      <c r="AY24" s="28"/>
+      <c r="AZ24" s="28"/>
+      <c r="BA24" s="28"/>
+      <c r="BB24" s="28"/>
+      <c r="BC24" s="28"/>
+      <c r="BD24" s="28"/>
+      <c r="BE24" s="81"/>
+    </row>
+    <row r="25" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X25" s="30"/>
+      <c r="Y25" s="28"/>
+      <c r="Z25" s="28"/>
+      <c r="AA25" s="28"/>
+      <c r="AB25" s="28"/>
+      <c r="AC25" s="28"/>
+      <c r="AD25" s="28"/>
+      <c r="AE25" s="28"/>
+      <c r="AF25" s="28"/>
+      <c r="AG25" s="28"/>
+      <c r="AH25" s="28"/>
+      <c r="AI25" s="28"/>
+      <c r="AJ25" s="28"/>
+      <c r="AK25" s="28"/>
+      <c r="AL25" s="28"/>
+      <c r="AM25" s="28"/>
+      <c r="AN25" s="28"/>
+      <c r="AO25" s="28"/>
+      <c r="AP25" s="28"/>
+      <c r="AQ25" s="28"/>
+      <c r="AR25" s="28"/>
+      <c r="AS25" s="28"/>
+      <c r="AT25" s="28"/>
+      <c r="AU25" s="28"/>
+      <c r="AV25" s="28"/>
+      <c r="AW25" s="28"/>
+      <c r="AX25" s="28"/>
+      <c r="AY25" s="28"/>
+      <c r="AZ25" s="28"/>
+      <c r="BA25" s="28"/>
+      <c r="BB25" s="28"/>
+      <c r="BC25" s="28"/>
+      <c r="BD25" s="28"/>
+      <c r="BE25" s="81"/>
+    </row>
+    <row r="26" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X26" s="30"/>
+      <c r="Y26" s="28"/>
+      <c r="Z26" s="28"/>
+      <c r="AA26" s="28"/>
+      <c r="AB26" s="28"/>
+      <c r="AC26" s="28"/>
+      <c r="AD26" s="28"/>
+      <c r="AE26" s="28"/>
+      <c r="AF26" s="28"/>
+      <c r="AG26" s="28"/>
+      <c r="AH26" s="28"/>
+      <c r="AI26" s="28"/>
+      <c r="AJ26" s="28"/>
+      <c r="AK26" s="28"/>
+      <c r="AL26" s="28"/>
+      <c r="AM26" s="28"/>
+      <c r="AN26" s="28"/>
+      <c r="AO26" s="28"/>
+      <c r="AP26" s="28"/>
+      <c r="AQ26" s="28"/>
+      <c r="AR26" s="28"/>
+      <c r="AS26" s="28"/>
+      <c r="AT26" s="28"/>
+      <c r="AU26" s="28"/>
+      <c r="AV26" s="28"/>
+      <c r="AW26" s="28"/>
+      <c r="AX26" s="28"/>
+      <c r="AY26" s="28"/>
+      <c r="AZ26" s="28"/>
+      <c r="BA26" s="28"/>
+      <c r="BB26" s="28"/>
+      <c r="BC26" s="28"/>
+      <c r="BD26" s="28"/>
+      <c r="BE26" s="81"/>
+    </row>
+    <row r="27" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X27" s="30"/>
+      <c r="Y27" s="28"/>
+      <c r="Z27" s="28"/>
+      <c r="AA27" s="28"/>
+      <c r="AB27" s="28"/>
+      <c r="AC27" s="28"/>
+      <c r="AD27" s="28"/>
+      <c r="AE27" s="28"/>
+      <c r="AF27" s="28"/>
+      <c r="AG27" s="28"/>
+      <c r="AH27" s="28"/>
+      <c r="AI27" s="28"/>
+      <c r="AJ27" s="28"/>
+      <c r="AK27" s="28"/>
+      <c r="AL27" s="28"/>
+      <c r="AM27" s="28"/>
+      <c r="AN27" s="28"/>
+      <c r="AO27" s="28"/>
+      <c r="AP27" s="28"/>
+      <c r="AQ27" s="28"/>
+      <c r="AR27" s="28"/>
+      <c r="AS27" s="28"/>
+      <c r="AT27" s="28"/>
+      <c r="AU27" s="28"/>
+      <c r="AV27" s="28"/>
+      <c r="AW27" s="28"/>
+      <c r="AX27" s="28"/>
+      <c r="AY27" s="28"/>
+      <c r="AZ27" s="28"/>
+      <c r="BA27" s="28"/>
+      <c r="BB27" s="28"/>
+      <c r="BC27" s="28"/>
+      <c r="BD27" s="28"/>
+      <c r="BE27" s="81"/>
+    </row>
+    <row r="28" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X28" s="30"/>
+      <c r="Y28" s="28"/>
+      <c r="Z28" s="28"/>
+      <c r="AA28" s="28"/>
+      <c r="AB28" s="28"/>
+      <c r="AC28" s="28"/>
+      <c r="AD28" s="28"/>
+      <c r="AE28" s="28"/>
+      <c r="AF28" s="28"/>
+      <c r="AG28" s="28"/>
+      <c r="AH28" s="28"/>
+      <c r="AI28" s="28"/>
+      <c r="AJ28" s="28"/>
+      <c r="AK28" s="28"/>
+      <c r="AL28" s="28"/>
+      <c r="AM28" s="28"/>
+      <c r="AN28" s="28"/>
+      <c r="AO28" s="28"/>
+      <c r="AP28" s="28"/>
+      <c r="AQ28" s="28"/>
+      <c r="AR28" s="28"/>
+      <c r="AS28" s="28"/>
+      <c r="AT28" s="28"/>
+      <c r="AU28" s="28"/>
+      <c r="AV28" s="28"/>
+      <c r="AW28" s="28"/>
+      <c r="AX28" s="28"/>
+      <c r="AY28" s="28"/>
+      <c r="AZ28" s="28"/>
+      <c r="BA28" s="28"/>
+      <c r="BB28" s="28"/>
+      <c r="BC28" s="28"/>
+      <c r="BD28" s="28"/>
+      <c r="BE28" s="81"/>
+    </row>
+    <row r="29" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X29" s="30"/>
+      <c r="Y29" s="28"/>
+      <c r="Z29" s="28"/>
+      <c r="AA29" s="28"/>
+      <c r="AB29" s="28"/>
+      <c r="AC29" s="28"/>
+      <c r="AD29" s="28"/>
+      <c r="AE29" s="28"/>
+      <c r="AF29" s="28"/>
+      <c r="AG29" s="28"/>
+      <c r="AH29" s="28"/>
+      <c r="AI29" s="28"/>
+      <c r="AJ29" s="28"/>
+      <c r="AK29" s="28"/>
+      <c r="AL29" s="28"/>
+      <c r="AM29" s="28"/>
+      <c r="AN29" s="28"/>
+      <c r="AO29" s="28"/>
+      <c r="AP29" s="28"/>
+      <c r="AQ29" s="28"/>
+      <c r="AR29" s="28"/>
+      <c r="AS29" s="28"/>
+      <c r="AT29" s="28"/>
+      <c r="AU29" s="28"/>
+      <c r="AV29" s="28"/>
+      <c r="AW29" s="28"/>
+      <c r="AX29" s="28"/>
+      <c r="AY29" s="28"/>
+      <c r="AZ29" s="28"/>
+      <c r="BA29" s="28"/>
+      <c r="BB29" s="28"/>
+      <c r="BC29" s="28"/>
+      <c r="BD29" s="28"/>
+      <c r="BE29" s="81"/>
+    </row>
+    <row r="30" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X30" s="30"/>
+      <c r="Y30" s="28"/>
+      <c r="Z30" s="28"/>
+      <c r="AA30" s="28"/>
+      <c r="AB30" s="28"/>
+      <c r="AC30" s="28"/>
+      <c r="AD30" s="28"/>
+      <c r="AE30" s="28"/>
+      <c r="AF30" s="28"/>
+      <c r="AG30" s="28"/>
+      <c r="AH30" s="28"/>
+      <c r="AI30" s="28"/>
+      <c r="AJ30" s="28"/>
+      <c r="AK30" s="28"/>
+      <c r="AL30" s="28"/>
+      <c r="AM30" s="28"/>
+      <c r="AN30" s="28"/>
+      <c r="AO30" s="28"/>
+      <c r="AP30" s="28"/>
+      <c r="AQ30" s="28"/>
+      <c r="AR30" s="28"/>
+      <c r="AS30" s="28"/>
+      <c r="AT30" s="28"/>
+      <c r="AU30" s="28"/>
+      <c r="AV30" s="28"/>
+      <c r="AW30" s="28"/>
+      <c r="AX30" s="28"/>
+      <c r="AY30" s="28"/>
+      <c r="AZ30" s="28"/>
+      <c r="BA30" s="28"/>
+      <c r="BB30" s="28"/>
+      <c r="BC30" s="28"/>
+      <c r="BD30" s="28"/>
+      <c r="BE30" s="81"/>
+    </row>
+    <row r="31" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X31" s="30"/>
+      <c r="Y31" s="28"/>
+      <c r="Z31" s="28"/>
+      <c r="AA31" s="28"/>
+      <c r="AB31" s="28"/>
+      <c r="AC31" s="28"/>
+      <c r="AD31" s="28"/>
+      <c r="AE31" s="28"/>
+      <c r="AF31" s="28"/>
+      <c r="AG31" s="28"/>
+      <c r="AH31" s="28"/>
+      <c r="AI31" s="28"/>
+      <c r="AJ31" s="28"/>
+      <c r="AK31" s="28"/>
+      <c r="AL31" s="28"/>
+      <c r="AM31" s="28"/>
+      <c r="AN31" s="28"/>
+      <c r="AO31" s="28"/>
+      <c r="AP31" s="28"/>
+      <c r="AQ31" s="28"/>
+      <c r="AR31" s="28"/>
+      <c r="AS31" s="28"/>
+      <c r="AT31" s="28"/>
+      <c r="AU31" s="28"/>
+      <c r="AV31" s="28"/>
+      <c r="AW31" s="28"/>
+      <c r="AX31" s="28"/>
+      <c r="AY31" s="28"/>
+      <c r="AZ31" s="28"/>
+      <c r="BA31" s="28"/>
+      <c r="BB31" s="28"/>
+      <c r="BC31" s="28"/>
+      <c r="BD31" s="28"/>
+      <c r="BE31" s="81"/>
+    </row>
+    <row r="32" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X32" s="30"/>
+      <c r="Y32" s="28"/>
+      <c r="Z32" s="28"/>
+      <c r="AA32" s="28"/>
+      <c r="AB32" s="28"/>
+      <c r="AC32" s="28"/>
+      <c r="AD32" s="28"/>
+      <c r="AE32" s="28"/>
+      <c r="AF32" s="28"/>
+      <c r="AG32" s="28"/>
+      <c r="AH32" s="28"/>
+      <c r="AI32" s="28"/>
+      <c r="AJ32" s="28"/>
+      <c r="AK32" s="28"/>
+      <c r="AL32" s="28"/>
+      <c r="AM32" s="28"/>
+      <c r="AN32" s="28"/>
+      <c r="AO32" s="28"/>
+      <c r="AP32" s="28"/>
+      <c r="AQ32" s="28"/>
+      <c r="AR32" s="28"/>
+      <c r="AS32" s="28"/>
+      <c r="AT32" s="28"/>
+      <c r="AU32" s="28"/>
+      <c r="AV32" s="28"/>
+      <c r="AW32" s="28"/>
+      <c r="AX32" s="28"/>
+      <c r="AY32" s="28"/>
+      <c r="AZ32" s="28"/>
+      <c r="BA32" s="28"/>
+      <c r="BB32" s="28"/>
+      <c r="BC32" s="28"/>
+      <c r="BD32" s="28"/>
+      <c r="BE32" s="81"/>
+    </row>
+    <row r="33" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X33" s="30"/>
+      <c r="Y33" s="28"/>
+      <c r="Z33" s="28"/>
+      <c r="AA33" s="28"/>
+      <c r="AB33" s="28"/>
+      <c r="AC33" s="28"/>
+      <c r="AD33" s="28"/>
+      <c r="AE33" s="28"/>
+      <c r="AF33" s="28"/>
+      <c r="AG33" s="28"/>
+      <c r="AH33" s="28"/>
+      <c r="AI33" s="28"/>
+      <c r="AJ33" s="28"/>
+      <c r="AK33" s="28"/>
+      <c r="AL33" s="28"/>
+      <c r="AM33" s="28"/>
+      <c r="AN33" s="28"/>
+      <c r="AO33" s="28"/>
+      <c r="AP33" s="28"/>
+      <c r="AQ33" s="28"/>
+      <c r="AR33" s="28"/>
+      <c r="AS33" s="28"/>
+      <c r="AT33" s="28"/>
+      <c r="AU33" s="28"/>
+      <c r="AV33" s="28"/>
+      <c r="AW33" s="28"/>
+      <c r="AX33" s="28"/>
+      <c r="AY33" s="28"/>
+      <c r="AZ33" s="28"/>
+      <c r="BA33" s="28"/>
+      <c r="BB33" s="28"/>
+      <c r="BC33" s="28"/>
+      <c r="BD33" s="28"/>
+      <c r="BE33" s="81"/>
+    </row>
+    <row r="34" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X34" s="30"/>
+      <c r="Y34" s="28"/>
+      <c r="Z34" s="28"/>
+      <c r="AA34" s="28"/>
+      <c r="AB34" s="28"/>
+      <c r="AC34" s="28"/>
+      <c r="AD34" s="28"/>
+      <c r="AE34" s="28"/>
+      <c r="AF34" s="28"/>
+      <c r="AG34" s="28"/>
+      <c r="AH34" s="28"/>
+      <c r="AI34" s="28"/>
+      <c r="AJ34" s="28"/>
+      <c r="AK34" s="28"/>
+      <c r="AL34" s="28"/>
+      <c r="AM34" s="28"/>
+      <c r="AN34" s="28"/>
+      <c r="AO34" s="28"/>
+      <c r="AP34" s="28"/>
+      <c r="AQ34" s="28"/>
+      <c r="AR34" s="28"/>
+      <c r="AS34" s="28"/>
+      <c r="AT34" s="28"/>
+      <c r="AU34" s="28"/>
+      <c r="AV34" s="28"/>
+      <c r="AW34" s="28"/>
+      <c r="AX34" s="28"/>
+      <c r="AY34" s="28"/>
+      <c r="AZ34" s="28"/>
+      <c r="BA34" s="28"/>
+      <c r="BB34" s="28"/>
+      <c r="BC34" s="28"/>
+      <c r="BD34" s="28"/>
+      <c r="BE34" s="81"/>
+    </row>
+    <row r="35" spans="24:57" x14ac:dyDescent="0.2">
+      <c r="X35" s="30"/>
+      <c r="Y35" s="28"/>
+      <c r="Z35" s="28"/>
+      <c r="AA35" s="28"/>
+      <c r="AB35" s="28"/>
+      <c r="AC35" s="28"/>
+      <c r="AD35" s="28"/>
+      <c r="AE35" s="28"/>
+      <c r="AF35" s="28"/>
+      <c r="AG35" s="28"/>
+      <c r="AH35" s="28"/>
+      <c r="AI35" s="28"/>
+      <c r="AJ35" s="28"/>
+      <c r="AK35" s="28"/>
+      <c r="AL35" s="28"/>
+      <c r="AM35" s="28"/>
+      <c r="AN35" s="28"/>
+      <c r="AO35" s="28"/>
+      <c r="AP35" s="28"/>
+      <c r="AQ35" s="28"/>
+      <c r="AR35" s="28"/>
+      <c r="AS35" s="28"/>
+      <c r="AT35" s="28"/>
+      <c r="AU35" s="28"/>
+      <c r="AV35" s="28"/>
+      <c r="AW35" s="28"/>
+      <c r="AX35" s="28"/>
+      <c r="AY35" s="28"/>
+      <c r="AZ35" s="28"/>
+      <c r="BA35" s="28"/>
+      <c r="BB35" s="28"/>
+      <c r="BC35" s="28"/>
+      <c r="BD35" s="28"/>
+      <c r="BE35" s="81"/>
+    </row>
+    <row r="36" spans="24:57" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X36" s="31"/>
+      <c r="Y36" s="82"/>
+      <c r="Z36" s="82"/>
+      <c r="AA36" s="82"/>
+      <c r="AB36" s="82"/>
+      <c r="AC36" s="82"/>
+      <c r="AD36" s="82"/>
+      <c r="AE36" s="82"/>
+      <c r="AF36" s="82"/>
+      <c r="AG36" s="82"/>
+      <c r="AH36" s="82"/>
+      <c r="AI36" s="82"/>
+      <c r="AJ36" s="82"/>
+      <c r="AK36" s="82"/>
+      <c r="AL36" s="82"/>
+      <c r="AM36" s="82"/>
+      <c r="AN36" s="82"/>
+      <c r="AO36" s="82"/>
+      <c r="AP36" s="82"/>
+      <c r="AQ36" s="82"/>
+      <c r="AR36" s="82"/>
+      <c r="AS36" s="82"/>
+      <c r="AT36" s="82"/>
+      <c r="AU36" s="82"/>
+      <c r="AV36" s="82"/>
+      <c r="AW36" s="82"/>
+      <c r="AX36" s="82"/>
+      <c r="AY36" s="82"/>
+      <c r="AZ36" s="82"/>
+      <c r="BA36" s="82"/>
+      <c r="BB36" s="82"/>
+      <c r="BC36" s="82"/>
+      <c r="BD36" s="82"/>
+      <c r="BE36" s="83"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>